<commit_message>
shows how to use the SlideCollection.add method
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0CE1F4-DA50-4D40-A636-03DF563A86F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9D5190-2929-4486-961A-6ED2EC312966}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Class</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>powerpoint-insert-slides</t>
+  </si>
+  <si>
+    <t>SlideCollection</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>powerpoint-add-slides</t>
+  </si>
+  <si>
+    <t>addSlide</t>
   </si>
 </sst>
 </file>
@@ -88,12 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,8 +141,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E2" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E2" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E3" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E3" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -441,18 +454,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="A3:E4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
@@ -489,6 +502,23 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update PowerPoint API spreadsheet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9D5190-2929-4486-961A-6ED2EC312966}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ECC97B-DD43-4847-B633-26DFE031FA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Class</t>
   </si>
@@ -59,6 +59,42 @@
   </si>
   <si>
     <t>addSlide</t>
+  </si>
+  <si>
+    <t>TagCollection</t>
+  </si>
+  <si>
+    <t>powerpoint-tags</t>
+  </si>
+  <si>
+    <t>addMultipleSlideTags</t>
+  </si>
+  <si>
+    <t>getItemAt</t>
+  </si>
+  <si>
+    <t>addTagToSelectedSlide</t>
+  </si>
+  <si>
+    <t>getItem</t>
+  </si>
+  <si>
+    <t>Slide</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>deleteSlidesByAudience</t>
+  </si>
+  <si>
+    <t>ShapeCollection</t>
+  </si>
+  <si>
+    <t>addShapeTag</t>
+  </si>
+  <si>
+    <t>deletePresentationTag</t>
   </si>
 </sst>
 </file>
@@ -141,8 +177,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E3" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E3" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E9" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E9" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -454,11 +490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,6 +557,108 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Allow for mapping for custom functions and their JSDoc
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A812B2C9-C753-41AC-B03E-52134E8AA014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F1375B-C4D6-4CDF-959E-F02C3193EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="3615" windowWidth="18225" windowHeight="11422" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Class</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>createTextBox</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>PowerPoint</t>
   </si>
 </sst>
 </file>
@@ -157,13 +163,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,17 +203,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E12" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E12" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
-    <sortCondition ref="A1:A2"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F12" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F12" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
+    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{C4D3C13D-AC7C-4710-891C-E576D03BABFC}" name="Member ID (methods only)"/>
-    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,223 +514,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.53125" customWidth="1"/>
+    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[excel] (Custom Functions) Allow for mapping for custom functions and their JSDoc (#687)
* Allow for mapping for custom functions and their JSDoc

* Remove extra blank line
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A812B2C9-C753-41AC-B03E-52134E8AA014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F1375B-C4D6-4CDF-959E-F02C3193EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="3615" windowWidth="18225" windowHeight="11422" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Class</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>createTextBox</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>PowerPoint</t>
   </si>
 </sst>
 </file>
@@ -157,13 +163,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,17 +203,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:E12" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E12" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
-    <sortCondition ref="A1:A2"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F12" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F12" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
+    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{C4D3C13D-AC7C-4710-891C-E576D03BABFC}" name="Member ID (methods only)"/>
-    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,223 +514,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.53125" customWidth="1"/>
+    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes based on code review feedback.
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25911"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F1375B-C4D6-4CDF-959E-F02C3193EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAA626B-35A4-4B9C-8701-B311960C7213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="9600" yWindow="3300" windowWidth="28800" windowHeight="11295" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
   <si>
     <t>Class</t>
   </si>
@@ -122,13 +122,97 @@
   </si>
   <si>
     <t>PowerPoint</t>
+  </si>
+  <si>
+    <t>TextRange</t>
+  </si>
+  <si>
+    <t>SlideScopedCollection</t>
+  </si>
+  <si>
+    <t>getSelectedSlides</t>
+  </si>
+  <si>
+    <t>ShapeScopedCollection</t>
+  </si>
+  <si>
+    <t>getSelectedShapes</t>
+  </si>
+  <si>
+    <t>getSelectedTextRange</t>
+  </si>
+  <si>
+    <t>setSelectedSlides</t>
+  </si>
+  <si>
+    <t>setSelectedShapes</t>
+  </si>
+  <si>
+    <t>setSelected</t>
+  </si>
+  <si>
+    <t>powerpoint-slide-management-get-set-slides</t>
+  </si>
+  <si>
+    <t>saveSlideSelection</t>
+  </si>
+  <si>
+    <t>loadSlideSelection</t>
+  </si>
+  <si>
+    <t>deleteSlides</t>
+  </si>
+  <si>
+    <t>changeFill</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>loadShapeSelection</t>
+  </si>
+  <si>
+    <t>saveShapeSelection</t>
+  </si>
+  <si>
+    <t>arrangeSelected</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-get-set-shapes</t>
+  </si>
+  <si>
+    <t>powerpoint-text-get-set-textrange</t>
+  </si>
+  <si>
+    <t>loadTextSelection</t>
+  </si>
+  <si>
+    <t>changeColor</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>fill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +222,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,12 +254,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -203,22 +295,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F12" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F12" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
-    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0CD83AD1-F92A-407D-8460-4E881461FD01}" name="Class" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0BC0A726-8DBE-4106-8D0F-2E7D6B206ECF}" name="Method/Prop/Rel Name" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{C4D3C13D-AC7C-4710-891C-E576D03BABFC}" name="Member ID (methods only)"/>
-    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{93F3F1A3-FAC6-45AF-9419-DAE9A30621C6}" name="SnippetIdIntheYAMLFile" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C72A9590-19FF-45ED-9604-345729551F30}" name="MethodNameInTheSnippet" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,24 +606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.53125" customWidth="1"/>
-    <col min="3" max="3" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -551,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -571,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -591,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -611,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -631,7 +723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -651,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -671,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -691,7 +783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -711,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -731,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -751,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -769,6 +861,411 @@
       </c>
       <c r="F12" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add additional metadata properties
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25914"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10328F5D-F9E4-48A7-8F22-4E78E97F2AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ED0287-4D8F-4538-B1B3-860DEA97492A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="3300" windowWidth="28800" windowHeight="11295" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>Class</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>fill</t>
+  </si>
+  <si>
+    <t>ShapeFill</t>
+  </si>
+  <si>
+    <t>setSolidColor</t>
+  </si>
+  <si>
+    <t>ShapeFont</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
 </sst>
 </file>
@@ -295,10 +307,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
-    <sortCondition ref="B1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+    <sortCondition ref="B1:B35"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -609,11 +621,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,9 +728,6 @@
       <c r="C5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5" t="s">
         <v>56</v>
       </c>
@@ -878,11 +887,11 @@
       <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>38</v>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -891,27 +900,24 @@
         <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,47 +937,47 @@
         <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,16 +988,16 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,17 +1007,17 @@
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
+      <c r="C20" t="s">
+        <v>20</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1021,17 +1027,17 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>41</v>
+      <c r="C21" t="s">
+        <v>16</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,19 +1045,19 @@
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,99 +1065,99 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>36</v>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>36</v>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
+      <c r="B26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1162,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1171,7 +1177,7 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,19 +1185,19 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,19 +1205,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1231,7 +1237,7 @@
         <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,7 +1248,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1251,7 +1257,7 @@
         <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,13 +1267,53 @@
       <c r="B33" t="s">
         <v>34</v>
       </c>
-      <c r="C33" t="s">
-        <v>60</v>
+      <c r="C33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
       </c>
       <c r="F33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update snippet metadata order.
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25914"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ED0287-4D8F-4538-B1B3-860DEA97492A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C730A9-8E55-4347-9DAA-A6AB4A82AA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="3300" windowWidth="28800" windowHeight="11295" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="6090" yWindow="3015" windowWidth="28800" windowHeight="11295" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -254,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -262,17 +262,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +652,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,20 +1071,20 @@
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F22" t="s">
-        <v>49</v>
+      <c r="F22" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1077,7 +1104,7 @@
         <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[PowerPoint] Rearrange metadata (#741)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26020"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357BFD34-6A35-4CD9-BE99-E6B97E208B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE0500-E0F8-48A8-82C4-7009C3650F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="3015" windowWidth="28800" windowHeight="11295" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t>Class</t>
   </si>
@@ -127,13 +127,7 @@
     <t>TextRange</t>
   </si>
   <si>
-    <t>SlideScopedCollection</t>
-  </si>
-  <si>
     <t>getSelectedSlides</t>
-  </si>
-  <si>
-    <t>ShapeScopedCollection</t>
   </si>
   <si>
     <t>getSelectedShapes</t>
@@ -355,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -643,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -654,21 +648,21 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -688,517 +682,517 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F22" t="s">
         <v>57</v>
       </c>
-      <c r="F15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>41</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
       <c r="F23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>10</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>16</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1207,30 +1201,30 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1238,7 +1232,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1247,50 +1241,50 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1298,19 +1292,19 @@
         <v>34</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1318,19 +1312,19 @@
         <v>34</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1338,13 +1332,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
         <v>57</v>
-      </c>
-      <c r="F35" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing duplicate mappings for PPT
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE0500-E0F8-48A8-82C4-7009C3650F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D877AA9-18BC-4DC8-AC17-04A93361A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
   <si>
     <t>Class</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>delete</t>
-  </si>
-  <si>
-    <t>deleteSlidesByAudience</t>
   </si>
   <si>
     <t>ShapeCollection</t>
@@ -331,10 +328,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="B1:B35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
+    <sortCondition ref="B1:B33"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -645,26 +642,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -682,149 +679,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
         <v>55</v>
       </c>
-      <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -842,197 +839,197 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
         <v>28</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -1044,49 +1041,49 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
       <c r="F22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -1098,101 +1095,101 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
-        <v>20</v>
+      <c r="C24" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
         <v>10</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1201,38 +1198,38 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1241,104 +1238,64 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
+      <c r="C32" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+      <c r="C33" t="s">
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing duplicate mappings for PPT (#757)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE0500-E0F8-48A8-82C4-7009C3650F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D877AA9-18BC-4DC8-AC17-04A93361A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
   <si>
     <t>Class</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>delete</t>
-  </si>
-  <si>
-    <t>deleteSlidesByAudience</t>
   </si>
   <si>
     <t>ShapeCollection</t>
@@ -331,10 +328,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="B1:B35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
+    <sortCondition ref="B1:B33"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -645,26 +642,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -682,149 +679,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
         <v>55</v>
       </c>
-      <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -842,197 +839,197 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
         <v>28</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -1044,49 +1041,49 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
       <c r="F22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -1098,101 +1095,101 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
-        <v>20</v>
+      <c r="C24" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
         <v>10</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1201,38 +1198,38 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1241,104 +1238,64 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
+      <c r="C32" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+      <c r="C33" t="s">
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping PPT snippets to additional enum endpoints
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D877AA9-18BC-4DC8-AC17-04A93361A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A54A2D-4529-4462-9CB3-CC4FF827258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
   <si>
     <t>Class</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>setSelectedTextRange</t>
+  </si>
+  <si>
+    <t>GeometricShapeType</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>ConnectorType</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,7 +302,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,10 +339,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
-    <sortCondition ref="B1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+    <sortCondition ref="B2:B35"/>
+    <sortCondition ref="C2:C35"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -346,9 +358,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,7 +398,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -492,7 +504,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,7 +646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,15 +654,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
@@ -683,40 +696,36 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,7 +745,7 @@
         <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,16 +756,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,76 +776,76 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>7</v>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,36 +856,36 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,50 +893,56 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
+      <c r="B13" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,7 +953,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
@@ -955,7 +970,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
@@ -968,40 +983,34 @@
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,7 +1021,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1021,7 +1030,7 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,16 +1041,16 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,19 +1058,19 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,16 +1078,19 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,19 +1098,19 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1106,19 +1118,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,17 +1137,17 @@
       <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>38</v>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1146,39 +1155,39 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
+      <c r="B27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1186,7 +1195,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -1195,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1206,19 +1215,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1238,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,19 +1255,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,19 +1275,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,6 +1305,46 @@
       </c>
       <c r="F33" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping PPT snippets to additional enum endpoints (#839)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D877AA9-18BC-4DC8-AC17-04A93361A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A54A2D-4529-4462-9CB3-CC4FF827258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
   <si>
     <t>Class</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>setSelectedTextRange</t>
+  </si>
+  <si>
+    <t>GeometricShapeType</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>ConnectorType</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,7 +302,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,10 +339,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F33" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
-    <sortCondition ref="B1:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+    <sortCondition ref="B2:B35"/>
+    <sortCondition ref="C2:C35"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -346,9 +358,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,7 +398,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -492,7 +504,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,7 +646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,15 +654,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
@@ -683,40 +696,36 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,7 +745,7 @@
         <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,16 +756,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,76 +776,76 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>7</v>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,36 +856,36 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,50 +893,56 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
+      <c r="B13" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,7 +953,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
@@ -955,7 +970,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
@@ -968,40 +983,34 @@
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,7 +1021,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1021,7 +1030,7 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,16 +1041,16 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,19 +1058,19 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,16 +1078,19 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,19 +1098,19 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1106,19 +1118,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,17 +1137,17 @@
       <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>38</v>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1146,39 +1155,39 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
+      <c r="B27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1186,7 +1195,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -1195,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1206,19 +1215,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1238,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,19 +1255,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,19 +1275,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,6 +1305,46 @@
       </c>
       <c r="F33" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping samples to more ref docs
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27818"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A54A2D-4529-4462-9CB3-CC4FF827258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3DE934-E68C-42CB-B8C3-31A0B6749E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="78">
   <si>
     <t>Class</t>
   </si>
@@ -221,6 +221,39 @@
   </si>
   <si>
     <t>ConnectorType</t>
+  </si>
+  <si>
+    <t>AddSlideOptions</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>SlideMasterCollection </t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>logSlideMasters</t>
+  </si>
+  <si>
+    <t>SlideLayoutCollection </t>
+  </si>
+  <si>
+    <t>SlideMaster</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>SlideLayout</t>
+  </si>
+  <si>
+    <t>InsertSlideOptions</t>
+  </si>
+  <si>
+    <t>InsertSlideFormatting</t>
   </si>
 </sst>
 </file>
@@ -293,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -304,7 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,11 +371,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="B2:B35"/>
-    <sortCondition ref="C2:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F42" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
+    <sortCondition ref="B1:B42"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -654,11 +685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,96 +727,87 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
       <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>26</v>
+      <c r="F3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
+      <c r="B5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,16 +818,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,76 +838,76 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>7</v>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,16 +918,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,84 +938,93 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>45</v>
+      <c r="B15" t="s">
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,7 +1035,7 @@
         <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>53</v>
@@ -1017,60 +1048,51 @@
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,16 +1103,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1098,19 +1120,19 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,96 +1140,96 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>43</v>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s">
-        <v>46</v>
+      <c r="F26" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="7">
-        <v>1</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>38</v>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" t="s">
-        <v>12</v>
+      <c r="B28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,19 +1237,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,19 +1257,19 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1255,19 +1277,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1275,75 +1297,209 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
+      <c r="B33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" t="s">
-        <v>56</v>
+        <v>11</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>39</v>
+      <c r="B34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>54</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (Slides) Mapping samples to more ref docs (#904)
* Mapping samples to more ref docs

* Update API set required to match getSelectedSlides

* Update samples/powerpoint/slide-management/add-slides.yaml

Co-authored-by: Alison McKay <almckay@microsoft.com>

* Apply typo fix

---------

Co-authored-by: Alison McKay <almckay@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27818"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A54A2D-4529-4462-9CB3-CC4FF827258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3DE934-E68C-42CB-B8C3-31A0B6749E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="78">
   <si>
     <t>Class</t>
   </si>
@@ -221,6 +221,39 @@
   </si>
   <si>
     <t>ConnectorType</t>
+  </si>
+  <si>
+    <t>AddSlideOptions</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>SlideMasterCollection </t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>logSlideMasters</t>
+  </si>
+  <si>
+    <t>SlideLayoutCollection </t>
+  </si>
+  <si>
+    <t>SlideMaster</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>SlideLayout</t>
+  </si>
+  <si>
+    <t>InsertSlideOptions</t>
+  </si>
+  <si>
+    <t>InsertSlideFormatting</t>
   </si>
 </sst>
 </file>
@@ -293,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -304,7 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,11 +371,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F35" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="B2:B35"/>
-    <sortCondition ref="C2:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F42" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
+    <sortCondition ref="B1:B42"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -654,11 +685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,96 +727,87 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
       <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>26</v>
+      <c r="F3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
+      <c r="B5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,16 +818,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,76 +838,76 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>7</v>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,16 +918,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,84 +938,93 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>45</v>
+      <c r="B15" t="s">
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,7 +1035,7 @@
         <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>53</v>
@@ -1017,60 +1048,51 @@
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,16 +1103,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1098,19 +1120,19 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,96 +1140,96 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>43</v>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s">
-        <v>46</v>
+      <c r="F26" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="7">
-        <v>1</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>38</v>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" t="s">
-        <v>12</v>
+      <c r="B28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,19 +1237,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,19 +1257,19 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1255,19 +1277,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1275,75 +1297,209 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
+      <c r="B33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" t="s">
-        <v>56</v>
+        <v>11</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>39</v>
+      <c r="B34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>54</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add powerpoint snippet for shape selection by type
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27818"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3DE934-E68C-42CB-B8C3-31A0B6749E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B942BA57-6848-4386-BDD6-6619EB96D845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="86">
   <si>
     <t>Class</t>
   </si>
@@ -254,22 +254,40 @@
   </si>
   <si>
     <t>InsertSlideFormatting</t>
+  </si>
+  <si>
+    <t>ShapeType</t>
+  </si>
+  <si>
+    <t>changeLines</t>
+  </si>
+  <si>
+    <t>ShapeLineDashStyle</t>
+  </si>
+  <si>
+    <t>changeGeometricShapes</t>
+  </si>
+  <si>
+    <t>transparency</t>
+  </si>
+  <si>
+    <t>ShapeLineFormat</t>
+  </si>
+  <si>
+    <t>dashStyle</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-get-shapes-by-type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -298,45 +316,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +357,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F42" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
-    <sortCondition ref="B1:B42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F47" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F47" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F47">
+    <sortCondition ref="B1:B47"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -685,25 +671,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -723,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -740,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -757,7 +743,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -774,50 +760,48 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="6"/>
       <c r="D5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="6"/>
       <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7">
@@ -830,14 +814,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="D8">
@@ -850,14 +834,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="D9">
@@ -870,14 +854,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10">
@@ -890,14 +874,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
       <c r="D11">
@@ -910,14 +894,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12">
@@ -930,14 +914,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13">
@@ -950,34 +934,34 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>37</v>
       </c>
       <c r="D15">
@@ -990,14 +974,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>37</v>
       </c>
       <c r="D16">
@@ -1010,14 +994,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
       <c r="E17" t="s">
@@ -1027,14 +1011,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="E18" t="s">
@@ -1044,14 +1028,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="s">
@@ -1061,14 +1045,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
       <c r="E20" t="s">
@@ -1078,14 +1062,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>51</v>
       </c>
       <c r="E21" t="s">
@@ -1095,7 +1079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1115,7 +1099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1135,7 +1119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1155,7 +1139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1175,331 +1159,419 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>62</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>54</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="7" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C34" t="s">
         <v>38</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>53</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C35" t="s">
         <v>38</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>53</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
         <v>13</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>14</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F42" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
         <v>13</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C43" t="s">
         <v>20</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
         <v>13</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C44" t="s">
         <v>18</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>14</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
         <v>33</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C45" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E45" t="s">
         <v>54</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>54</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
         <v>54</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F47" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (Shapes) Add PowerPoint snippet for shape selection by type (#905)
* Add powerpoint snippet for shape selection by type

* Additional mapping

* Apply suggestions from code review

Co-authored-by: Elizabeth Samuel <elizs@microsoft.com>

* Run yarn start with review suggestions

---------

Co-authored-by: Elizabeth Samuel <elizs@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27818"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3DE934-E68C-42CB-B8C3-31A0B6749E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3921BA39-CF98-4E6D-A0A2-1F10F9511274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="87">
   <si>
     <t>Class</t>
   </si>
@@ -254,22 +254,43 @@
   </si>
   <si>
     <t>InsertSlideFormatting</t>
+  </si>
+  <si>
+    <t>ShapeType</t>
+  </si>
+  <si>
+    <t>changeLines</t>
+  </si>
+  <si>
+    <t>ShapeLineDashStyle</t>
+  </si>
+  <si>
+    <t>changeGeometricShapes</t>
+  </si>
+  <si>
+    <t>transparency</t>
+  </si>
+  <si>
+    <t>ShapeLineFormat</t>
+  </si>
+  <si>
+    <t>dashStyle</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-get-shapes-by-type</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -298,45 +319,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +360,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F42" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F42" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
-    <sortCondition ref="B1:B42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F48" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F48" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
+    <sortCondition ref="B1:B48"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -685,25 +674,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -723,7 +712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -740,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -757,7 +746,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -774,50 +763,48 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="6"/>
       <c r="D5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="6"/>
       <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7">
@@ -830,14 +817,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="D8">
@@ -850,14 +837,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="D9">
@@ -870,14 +857,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10">
@@ -890,14 +877,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
       <c r="D11">
@@ -910,14 +897,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12">
@@ -930,14 +917,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13">
@@ -950,34 +937,34 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>37</v>
       </c>
       <c r="D15">
@@ -990,14 +977,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>37</v>
       </c>
       <c r="D16">
@@ -1010,14 +997,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
       <c r="E17" t="s">
@@ -1027,14 +1014,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="E18" t="s">
@@ -1044,14 +1031,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="s">
@@ -1061,14 +1048,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
       <c r="E20" t="s">
@@ -1078,44 +1065,41 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>53</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1107,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1132,10 +1116,10 @@
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1143,7 +1127,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1152,10 +1136,10 @@
         <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1163,235 +1147,229 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>14</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C28" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>54</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="7" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="7">
-        <v>1</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C35" t="s">
         <v>38</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>53</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>53</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
         <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
@@ -1400,106 +1378,220 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
         <v>13</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>20</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>14</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
         <v>13</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C45" t="s">
         <v>18</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
         <v>14</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F45" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
         <v>33</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C46" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E46" t="s">
         <v>54</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F46" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
         <v>54</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
         <v>54</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F48" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] [Word] Map snippets at class/enum level
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3921BA39-CF98-4E6D-A0A2-1F10F9511274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26A2B6-776E-489D-B4ED-440243E2B3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>TextVerticalAlignment</t>
+  </si>
+  <si>
+    <t>createShapeWithText</t>
   </si>
 </sst>
 </file>
@@ -323,9 +332,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,10 +370,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F48" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F48" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
-    <sortCondition ref="B1:B48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F63" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F63" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F62">
+    <sortCondition ref="B1:B62"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -674,25 +684,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -712,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -729,7 +739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -746,7 +756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -763,7 +773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -780,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -797,27 +807,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -834,10 +841,10 @@
         <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -854,10 +861,10 @@
         <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -865,19 +872,19 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -894,10 +901,10 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -905,19 +912,19 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -934,10 +941,10 @@
         <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -945,19 +952,19 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -965,19 +972,19 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -994,44 +1001,47 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
+      <c r="D18" t="s">
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1039,16 +1049,16 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -1065,7 +1075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1073,16 +1083,16 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
         <v>53</v>
@@ -1099,67 +1109,58 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+      <c r="D25" t="s">
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1167,19 +1168,19 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1187,412 +1188,680 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="D27">
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
         <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
       </c>
       <c r="F33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
         <v>20</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>40</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C42" t="s">
         <v>38</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>53</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C43" t="s">
         <v>38</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>53</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D44" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" t="s">
         <v>11</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
         <v>16</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>40</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
         <v>74</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E48" t="s">
         <v>11</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
         <v>72</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
         <v>70</v>
       </c>
-      <c r="D40">
+      <c r="D50">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E50" t="s">
         <v>11</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" t="s">
         <v>74</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E52" t="s">
         <v>11</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F52" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s">
         <v>70</v>
       </c>
-      <c r="D42">
+      <c r="D54">
         <v>2</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E54" t="s">
         <v>11</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F54" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" t="s">
         <v>13</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D55" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
         <v>10</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>14</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
         <v>13</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C57" t="s">
         <v>20</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F57" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
         <v>13</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C58" t="s">
         <v>18</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>14</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
         <v>33</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D59" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
         <v>57</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E60" t="s">
         <v>54</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>54</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>54</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F62" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PowerPoint] [Word] Map snippets at class/enum level (#931)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3921BA39-CF98-4E6D-A0A2-1F10F9511274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26A2B6-776E-489D-B4ED-440243E2B3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="38640" windowHeight="21120" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>TextVerticalAlignment</t>
+  </si>
+  <si>
+    <t>createShapeWithText</t>
   </si>
 </sst>
 </file>
@@ -323,9 +332,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,10 +370,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F48" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F48" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
-    <sortCondition ref="B1:B48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F63" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F63" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F62">
+    <sortCondition ref="B1:B62"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -674,25 +684,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -712,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -729,7 +739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -746,7 +756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -763,7 +773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -780,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -797,27 +807,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -834,10 +841,10 @@
         <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -854,10 +861,10 @@
         <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -865,19 +872,19 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -894,10 +901,10 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -905,19 +912,19 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -934,10 +941,10 @@
         <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -945,19 +952,19 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -965,19 +972,19 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -994,44 +1001,47 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
+      <c r="D18" t="s">
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1039,16 +1049,16 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -1065,7 +1075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1073,16 +1083,16 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
         <v>53</v>
@@ -1099,67 +1109,58 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+      <c r="D25" t="s">
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1167,19 +1168,19 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1187,412 +1188,680 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="D27">
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
         <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
       </c>
       <c r="F33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
         <v>20</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>40</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C42" t="s">
         <v>38</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>53</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C43" t="s">
         <v>38</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>53</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D44" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" t="s">
         <v>11</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
         <v>16</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>40</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
         <v>74</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E48" t="s">
         <v>11</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
         <v>72</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
         <v>70</v>
       </c>
-      <c r="D40">
+      <c r="D50">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E50" t="s">
         <v>11</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" t="s">
         <v>74</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E52" t="s">
         <v>11</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F52" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s">
         <v>70</v>
       </c>
-      <c r="D42">
+      <c r="D54">
         <v>2</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E54" t="s">
         <v>11</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F54" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" t="s">
         <v>13</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D55" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
         <v>10</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>14</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
         <v>13</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C57" t="s">
         <v>20</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F57" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
         <v>13</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C58" t="s">
         <v>18</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>14</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
         <v>33</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D59" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
         <v>57</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E60" t="s">
         <v>54</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>54</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>54</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F62" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PowerPoint] [Word] Fix typos
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26A2B6-776E-489D-B4ED-440243E2B3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F702E683-5963-49B3-9B3C-844898E95C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="90">
   <si>
     <t>Class</t>
   </si>
@@ -332,10 +332,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1500,9 +1499,6 @@
       <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
       <c r="D44" t="s">
         <v>87</v>
       </c>
@@ -1850,17 +1846,16 @@
       <c r="A63" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="2"/>
       <c r="D63" t="s">
         <v>65</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Add types (#934)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28112"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F702E683-5963-49B3-9B3C-844898E95C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7D4F8-4522-4A82-859C-D8CDDE4C856B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="100">
   <si>
     <t>Class</t>
   </si>
@@ -290,6 +290,36 @@
   </si>
   <si>
     <t>createShapeWithText</t>
+  </si>
+  <si>
+    <t>ShapeScopedCollection</t>
+  </si>
+  <si>
+    <t>getCount</t>
+  </si>
+  <si>
+    <t>SlideScopedCollection</t>
+  </si>
+  <si>
+    <t>foregroundColor</t>
+  </si>
+  <si>
+    <t>createShapes</t>
+  </si>
+  <si>
+    <t>ShapeAddOptions</t>
+  </si>
+  <si>
+    <t>removeAll</t>
+  </si>
+  <si>
+    <t>TextFrame</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>addPresentationTag</t>
   </si>
 </sst>
 </file>
@@ -369,10 +399,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F63" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F63" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F62">
-    <sortCondition ref="B1:B62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F71" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F71" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F70">
+    <sortCondition ref="B1:B70"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -683,11 +713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,13 +1078,16 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1065,13 +1098,13 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1082,7 +1115,7 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>53</v>
@@ -1099,7 +1132,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
         <v>53</v>
@@ -1116,13 +1149,13 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1133,13 +1166,13 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1147,16 +1180,16 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1164,13 +1197,10 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -1186,17 +1216,14 @@
       <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+      <c r="D27" t="s">
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1207,7 +1234,7 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1216,7 +1243,7 @@
         <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1227,16 +1254,16 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,16 +1274,16 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1264,16 +1291,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1281,19 +1311,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1303,8 +1333,8 @@
       <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
-        <v>82</v>
+      <c r="D33" t="s">
+        <v>87</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -1318,16 +1348,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1335,16 +1365,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,16 +1385,16 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
       </c>
       <c r="E36" t="s">
         <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1369,16 +1402,16 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
         <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1386,16 +1419,16 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1403,7 +1436,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D39" t="s">
         <v>65</v>
@@ -1420,16 +1453,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
         <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1437,19 +1470,16 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,19 +1487,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D42" t="s">
+        <v>87</v>
       </c>
       <c r="E42" t="s">
         <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1477,10 +1504,10 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1489,7 +1516,7 @@
         <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1497,16 +1524,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1514,19 +1541,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1534,10 +1558,10 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1546,7 +1570,7 @@
         <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1554,16 +1578,19 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F47" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1571,16 +1598,19 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>38</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F48" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,7 +1618,7 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="D49" t="s">
         <v>87</v>
@@ -1597,7 +1627,7 @@
         <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1605,19 +1635,19 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1625,16 +1655,19 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F51" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1642,10 +1675,10 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
@@ -1659,10 +1692,10 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="C53" t="s">
+        <v>74</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
@@ -1676,13 +1709,10 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>87</v>
       </c>
       <c r="E54" t="s">
         <v>11</v>
@@ -1696,16 +1726,19 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1713,19 +1746,16 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>87</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1733,19 +1763,16 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1753,19 +1780,16 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="D58" t="s">
+        <v>87</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1773,16 +1797,19 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1790,16 +1817,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="D60" t="s">
+        <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1807,19 +1834,16 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1827,19 +1851,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D62" t="s">
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1847,15 +1868,166 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" t="s">
         <v>88</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D71" t="s">
         <v>65</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E71" t="s">
         <v>24</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F71" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Add manage-hyperlinks (#936)
* [PowerPoint] Add manage-hyperlinks

* Tweak

* Apply suggestions from code review

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>

* Run yarn start

---------

Co-authored-by: Alex Jerabek <38896772+AlexJerabek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28112"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7D4F8-4522-4A82-859C-D8CDDE4C856B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5FEB3-B198-4262-9DA9-3DC31BAAB322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="104">
   <si>
     <t>Class</t>
   </si>
@@ -320,6 +320,18 @@
   </si>
   <si>
     <t>addPresentationTag</t>
+  </si>
+  <si>
+    <t>Hyperlink</t>
+  </si>
+  <si>
+    <t>HyperlinkCollection</t>
+  </si>
+  <si>
+    <t>powerpoint-manage-hyperlinks</t>
+  </si>
+  <si>
+    <t>getHyperlinks</t>
   </si>
 </sst>
 </file>
@@ -362,9 +374,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +412,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F71" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F71" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F70">
-    <sortCondition ref="B1:B70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F73" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F73" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F72">
+    <sortCondition ref="B1:B72"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -713,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,34 +819,36 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
+      <c r="B5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
+        <v>87</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+        <v>87</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -841,10 +856,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -858,19 +873,16 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -880,17 +892,14 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="D9" t="s">
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -910,7 +919,7 @@
         <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -921,16 +930,16 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -941,16 +950,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,16 +970,16 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -981,16 +990,16 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1001,16 +1010,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1021,16 +1030,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1041,16 +1050,16 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1058,16 +1067,19 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1075,19 +1087,19 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,14 +1109,14 @@
       <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
-        <v>58</v>
+      <c r="D20" t="s">
+        <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1115,13 +1127,16 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,13 +1147,13 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
         <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1149,7 +1164,7 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
         <v>53</v>
@@ -1166,13 +1181,13 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1183,7 +1198,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1197,16 +1212,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1214,16 +1229,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1231,13 +1246,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
@@ -1253,17 +1265,14 @@
       <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
+      <c r="D29" t="s">
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1274,7 +1283,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1283,7 +1292,7 @@
         <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1294,16 +1303,16 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1314,16 +1323,16 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1331,16 +1340,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1348,16 +1360,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>70</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1367,17 +1382,14 @@
       <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="C35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+      <c r="D35" t="s">
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1388,13 +1400,13 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1402,16 +1414,19 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1419,16 +1434,16 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1436,16 +1451,16 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1453,16 +1468,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1470,10 +1485,10 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
       </c>
       <c r="E41" t="s">
         <v>85</v>
@@ -1487,16 +1502,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D42" t="s">
         <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1504,19 +1519,16 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1524,16 +1536,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F44" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1541,16 +1553,19 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
         <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1558,19 +1573,16 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1580,11 +1592,8 @@
       <c r="B47" t="s">
         <v>19</v>
       </c>
-      <c r="C47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
+      <c r="D47" t="s">
+        <v>87</v>
       </c>
       <c r="E47" t="s">
         <v>53</v>
@@ -1601,16 +1610,16 @@
         <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F48" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1618,16 +1627,19 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1635,19 +1647,19 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,17 +1669,14 @@
       <c r="B51" t="s">
         <v>9</v>
       </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
+      <c r="D51" t="s">
+        <v>87</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1675,16 +1684,19 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
       </c>
       <c r="F52" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1692,16 +1704,19 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1709,7 +1724,7 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
         <v>87</v>
@@ -1726,13 +1741,10 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
@@ -1746,7 +1758,7 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" t="s">
         <v>87</v>
@@ -1763,10 +1775,13 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
@@ -1780,7 +1795,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D58" t="s">
         <v>87</v>
@@ -1797,13 +1812,10 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E59" t="s">
         <v>11</v>
@@ -1817,16 +1829,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F60" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1834,16 +1846,19 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F61" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1851,16 +1866,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D62" t="s">
         <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1868,19 +1883,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D63" t="s">
+        <v>87</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1890,17 +1902,14 @@
       <c r="B64" t="s">
         <v>13</v>
       </c>
-      <c r="C64" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+      <c r="D64" t="s">
+        <v>87</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
       </c>
       <c r="F64" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1911,7 +1920,7 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1920,7 +1929,7 @@
         <v>14</v>
       </c>
       <c r="F65" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,16 +1937,19 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F66" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1945,16 +1957,19 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
-      </c>
-      <c r="D67" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1962,16 +1977,16 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" t="s">
-        <v>57</v>
+        <v>97</v>
+      </c>
+      <c r="D68" t="s">
+        <v>87</v>
       </c>
       <c r="E68" t="s">
         <v>54</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1981,17 +1996,14 @@
       <c r="B69" t="s">
         <v>33</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
+      <c r="D69" t="s">
+        <v>87</v>
       </c>
       <c r="E69" t="s">
         <v>54</v>
       </c>
       <c r="F69" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2001,17 +2013,14 @@
       <c r="B70" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+      <c r="C70" t="s">
+        <v>57</v>
       </c>
       <c r="E70" t="s">
         <v>54</v>
       </c>
       <c r="F70" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2019,15 +2028,55 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>54</v>
+      </c>
+      <c r="F71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>54</v>
+      </c>
+      <c r="F72" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73" t="s">
         <v>88</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D73" t="s">
         <v>65</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E73" t="s">
         <v>24</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (1.6) Promote snippets for GA release
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5FEB3-B198-4262-9DA9-3DC31BAAB322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB5342E-0296-4062-9D8A-5589C0EE720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -328,10 +328,10 @@
     <t>HyperlinkCollection</t>
   </si>
   <si>
-    <t>powerpoint-manage-hyperlinks</t>
-  </si>
-  <si>
     <t>getHyperlinks</t>
+  </si>
+  <si>
+    <t>powerpoint-hyperlinks-manage-hyperlinks</t>
   </si>
 </sst>
 </file>
@@ -374,10 +374,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +729,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,36 +818,34 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>102</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
         <v>102</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[PowerPoint] (1.6) Promote snippets for GA release (#941)
* [PowerPoint] (1.6) Promote snippets for GA release

* Updates
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5FEB3-B198-4262-9DA9-3DC31BAAB322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB5342E-0296-4062-9D8A-5589C0EE720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -328,10 +328,10 @@
     <t>HyperlinkCollection</t>
   </si>
   <si>
-    <t>powerpoint-manage-hyperlinks</t>
-  </si>
-  <si>
     <t>getHyperlinks</t>
+  </si>
+  <si>
+    <t>powerpoint-hyperlinks-manage-hyperlinks</t>
   </si>
 </sst>
 </file>
@@ -374,10 +374,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +729,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,36 +818,34 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>102</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
         <v>102</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[PowerPoint] Add group-ungroup-shapes snippet (#982)
* [PowerPoint] Add group-ungroup-shapes snippet

* Add API mapping
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB5342E-0296-4062-9D8A-5589C0EE720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3B9FDE-95E3-4718-8BA5-5E050892338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="111">
   <si>
     <t>Class</t>
   </si>
@@ -332,6 +332,27 @@
   </si>
   <si>
     <t>powerpoint-hyperlinks-manage-hyperlinks</t>
+  </si>
+  <si>
+    <t>addGroup</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-group-ungroup-shapes</t>
+  </si>
+  <si>
+    <t>groupShapes</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>ungroupShapes</t>
+  </si>
+  <si>
+    <t>ShapeGroup</t>
+  </si>
+  <si>
+    <t>ungroup</t>
   </si>
 </sst>
 </file>
@@ -374,9 +395,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +433,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F73" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F73" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F72">
-    <sortCondition ref="B1:B72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F77" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F77" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F76">
+    <sortCondition ref="B1:B76"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -725,11 +747,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,14 +1182,14 @@
       <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
+      <c r="C23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1178,7 +1200,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1195,7 +1217,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1212,13 +1234,13 @@
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,13 +1251,13 @@
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1243,16 +1265,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1260,16 +1282,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1279,17 +1301,14 @@
       <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+      <c r="D30" t="s">
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1300,7 +1319,7 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1309,7 +1328,7 @@
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1319,17 +1338,17 @@
       <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C32" t="s">
-        <v>29</v>
+      <c r="C32" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
+      <c r="E32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1340,16 +1359,16 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1360,16 +1379,16 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,16 +1396,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1394,16 +1416,19 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1413,17 +1438,14 @@
       <c r="B37" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
+      <c r="D37" t="s">
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1434,13 +1456,13 @@
         <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1448,16 +1470,19 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1465,16 +1490,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1482,16 +1507,16 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1499,33 +1524,34 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>62</v>
       </c>
       <c r="E42" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>32</v>
       </c>
-      <c r="B43" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" t="s">
-        <v>79</v>
+      <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1533,16 +1559,19 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" t="s">
-        <v>44</v>
+        <v>109</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1550,19 +1579,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1570,10 +1596,10 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
@@ -1587,16 +1613,16 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1604,19 +1630,16 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1624,10 +1647,10 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1636,7 +1659,7 @@
         <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1644,19 +1667,16 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1664,16 +1684,16 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D51" t="s">
         <v>87</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,19 +1701,19 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,19 +1721,19 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,16 +1741,19 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1738,16 +1761,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" t="s">
-        <v>74</v>
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>87</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,16 +1778,19 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
       </c>
       <c r="E56" t="s">
         <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1772,19 +1798,19 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F57" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1792,7 +1818,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D58" t="s">
         <v>87</v>
@@ -1809,7 +1835,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
@@ -1826,7 +1852,7 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
@@ -1843,7 +1869,7 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
         <v>70</v>
@@ -1863,16 +1889,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
         <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1880,16 +1906,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
-      </c>
-      <c r="D63" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F63" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,16 +1923,16 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
         <v>87</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F64" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1914,19 +1940,19 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1934,19 +1960,16 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" t="s">
-        <v>20</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1954,19 +1977,16 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1974,16 +1994,16 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
       </c>
       <c r="E68" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F68" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1991,16 +2011,19 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
-      </c>
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2008,16 +2031,19 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2025,19 +2051,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2045,19 +2071,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="D72" t="s">
+        <v>87</v>
       </c>
       <c r="E72" t="s">
         <v>54</v>
       </c>
       <c r="F72" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2065,15 +2088,89 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F73" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" t="s">
+        <v>54</v>
+      </c>
+      <c r="F74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F75" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F76" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>32</v>
+      </c>
+      <c r="B77" t="s">
         <v>88</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D77" t="s">
         <v>65</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E77" t="s">
         <v>24</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F77" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Add export-import-slide snippet (#978)
* [PowerPoint] Add export-import-slide snippet

* Updates based on suggestions

* API mappings

* Apply suggestions from code review

Co-authored-by: David Chesnut <davech@microsoft.com>

---------

Co-authored-by: David Chesnut <davech@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3B9FDE-95E3-4718-8BA5-5E050892338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46508F0-940A-4E1D-A8E0-6CC3EEAB364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Snippets" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="115">
   <si>
     <t>Class</t>
   </si>
@@ -334,19 +334,31 @@
     <t>powerpoint-hyperlinks-manage-hyperlinks</t>
   </si>
   <si>
+    <t>exportAsBase64</t>
+  </si>
+  <si>
+    <t>powerpoint-slide-management-export-import-slide</t>
+  </si>
+  <si>
+    <t>getImageAsBase64</t>
+  </si>
+  <si>
+    <t>exportSlide</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-group-ungroup-shapes</t>
+  </si>
+  <si>
+    <t>ungroupShapes</t>
+  </si>
+  <si>
     <t>addGroup</t>
   </si>
   <si>
-    <t>powerpoint-shapes-group-ungroup-shapes</t>
-  </si>
-  <si>
     <t>groupShapes</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>ungroupShapes</t>
   </si>
   <si>
     <t>ShapeGroup</t>
@@ -395,10 +407,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +444,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F77" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F77" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F76">
-    <sortCondition ref="B1:B76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F79" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F78">
+    <sortCondition ref="B1:B78"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -747,11 +758,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,14 +1193,14 @@
       <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="C23" t="s">
         <v>108</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1338,17 +1349,17 @@
       <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>104</v>
+      <c r="C32" t="s">
+        <v>111</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>106</v>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1540,18 +1551,17 @@
       <c r="A43" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="2"/>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
       <c r="D43" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>108</v>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1559,19 +1569,19 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="F44" t="s">
         <v>110</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1724,16 +1734,16 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F53" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1744,16 +1754,16 @@
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F54" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,16 +1771,19 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1778,19 +1791,19 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,17 +1813,14 @@
       <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C57" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
+      <c r="D57" t="s">
+        <v>87</v>
       </c>
       <c r="E57" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1818,16 +1828,19 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
-      </c>
-      <c r="D58" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
       </c>
       <c r="E58" t="s">
         <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1835,16 +1848,19 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1852,7 +1868,7 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
@@ -1869,13 +1885,10 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E61" t="s">
         <v>11</v>
@@ -1889,7 +1902,7 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D62" t="s">
         <v>87</v>
@@ -1906,10 +1919,13 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
       </c>
       <c r="E63" t="s">
         <v>11</v>
@@ -1923,7 +1939,7 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D64" t="s">
         <v>87</v>
@@ -1940,13 +1956,10 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E65" t="s">
         <v>11</v>
@@ -1960,16 +1973,16 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D66" t="s">
         <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,16 +1990,19 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
-      </c>
-      <c r="D67" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F67" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,16 +2010,16 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,19 +2027,16 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D69" t="s">
+        <v>87</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2033,17 +2046,14 @@
       <c r="B70" t="s">
         <v>13</v>
       </c>
-      <c r="C70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+      <c r="D70" t="s">
+        <v>87</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2054,7 +2064,7 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2063,7 +2073,7 @@
         <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2071,16 +2081,19 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D72" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F72" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2088,16 +2101,19 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
-      </c>
-      <c r="D73" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2105,16 +2121,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" t="s">
-        <v>57</v>
+        <v>97</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
       </c>
       <c r="E74" t="s">
         <v>54</v>
       </c>
       <c r="F74" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2124,17 +2140,14 @@
       <c r="B75" t="s">
         <v>33</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
+      <c r="D75" t="s">
+        <v>87</v>
       </c>
       <c r="E75" t="s">
         <v>54</v>
       </c>
       <c r="F75" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2144,17 +2157,14 @@
       <c r="B76" t="s">
         <v>33</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
+      <c r="C76" t="s">
+        <v>57</v>
       </c>
       <c r="E76" t="s">
         <v>54</v>
       </c>
       <c r="F76" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2162,15 +2172,55 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>54</v>
+      </c>
+      <c r="F77" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>54</v>
+      </c>
+      <c r="F78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" t="s">
         <v>88</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D79" t="s">
         <v>65</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>24</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update based on feedback and add API mapping
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46508F0-940A-4E1D-A8E0-6CC3EEAB364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE69A2-10C0-4C45-973C-27A3EC176BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="167">
   <si>
     <t>Class</t>
   </si>
@@ -365,6 +365,162 @@
   </si>
   <si>
     <t>ungroup</t>
+  </si>
+  <si>
+    <t>addTable</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-add-modify-tables</t>
+  </si>
+  <si>
+    <t>addBasicTable</t>
+  </si>
+  <si>
+    <t>TableAddOptions</t>
+  </si>
+  <si>
+    <t>tableWidthHeight</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>tableColumnWidthsRowHeights</t>
+  </si>
+  <si>
+    <t>tableValues</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>TableColumnProperties</t>
+  </si>
+  <si>
+    <t>TableRowProperties</t>
+  </si>
+  <si>
+    <t>columnWidth</t>
+  </si>
+  <si>
+    <t>rowHeight</t>
+  </si>
+  <si>
+    <t>mergedAreas</t>
+  </si>
+  <si>
+    <t>tableMergeAreas</t>
+  </si>
+  <si>
+    <t>TableMergedAreaProperties</t>
+  </si>
+  <si>
+    <t>columnCount</t>
+  </si>
+  <si>
+    <t>columnIndex</t>
+  </si>
+  <si>
+    <t>rowCount</t>
+  </si>
+  <si>
+    <t>rowIndex</t>
+  </si>
+  <si>
+    <t>specificCellProperties</t>
+  </si>
+  <si>
+    <t>tableCellFillFont</t>
+  </si>
+  <si>
+    <t>TableCellProperties</t>
+  </si>
+  <si>
+    <t>FillProperties</t>
+  </si>
+  <si>
+    <t>FontProperties</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>doubleStrikethrough</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>uniformCellProperties</t>
+  </si>
+  <si>
+    <t>tableBorders</t>
+  </si>
+  <si>
+    <t>borders</t>
+  </si>
+  <si>
+    <t>TableCellBorders</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>BorderProperties</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>indentLevel</t>
+  </si>
+  <si>
+    <t>tableIndentMargin</t>
+  </si>
+  <si>
+    <t>horizontalAlignment</t>
+  </si>
+  <si>
+    <t>verticalAlignment</t>
+  </si>
+  <si>
+    <t>tableCellAlignment</t>
+  </si>
+  <si>
+    <t>ParagraphHorizontalAlignment</t>
+  </si>
+  <si>
+    <t>getTableFromShape</t>
+  </si>
+  <si>
+    <t>getTable</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>updateTableValues</t>
+  </si>
+  <si>
+    <t>getCellOrNullObject</t>
+  </si>
+  <si>
+    <t>TableCell</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -444,10 +600,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F79" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F78">
-    <sortCondition ref="B1:B78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F129">
+    <sortCondition ref="B1:B129"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -758,11 +914,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,16 +974,16 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -835,16 +991,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -852,16 +1008,16 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -869,16 +1025,16 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -886,16 +1042,16 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,16 +1059,16 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -920,16 +1076,16 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -937,19 +1093,16 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,19 +1110,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,19 +1127,16 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,19 +1144,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,19 +1161,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,19 +1178,16 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,19 +1195,16 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,19 +1212,16 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,19 +1229,16 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1117,19 +1246,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1137,16 +1263,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1154,19 +1280,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1174,16 +1297,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>58</v>
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,16 +1314,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>108</v>
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1208,10 +1331,13 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1225,16 +1351,19 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1242,16 +1371,19 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1259,16 +1391,19 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1276,16 +1411,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,16 +1431,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,16 +1451,19 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,19 +1471,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1347,19 +1491,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1367,19 +1511,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1387,19 +1531,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1407,19 +1548,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1427,19 +1568,19 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1447,16 +1588,16 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1464,16 +1605,16 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1481,19 +1622,16 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
         <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,16 +1639,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1518,16 +1656,16 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1535,16 +1673,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1552,16 +1690,16 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1569,19 +1707,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1589,16 +1724,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1606,16 +1741,19 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1623,16 +1761,19 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>111</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,16 +1781,19 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,19 +1801,19 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1677,16 +1821,19 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" t="s">
-        <v>65</v>
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,16 +1841,19 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F51" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,19 +1861,19 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1731,19 +1881,19 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1751,19 +1901,16 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>87</v>
       </c>
       <c r="E54" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,19 +1918,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
         <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1791,10 +1935,10 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1803,7 +1947,7 @@
         <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,16 +1955,16 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1828,19 +1972,16 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="D58" t="s">
+        <v>87</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,19 +1989,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F59" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1868,16 +2006,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="F60" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1885,16 +2023,19 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>114</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="F61" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,16 +2043,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1919,19 +2060,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
+        <v>83</v>
+      </c>
+      <c r="D63" t="s">
+        <v>87</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,16 +2077,16 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D64" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,16 +2094,16 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+      <c r="D65" t="s">
+        <v>87</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1973,16 +2111,19 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,19 +2131,16 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
+        <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,7 +2148,7 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
@@ -2019,7 +2157,7 @@
         <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,16 +2165,19 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
-      </c>
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F69" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,16 +2185,19 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>104</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2061,19 +2205,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2081,19 +2225,19 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2101,19 +2245,19 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2121,16 +2265,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
         <v>87</v>
       </c>
       <c r="E74" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F74" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,16 +2282,19 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F75" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2155,16 +2302,19 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F76" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2172,19 +2322,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>87</v>
       </c>
       <c r="E77" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F77" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,19 +2339,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="C78" t="s">
+        <v>74</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,15 +2356,906 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="D81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
+        <v>69</v>
+      </c>
+      <c r="C84" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" t="s">
+        <v>53</v>
+      </c>
+      <c r="F85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>162</v>
+      </c>
+      <c r="D86" t="s">
+        <v>87</v>
+      </c>
+      <c r="E86" t="s">
+        <v>116</v>
+      </c>
+      <c r="F86" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" t="s">
+        <v>164</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>116</v>
+      </c>
+      <c r="F87" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" t="s">
+        <v>68</v>
+      </c>
+      <c r="E88" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" t="s">
+        <v>116</v>
+      </c>
+      <c r="F89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" t="s">
+        <v>116</v>
+      </c>
+      <c r="F90" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91" t="s">
+        <v>129</v>
+      </c>
+      <c r="E91" t="s">
+        <v>116</v>
+      </c>
+      <c r="F91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+      <c r="E92" t="s">
+        <v>116</v>
+      </c>
+      <c r="F92" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>32</v>
+      </c>
+      <c r="B93" t="s">
+        <v>118</v>
+      </c>
+      <c r="C93" t="s">
+        <v>136</v>
+      </c>
+      <c r="E93" t="s">
+        <v>116</v>
+      </c>
+      <c r="F93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94" t="s">
+        <v>146</v>
+      </c>
+      <c r="E94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F94" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>32</v>
+      </c>
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" t="s">
+        <v>120</v>
+      </c>
+      <c r="E95" t="s">
+        <v>116</v>
+      </c>
+      <c r="F95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" t="s">
+        <v>116</v>
+      </c>
+      <c r="F96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97" t="s">
+        <v>165</v>
+      </c>
+      <c r="D97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" t="s">
+        <v>116</v>
+      </c>
+      <c r="F97" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98" t="s">
+        <v>165</v>
+      </c>
+      <c r="C98" t="s">
+        <v>166</v>
+      </c>
+      <c r="E98" t="s">
+        <v>116</v>
+      </c>
+      <c r="F98" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99" t="s">
+        <v>68</v>
+      </c>
+      <c r="E99" t="s">
+        <v>116</v>
+      </c>
+      <c r="F99" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100" t="s">
+        <v>151</v>
+      </c>
+      <c r="E100" t="s">
+        <v>116</v>
+      </c>
+      <c r="F100" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" t="s">
+        <v>149</v>
+      </c>
+      <c r="C101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E101" t="s">
+        <v>116</v>
+      </c>
+      <c r="F101" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" t="s">
+        <v>149</v>
+      </c>
+      <c r="C102" t="s">
+        <v>150</v>
+      </c>
+      <c r="E102" t="s">
+        <v>116</v>
+      </c>
+      <c r="F102" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" t="s">
+        <v>149</v>
+      </c>
+      <c r="C103" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" t="s">
+        <v>116</v>
+      </c>
+      <c r="F103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>32</v>
+      </c>
+      <c r="B104" t="s">
+        <v>138</v>
+      </c>
+      <c r="D104" t="s">
+        <v>68</v>
+      </c>
+      <c r="E104" t="s">
+        <v>116</v>
+      </c>
+      <c r="F104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" t="s">
+        <v>138</v>
+      </c>
+      <c r="C105" t="s">
+        <v>148</v>
+      </c>
+      <c r="E105" t="s">
+        <v>116</v>
+      </c>
+      <c r="F105" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>32</v>
+      </c>
+      <c r="B106" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106" t="s">
+        <v>58</v>
+      </c>
+      <c r="E106" t="s">
+        <v>116</v>
+      </c>
+      <c r="F106" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C107" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" t="s">
+        <v>116</v>
+      </c>
+      <c r="F107" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>32</v>
+      </c>
+      <c r="B108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C108" t="s">
+        <v>156</v>
+      </c>
+      <c r="E108" t="s">
+        <v>116</v>
+      </c>
+      <c r="F108" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>32</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+      <c r="C109" t="s">
+        <v>154</v>
+      </c>
+      <c r="E109" t="s">
+        <v>116</v>
+      </c>
+      <c r="F109" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>32</v>
+      </c>
+      <c r="B110" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110" t="s">
+        <v>157</v>
+      </c>
+      <c r="E110" t="s">
+        <v>116</v>
+      </c>
+      <c r="F110" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>32</v>
+      </c>
+      <c r="B111" t="s">
+        <v>125</v>
+      </c>
+      <c r="D111" t="s">
+        <v>68</v>
+      </c>
+      <c r="E111" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>32</v>
+      </c>
+      <c r="B112" t="s">
+        <v>125</v>
+      </c>
+      <c r="C112" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" t="s">
+        <v>116</v>
+      </c>
+      <c r="F112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>32</v>
+      </c>
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+      <c r="D113" t="s">
+        <v>68</v>
+      </c>
+      <c r="E113" t="s">
+        <v>116</v>
+      </c>
+      <c r="F113" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
+        <v>132</v>
+      </c>
+      <c r="E114" t="s">
+        <v>116</v>
+      </c>
+      <c r="F114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" t="s">
+        <v>131</v>
+      </c>
+      <c r="C115" t="s">
+        <v>133</v>
+      </c>
+      <c r="E115" t="s">
+        <v>116</v>
+      </c>
+      <c r="F115" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" t="s">
+        <v>134</v>
+      </c>
+      <c r="E116" t="s">
+        <v>116</v>
+      </c>
+      <c r="F116" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117" t="s">
+        <v>131</v>
+      </c>
+      <c r="C117" t="s">
+        <v>135</v>
+      </c>
+      <c r="E117" t="s">
+        <v>116</v>
+      </c>
+      <c r="F117" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>32</v>
+      </c>
+      <c r="B118" t="s">
+        <v>126</v>
+      </c>
+      <c r="D118" t="s">
+        <v>68</v>
+      </c>
+      <c r="E118" t="s">
+        <v>116</v>
+      </c>
+      <c r="F118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>32</v>
+      </c>
+      <c r="B119" t="s">
+        <v>126</v>
+      </c>
+      <c r="C119" t="s">
+        <v>128</v>
+      </c>
+      <c r="E119" t="s">
+        <v>116</v>
+      </c>
+      <c r="F119" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>32</v>
+      </c>
+      <c r="B120" t="s">
+        <v>98</v>
+      </c>
+      <c r="D120" t="s">
+        <v>87</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>32</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" t="s">
+        <v>87</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>32</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>32</v>
+      </c>
+      <c r="B123" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>32</v>
+      </c>
+      <c r="B124" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>32</v>
+      </c>
+      <c r="B125" t="s">
+        <v>97</v>
+      </c>
+      <c r="D125" t="s">
+        <v>87</v>
+      </c>
+      <c r="E125" t="s">
+        <v>54</v>
+      </c>
+      <c r="F125" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" t="s">
+        <v>33</v>
+      </c>
+      <c r="D126" t="s">
+        <v>87</v>
+      </c>
+      <c r="E126" t="s">
+        <v>54</v>
+      </c>
+      <c r="F126" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>32</v>
+      </c>
+      <c r="B127" t="s">
+        <v>33</v>
+      </c>
+      <c r="C127" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" t="s">
+        <v>54</v>
+      </c>
+      <c r="F127" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" t="s">
+        <v>54</v>
+      </c>
+      <c r="F128" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129" t="s">
+        <v>54</v>
+      </c>
+      <c r="F129" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>32</v>
+      </c>
+      <c r="B130" t="s">
         <v>88</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D130" t="s">
         <v>65</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E130" t="s">
         <v>24</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F130" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Add add-modify-tables snippet (#979)
* [PowerPoint] Add add-modify-tables snippet

* Update how to update table values

* Update based on feedback and add API mapping
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46508F0-940A-4E1D-A8E0-6CC3EEAB364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE69A2-10C0-4C45-973C-27A3EC176BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="167">
   <si>
     <t>Class</t>
   </si>
@@ -365,6 +365,162 @@
   </si>
   <si>
     <t>ungroup</t>
+  </si>
+  <si>
+    <t>addTable</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-add-modify-tables</t>
+  </si>
+  <si>
+    <t>addBasicTable</t>
+  </si>
+  <si>
+    <t>TableAddOptions</t>
+  </si>
+  <si>
+    <t>tableWidthHeight</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>tableColumnWidthsRowHeights</t>
+  </si>
+  <si>
+    <t>tableValues</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>TableColumnProperties</t>
+  </si>
+  <si>
+    <t>TableRowProperties</t>
+  </si>
+  <si>
+    <t>columnWidth</t>
+  </si>
+  <si>
+    <t>rowHeight</t>
+  </si>
+  <si>
+    <t>mergedAreas</t>
+  </si>
+  <si>
+    <t>tableMergeAreas</t>
+  </si>
+  <si>
+    <t>TableMergedAreaProperties</t>
+  </si>
+  <si>
+    <t>columnCount</t>
+  </si>
+  <si>
+    <t>columnIndex</t>
+  </si>
+  <si>
+    <t>rowCount</t>
+  </si>
+  <si>
+    <t>rowIndex</t>
+  </si>
+  <si>
+    <t>specificCellProperties</t>
+  </si>
+  <si>
+    <t>tableCellFillFont</t>
+  </si>
+  <si>
+    <t>TableCellProperties</t>
+  </si>
+  <si>
+    <t>FillProperties</t>
+  </si>
+  <si>
+    <t>FontProperties</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>doubleStrikethrough</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>uniformCellProperties</t>
+  </si>
+  <si>
+    <t>tableBorders</t>
+  </si>
+  <si>
+    <t>borders</t>
+  </si>
+  <si>
+    <t>TableCellBorders</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>BorderProperties</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>indentLevel</t>
+  </si>
+  <si>
+    <t>tableIndentMargin</t>
+  </si>
+  <si>
+    <t>horizontalAlignment</t>
+  </si>
+  <si>
+    <t>verticalAlignment</t>
+  </si>
+  <si>
+    <t>tableCellAlignment</t>
+  </si>
+  <si>
+    <t>ParagraphHorizontalAlignment</t>
+  </si>
+  <si>
+    <t>getTableFromShape</t>
+  </si>
+  <si>
+    <t>getTable</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>updateTableValues</t>
+  </si>
+  <si>
+    <t>getCellOrNullObject</t>
+  </si>
+  <si>
+    <t>TableCell</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -444,10 +600,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F79" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F79" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F78">
-    <sortCondition ref="B1:B78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F129">
+    <sortCondition ref="B1:B129"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -758,11 +914,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,16 +974,16 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -835,16 +991,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -852,16 +1008,16 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -869,16 +1025,16 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -886,16 +1042,16 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,16 +1059,16 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -920,16 +1076,16 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -937,19 +1093,16 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,19 +1110,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,19 +1127,16 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,19 +1144,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,19 +1161,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,19 +1178,16 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,19 +1195,16 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,19 +1212,16 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,19 +1229,16 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1117,19 +1246,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1137,16 +1263,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1154,19 +1280,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1174,16 +1297,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>58</v>
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,16 +1314,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>108</v>
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1208,10 +1331,13 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1225,16 +1351,19 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1242,16 +1371,19 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1259,16 +1391,19 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1276,16 +1411,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,16 +1431,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,16 +1451,19 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,19 +1471,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1347,19 +1491,19 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1367,19 +1511,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1387,19 +1531,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1407,19 +1548,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1427,19 +1568,19 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1447,16 +1588,16 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1464,16 +1605,16 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1481,19 +1622,16 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
         <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,16 +1639,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1518,16 +1656,16 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1535,16 +1673,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1552,16 +1690,16 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1569,19 +1707,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1589,16 +1724,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1606,16 +1741,19 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1623,16 +1761,19 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>111</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,16 +1781,19 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,19 +1801,19 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1677,16 +1821,19 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" t="s">
-        <v>65</v>
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,16 +1841,19 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F51" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,19 +1861,19 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1731,19 +1881,19 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1751,19 +1901,16 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>87</v>
       </c>
       <c r="E54" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,19 +1918,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
         <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1791,10 +1935,10 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1803,7 +1947,7 @@
         <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,16 +1955,16 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1828,19 +1972,16 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="D58" t="s">
+        <v>87</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,19 +1989,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F59" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1868,16 +2006,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="D60" t="s">
         <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="F60" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1885,16 +2023,19 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>114</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="F61" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,16 +2043,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1919,19 +2060,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
+        <v>83</v>
+      </c>
+      <c r="D63" t="s">
+        <v>87</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,16 +2077,16 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D64" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,16 +2094,16 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+      <c r="D65" t="s">
+        <v>87</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1973,16 +2111,19 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,19 +2131,16 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
+        <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,7 +2148,7 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
@@ -2019,7 +2157,7 @@
         <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,16 +2165,19 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
-      </c>
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F69" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,16 +2185,19 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>104</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2061,19 +2205,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2081,19 +2225,19 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2101,19 +2245,19 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2121,16 +2265,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
         <v>87</v>
       </c>
       <c r="E74" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F74" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,16 +2282,19 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F75" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2155,16 +2302,19 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F76" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2172,19 +2322,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>87</v>
       </c>
       <c r="E77" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F77" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,19 +2339,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="C78" t="s">
+        <v>74</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,15 +2356,906 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="D81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
+        <v>69</v>
+      </c>
+      <c r="C84" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" t="s">
+        <v>53</v>
+      </c>
+      <c r="F85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>162</v>
+      </c>
+      <c r="D86" t="s">
+        <v>87</v>
+      </c>
+      <c r="E86" t="s">
+        <v>116</v>
+      </c>
+      <c r="F86" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" t="s">
+        <v>164</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>116</v>
+      </c>
+      <c r="F87" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" t="s">
+        <v>68</v>
+      </c>
+      <c r="E88" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" t="s">
+        <v>116</v>
+      </c>
+      <c r="F89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" t="s">
+        <v>116</v>
+      </c>
+      <c r="F90" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91" t="s">
+        <v>129</v>
+      </c>
+      <c r="E91" t="s">
+        <v>116</v>
+      </c>
+      <c r="F91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+      <c r="E92" t="s">
+        <v>116</v>
+      </c>
+      <c r="F92" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>32</v>
+      </c>
+      <c r="B93" t="s">
+        <v>118</v>
+      </c>
+      <c r="C93" t="s">
+        <v>136</v>
+      </c>
+      <c r="E93" t="s">
+        <v>116</v>
+      </c>
+      <c r="F93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94" t="s">
+        <v>146</v>
+      </c>
+      <c r="E94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F94" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>32</v>
+      </c>
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" t="s">
+        <v>120</v>
+      </c>
+      <c r="E95" t="s">
+        <v>116</v>
+      </c>
+      <c r="F95" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" t="s">
+        <v>116</v>
+      </c>
+      <c r="F96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97" t="s">
+        <v>165</v>
+      </c>
+      <c r="D97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" t="s">
+        <v>116</v>
+      </c>
+      <c r="F97" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98" t="s">
+        <v>165</v>
+      </c>
+      <c r="C98" t="s">
+        <v>166</v>
+      </c>
+      <c r="E98" t="s">
+        <v>116</v>
+      </c>
+      <c r="F98" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99" t="s">
+        <v>68</v>
+      </c>
+      <c r="E99" t="s">
+        <v>116</v>
+      </c>
+      <c r="F99" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100" t="s">
+        <v>151</v>
+      </c>
+      <c r="E100" t="s">
+        <v>116</v>
+      </c>
+      <c r="F100" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" t="s">
+        <v>149</v>
+      </c>
+      <c r="C101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E101" t="s">
+        <v>116</v>
+      </c>
+      <c r="F101" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" t="s">
+        <v>149</v>
+      </c>
+      <c r="C102" t="s">
+        <v>150</v>
+      </c>
+      <c r="E102" t="s">
+        <v>116</v>
+      </c>
+      <c r="F102" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" t="s">
+        <v>149</v>
+      </c>
+      <c r="C103" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" t="s">
+        <v>116</v>
+      </c>
+      <c r="F103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>32</v>
+      </c>
+      <c r="B104" t="s">
+        <v>138</v>
+      </c>
+      <c r="D104" t="s">
+        <v>68</v>
+      </c>
+      <c r="E104" t="s">
+        <v>116</v>
+      </c>
+      <c r="F104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" t="s">
+        <v>138</v>
+      </c>
+      <c r="C105" t="s">
+        <v>148</v>
+      </c>
+      <c r="E105" t="s">
+        <v>116</v>
+      </c>
+      <c r="F105" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>32</v>
+      </c>
+      <c r="B106" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106" t="s">
+        <v>58</v>
+      </c>
+      <c r="E106" t="s">
+        <v>116</v>
+      </c>
+      <c r="F106" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C107" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" t="s">
+        <v>116</v>
+      </c>
+      <c r="F107" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>32</v>
+      </c>
+      <c r="B108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C108" t="s">
+        <v>156</v>
+      </c>
+      <c r="E108" t="s">
+        <v>116</v>
+      </c>
+      <c r="F108" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>32</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+      <c r="C109" t="s">
+        <v>154</v>
+      </c>
+      <c r="E109" t="s">
+        <v>116</v>
+      </c>
+      <c r="F109" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>32</v>
+      </c>
+      <c r="B110" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110" t="s">
+        <v>157</v>
+      </c>
+      <c r="E110" t="s">
+        <v>116</v>
+      </c>
+      <c r="F110" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>32</v>
+      </c>
+      <c r="B111" t="s">
+        <v>125</v>
+      </c>
+      <c r="D111" t="s">
+        <v>68</v>
+      </c>
+      <c r="E111" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>32</v>
+      </c>
+      <c r="B112" t="s">
+        <v>125</v>
+      </c>
+      <c r="C112" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" t="s">
+        <v>116</v>
+      </c>
+      <c r="F112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>32</v>
+      </c>
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+      <c r="D113" t="s">
+        <v>68</v>
+      </c>
+      <c r="E113" t="s">
+        <v>116</v>
+      </c>
+      <c r="F113" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
+        <v>132</v>
+      </c>
+      <c r="E114" t="s">
+        <v>116</v>
+      </c>
+      <c r="F114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" t="s">
+        <v>131</v>
+      </c>
+      <c r="C115" t="s">
+        <v>133</v>
+      </c>
+      <c r="E115" t="s">
+        <v>116</v>
+      </c>
+      <c r="F115" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" t="s">
+        <v>134</v>
+      </c>
+      <c r="E116" t="s">
+        <v>116</v>
+      </c>
+      <c r="F116" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117" t="s">
+        <v>131</v>
+      </c>
+      <c r="C117" t="s">
+        <v>135</v>
+      </c>
+      <c r="E117" t="s">
+        <v>116</v>
+      </c>
+      <c r="F117" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>32</v>
+      </c>
+      <c r="B118" t="s">
+        <v>126</v>
+      </c>
+      <c r="D118" t="s">
+        <v>68</v>
+      </c>
+      <c r="E118" t="s">
+        <v>116</v>
+      </c>
+      <c r="F118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>32</v>
+      </c>
+      <c r="B119" t="s">
+        <v>126</v>
+      </c>
+      <c r="C119" t="s">
+        <v>128</v>
+      </c>
+      <c r="E119" t="s">
+        <v>116</v>
+      </c>
+      <c r="F119" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>32</v>
+      </c>
+      <c r="B120" t="s">
+        <v>98</v>
+      </c>
+      <c r="D120" t="s">
+        <v>87</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>32</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" t="s">
+        <v>87</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>32</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>32</v>
+      </c>
+      <c r="B123" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>32</v>
+      </c>
+      <c r="B124" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>32</v>
+      </c>
+      <c r="B125" t="s">
+        <v>97</v>
+      </c>
+      <c r="D125" t="s">
+        <v>87</v>
+      </c>
+      <c r="E125" t="s">
+        <v>54</v>
+      </c>
+      <c r="F125" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" t="s">
+        <v>33</v>
+      </c>
+      <c r="D126" t="s">
+        <v>87</v>
+      </c>
+      <c r="E126" t="s">
+        <v>54</v>
+      </c>
+      <c r="F126" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>32</v>
+      </c>
+      <c r="B127" t="s">
+        <v>33</v>
+      </c>
+      <c r="C127" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" t="s">
+        <v>54</v>
+      </c>
+      <c r="F127" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" t="s">
+        <v>54</v>
+      </c>
+      <c r="F128" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>32</v>
+      </c>
+      <c r="B129" t="s">
+        <v>33</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129" t="s">
+        <v>54</v>
+      </c>
+      <c r="F129" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>32</v>
+      </c>
+      <c r="B130" t="s">
         <v>88</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D130" t="s">
         <v>65</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E130" t="s">
         <v>24</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F130" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Add binding-to-shapes snippet (#980)
* [PowerPoint] Add binding-to-shapes snippet

* Apply suggestions from code review

Co-authored-by: David Chesnut <davech@microsoft.com>

* Updates based on feedback

* Add API mappings

* Remove API mapping

* Update images

* Re-add API mapping

---------

Co-authored-by: David Chesnut <davech@microsoft.com>
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE69A2-10C0-4C45-973C-27A3EC176BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D30CE19-32FD-41C6-AE1E-126407A50794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="182">
   <si>
     <t>Class</t>
   </si>
@@ -521,6 +521,51 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>powerpoint-shapes-binding-to-shapes</t>
+  </si>
+  <si>
+    <t>getShapeForBindingId</t>
+  </si>
+  <si>
+    <t>getShape</t>
+  </si>
+  <si>
+    <t>BindingCollection</t>
+  </si>
+  <si>
+    <t>loadBindings</t>
+  </si>
+  <si>
+    <t>insertImageWithBinding</t>
+  </si>
+  <si>
+    <t>BindingType</t>
+  </si>
+  <si>
+    <t>bindings</t>
+  </si>
+  <si>
+    <t>setZOrder</t>
+  </si>
+  <si>
+    <t>changeZOrder</t>
+  </si>
+  <si>
+    <t>zOrderPosition</t>
+  </si>
+  <si>
+    <t>setImage</t>
+  </si>
+  <si>
+    <t>ShapeZOrder</t>
+  </si>
+  <si>
+    <t>sendToBack</t>
   </si>
 </sst>
 </file>
@@ -563,9 +608,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,10 +646,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F130" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F130" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F129">
-    <sortCondition ref="B1:B129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F142" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F142" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F141">
+    <sortCondition ref="B1:B141"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -914,11 +960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,102 +1019,114 @@
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>152</v>
-      </c>
+      <c r="B3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>147</v>
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" t="s">
-        <v>147</v>
+      <c r="B4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" t="s">
-        <v>147</v>
+      <c r="B5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>147</v>
+      <c r="B6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
+      <c r="B7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
+      <c r="B8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1076,16 +1134,16 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
+        <v>152</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1093,16 +1151,16 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
+        <v>152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
       </c>
       <c r="E10" t="s">
         <v>116</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1110,16 +1168,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
         <v>116</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1127,16 +1185,16 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
         <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1144,16 +1202,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" t="s">
-        <v>141</v>
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1161,10 +1219,10 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
       </c>
       <c r="E14" t="s">
         <v>116</v>
@@ -1178,10 +1236,10 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>116</v>
@@ -1197,8 +1255,8 @@
       <c r="B16" t="s">
         <v>140</v>
       </c>
-      <c r="C16" t="s">
-        <v>145</v>
+      <c r="D16" t="s">
+        <v>68</v>
       </c>
       <c r="E16" t="s">
         <v>116</v>
@@ -1212,16 +1270,16 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,16 +1287,16 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
+        <v>140</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1246,16 +1304,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" t="s">
-        <v>87</v>
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1263,16 +1321,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="C20" t="s">
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1280,16 +1338,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1297,16 +1355,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1314,16 +1372,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1331,19 +1389,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1351,19 +1406,16 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1371,19 +1423,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1391,19 +1440,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1411,19 +1457,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="D28" t="s">
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1433,17 +1476,14 @@
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
+      <c r="D29" t="s">
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1454,16 +1494,16 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1474,16 +1514,16 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1494,16 +1534,16 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1514,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1523,7 +1563,7 @@
         <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,16 +1571,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1548,19 +1591,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1568,19 +1611,19 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,16 +1631,19 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1605,16 +1651,19 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1622,16 +1671,19 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1639,16 +1691,16 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" t="s">
-        <v>48</v>
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1658,14 +1710,14 @@
       <c r="B41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
-        <v>50</v>
+      <c r="D41" t="s">
+        <v>87</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,13 +1728,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1693,13 +1748,16 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>161</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F43" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1707,16 +1765,19 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1724,16 +1785,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1741,19 +1802,16 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,19 +1819,16 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1781,19 +1836,16 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1801,19 +1853,16 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1821,19 +1870,16 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1841,19 +1887,16 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="E51" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,19 +1904,16 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1881,19 +1921,16 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
       </c>
       <c r="E53" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F53" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1901,7 +1938,7 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D54" t="s">
         <v>87</v>
@@ -1918,16 +1955,19 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>25</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F55" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1935,19 +1975,19 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F56" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1955,16 +1995,19 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>27</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1972,16 +2015,19 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1989,16 +2035,19 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2006,16 +2055,19 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F60" t="s">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2023,19 +2075,19 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2043,16 +2095,19 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
-      </c>
-      <c r="D62" t="s">
-        <v>65</v>
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
       </c>
       <c r="E62" t="s">
         <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2060,7 +2115,7 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D63" t="s">
         <v>87</v>
@@ -2069,7 +2124,7 @@
         <v>85</v>
       </c>
       <c r="F63" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,16 +2132,19 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>179</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F64" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2094,10 +2152,13 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
       </c>
       <c r="E65" t="s">
         <v>53</v>
@@ -2111,19 +2172,16 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E66" t="s">
         <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2131,16 +2189,16 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C67" t="s">
+        <v>82</v>
       </c>
       <c r="E67" t="s">
         <v>85</v>
       </c>
       <c r="F67" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2148,16 +2206,16 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
         <v>87</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F68" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2165,19 +2223,16 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E69" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F69" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2185,19 +2240,16 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" t="s">
-        <v>104</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="D70" t="s">
+        <v>87</v>
       </c>
       <c r="E70" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F70" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2205,19 +2257,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F71" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,19 +2277,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" t="s">
-        <v>38</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="D72" t="s">
+        <v>65</v>
       </c>
       <c r="E72" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F72" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,19 +2294,16 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
-      </c>
-      <c r="C73" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D73" t="s">
+        <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2265,16 +2311,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>84</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2282,19 +2328,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D75" t="s">
+        <v>87</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2302,19 +2345,19 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C76" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2322,50 +2365,52 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D77" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>32</v>
       </c>
-      <c r="B78" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" t="s">
-        <v>74</v>
-      </c>
-      <c r="E78" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" t="s">
-        <v>71</v>
+      <c r="B78" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" t="s">
+        <v>65</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>32</v>
       </c>
-      <c r="B79" t="s">
-        <v>72</v>
-      </c>
+      <c r="B79" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="2"/>
       <c r="D79" t="s">
-        <v>87</v>
-      </c>
-      <c r="E79" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,19 +2418,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
-      </c>
-      <c r="C80" t="s">
-        <v>70</v>
-      </c>
-      <c r="D80">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="D80" t="s">
+        <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F80" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2393,16 +2435,19 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>73</v>
-      </c>
-      <c r="D81" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F81" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2410,16 +2455,19 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>104</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F82" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2427,16 +2475,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
-      </c>
-      <c r="D83" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C83" t="s">
+        <v>106</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F83" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2444,19 +2495,19 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C84" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F84" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2464,16 +2515,19 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
       </c>
       <c r="E85" t="s">
         <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2481,16 +2535,16 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>9</v>
       </c>
       <c r="D86" t="s">
         <v>87</v>
       </c>
       <c r="E86" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F86" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2498,19 +2552,19 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>162</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F87" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2518,16 +2572,19 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>118</v>
-      </c>
-      <c r="D88" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="F88" t="s">
-        <v>119</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2535,16 +2592,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>118</v>
-      </c>
-      <c r="C89" t="s">
-        <v>124</v>
+        <v>75</v>
+      </c>
+      <c r="D89" t="s">
+        <v>87</v>
       </c>
       <c r="E89" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F89" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2552,16 +2609,16 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="C90" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="E90" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F90" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2569,16 +2626,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>118</v>
-      </c>
-      <c r="C91" t="s">
-        <v>129</v>
+        <v>72</v>
+      </c>
+      <c r="D91" t="s">
+        <v>87</v>
       </c>
       <c r="E91" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F91" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2586,16 +2643,19 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
+        <v>70</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F92" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2603,16 +2663,16 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>118</v>
-      </c>
-      <c r="C93" t="s">
-        <v>136</v>
+        <v>73</v>
+      </c>
+      <c r="D93" t="s">
+        <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F93" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2620,16 +2680,16 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="C94" t="s">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="E94" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F94" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2637,16 +2697,16 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>118</v>
-      </c>
-      <c r="C95" t="s">
-        <v>120</v>
+        <v>69</v>
+      </c>
+      <c r="D95" t="s">
+        <v>87</v>
       </c>
       <c r="E95" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2654,16 +2714,19 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="C96" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F96" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2671,16 +2734,16 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="D97" t="s">
         <v>87</v>
       </c>
       <c r="E97" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F97" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2688,10 +2751,10 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
-      </c>
-      <c r="C98" t="s">
-        <v>166</v>
+        <v>162</v>
+      </c>
+      <c r="D98" t="s">
+        <v>87</v>
       </c>
       <c r="E98" t="s">
         <v>116</v>
@@ -2705,16 +2768,19 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>149</v>
-      </c>
-      <c r="D99" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C99" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99" t="s">
         <v>116</v>
       </c>
       <c r="F99" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2722,16 +2788,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>149</v>
-      </c>
-      <c r="C100" t="s">
-        <v>151</v>
+        <v>118</v>
+      </c>
+      <c r="D100" t="s">
+        <v>68</v>
       </c>
       <c r="E100" t="s">
         <v>116</v>
       </c>
       <c r="F100" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2739,16 +2805,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="E101" t="s">
         <v>116</v>
       </c>
       <c r="F101" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2822,16 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C102" t="s">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
       <c r="F102" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2773,16 +2839,16 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="E103" t="s">
         <v>116</v>
       </c>
       <c r="F103" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2790,16 +2856,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
-      </c>
-      <c r="D104" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="C104" t="s">
+        <v>123</v>
       </c>
       <c r="E104" t="s">
         <v>116</v>
       </c>
       <c r="F104" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2807,16 +2873,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2824,16 +2890,16 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2841,16 +2907,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2858,16 +2924,16 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2875,16 +2941,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>138</v>
-      </c>
-      <c r="C109" t="s">
-        <v>154</v>
+        <v>165</v>
+      </c>
+      <c r="D109" t="s">
+        <v>87</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2892,16 +2958,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="C110" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2909,7 +2975,7 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="D111" t="s">
         <v>68</v>
@@ -2918,7 +2984,7 @@
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2926,16 +2992,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C112" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -2943,16 +3009,16 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>131</v>
-      </c>
-      <c r="D113" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C113" t="s">
+        <v>49</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -2960,16 +3026,16 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -2977,16 +3043,16 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>133</v>
+        <v>50</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -2994,16 +3060,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
-      </c>
-      <c r="C116" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="D116" t="s">
+        <v>68</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3011,16 +3077,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C117" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3028,16 +3094,16 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>126</v>
-      </c>
-      <c r="D118" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C118" t="s">
+        <v>58</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3045,16 +3111,16 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C119" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3062,16 +3128,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>98</v>
-      </c>
-      <c r="D120" t="s">
-        <v>87</v>
+        <v>138</v>
+      </c>
+      <c r="C120" t="s">
+        <v>156</v>
       </c>
       <c r="E120" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3079,16 +3145,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
-      </c>
-      <c r="D121" t="s">
-        <v>87</v>
+        <v>138</v>
+      </c>
+      <c r="C121" t="s">
+        <v>154</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3096,19 +3162,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="C122" t="s">
-        <v>10</v>
-      </c>
-      <c r="D122">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>15</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3116,19 +3179,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>13</v>
-      </c>
-      <c r="C123" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="D123" t="s">
+        <v>68</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3136,19 +3196,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="C124" t="s">
-        <v>18</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="E124" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3156,16 +3213,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="D125" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E125" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,16 +3230,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>33</v>
-      </c>
-      <c r="D126" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C126" t="s">
+        <v>132</v>
       </c>
       <c r="E126" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3190,16 +3247,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="C127" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="E127" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,19 +3264,16 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>33</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D128">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="C128" t="s">
+        <v>134</v>
       </c>
       <c r="E128" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3227,19 +3281,16 @@
         <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>33</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D129">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="C129" t="s">
+        <v>135</v>
       </c>
       <c r="E129" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3247,15 +3298,234 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" t="s">
+        <v>68</v>
+      </c>
+      <c r="E130" t="s">
+        <v>116</v>
+      </c>
+      <c r="F130" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>32</v>
+      </c>
+      <c r="B131" t="s">
+        <v>126</v>
+      </c>
+      <c r="C131" t="s">
+        <v>128</v>
+      </c>
+      <c r="E131" t="s">
+        <v>116</v>
+      </c>
+      <c r="F131" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>32</v>
+      </c>
+      <c r="B132" t="s">
+        <v>98</v>
+      </c>
+      <c r="D132" t="s">
+        <v>87</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>32</v>
+      </c>
+      <c r="B133" t="s">
+        <v>13</v>
+      </c>
+      <c r="D133" t="s">
+        <v>87</v>
+      </c>
+      <c r="E133" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>32</v>
+      </c>
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>32</v>
+      </c>
+      <c r="B135" t="s">
+        <v>13</v>
+      </c>
+      <c r="C135" t="s">
+        <v>20</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135" t="s">
+        <v>14</v>
+      </c>
+      <c r="F135" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>32</v>
+      </c>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" t="s">
+        <v>18</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>32</v>
+      </c>
+      <c r="B137" t="s">
+        <v>97</v>
+      </c>
+      <c r="D137" t="s">
+        <v>87</v>
+      </c>
+      <c r="E137" t="s">
+        <v>54</v>
+      </c>
+      <c r="F137" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>32</v>
+      </c>
+      <c r="B138" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
+        <v>87</v>
+      </c>
+      <c r="E138" t="s">
+        <v>54</v>
+      </c>
+      <c r="F138" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>32</v>
+      </c>
+      <c r="B139" t="s">
+        <v>33</v>
+      </c>
+      <c r="C139" t="s">
+        <v>57</v>
+      </c>
+      <c r="E139" t="s">
+        <v>54</v>
+      </c>
+      <c r="F139" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>32</v>
+      </c>
+      <c r="B140" t="s">
+        <v>33</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>54</v>
+      </c>
+      <c r="F140" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>32</v>
+      </c>
+      <c r="B141" t="s">
+        <v>33</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141" t="s">
+        <v>54</v>
+      </c>
+      <c r="F141" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>32</v>
+      </c>
+      <c r="B142" t="s">
         <v>88</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D142" t="s">
         <v>65</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E142" t="s">
         <v>24</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F142" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (tables) Work with text runs
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D30CE19-32FD-41C6-AE1E-126407A50794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3FA6A-923C-4ABF-8AAF-E4C511BAF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="185">
   <si>
     <t>Class</t>
   </si>
@@ -566,6 +566,15 @@
   </si>
   <si>
     <t>sendToBack</t>
+  </si>
+  <si>
+    <t>TextRun</t>
+  </si>
+  <si>
+    <t>tableTextRuns</t>
+  </si>
+  <si>
+    <t>textRuns</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,10 +656,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F142" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F142" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F141">
-    <sortCondition ref="B1:B141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F144" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F144" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F142">
+    <sortCondition ref="B1:B142"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -960,11 +970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,17 +1029,16 @@
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>168</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1037,19 +1046,19 @@
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>170</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1057,17 +1066,16 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1075,19 +1083,19 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1095,19 +1103,19 @@
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1115,17 +1123,16 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1693,13 +1700,13 @@
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" t="s">
         <v>168</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2381,17 +2388,16 @@
       <c r="A78" t="s">
         <v>32</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" t="s">
         <v>180</v>
       </c>
-      <c r="C78" s="2"/>
       <c r="D78" t="s">
         <v>65</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" t="s">
         <v>168</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2399,17 +2405,16 @@
       <c r="A79" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2"/>
       <c r="D79" t="s">
         <v>65</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" t="s">
         <v>168</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3164,14 +3169,14 @@
       <c r="B122" t="s">
         <v>138</v>
       </c>
-      <c r="C122" t="s">
-        <v>157</v>
+      <c r="C122" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
-      <c r="F122" t="s">
-        <v>158</v>
+      <c r="F122" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3179,16 +3184,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>125</v>
-      </c>
-      <c r="D123" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C123" t="s">
+        <v>157</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,8 +3203,8 @@
       <c r="B124" t="s">
         <v>125</v>
       </c>
-      <c r="C124" t="s">
-        <v>127</v>
+      <c r="D124" t="s">
+        <v>68</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3213,16 +3218,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>131</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C125" t="s">
+        <v>127</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3232,8 +3237,8 @@
       <c r="B126" t="s">
         <v>131</v>
       </c>
-      <c r="C126" t="s">
-        <v>132</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3250,7 +3255,7 @@
         <v>131</v>
       </c>
       <c r="C127" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3267,7 +3272,7 @@
         <v>131</v>
       </c>
       <c r="C128" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3284,7 +3289,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3298,16 +3303,16 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>126</v>
-      </c>
-      <c r="D130" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C130" t="s">
+        <v>135</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3317,8 +3322,8 @@
       <c r="B131" t="s">
         <v>126</v>
       </c>
-      <c r="C131" t="s">
-        <v>128</v>
+      <c r="D131" t="s">
+        <v>68</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3332,16 +3337,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>98</v>
-      </c>
-      <c r="D132" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C132" t="s">
+        <v>128</v>
       </c>
       <c r="E132" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,7 +3354,7 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D133" t="s">
         <v>87</v>
@@ -3358,7 +3363,7 @@
         <v>14</v>
       </c>
       <c r="F133" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3368,17 +3373,14 @@
       <c r="B134" t="s">
         <v>13</v>
       </c>
-      <c r="C134" t="s">
-        <v>10</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
+      <c r="D134" t="s">
+        <v>87</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3389,7 +3391,7 @@
         <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3398,7 +3400,7 @@
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3409,7 +3411,7 @@
         <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3418,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3426,16 +3428,19 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>97</v>
-      </c>
-      <c r="D137" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C137" t="s">
+        <v>18</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
       </c>
       <c r="E137" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3443,7 +3448,7 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D138" t="s">
         <v>87</v>
@@ -3452,7 +3457,7 @@
         <v>54</v>
       </c>
       <c r="F138" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3462,8 +3467,8 @@
       <c r="B139" t="s">
         <v>33</v>
       </c>
-      <c r="C139" t="s">
-        <v>57</v>
+      <c r="D139" t="s">
+        <v>87</v>
       </c>
       <c r="E139" t="s">
         <v>54</v>
@@ -3479,17 +3484,14 @@
       <c r="B140" t="s">
         <v>33</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
+      <c r="C140" t="s">
+        <v>57</v>
       </c>
       <c r="E140" t="s">
         <v>54</v>
       </c>
       <c r="F140" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,7 +3511,7 @@
         <v>54</v>
       </c>
       <c r="F141" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3517,15 +3519,53 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>54</v>
+      </c>
+      <c r="F142" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>32</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C143" s="3"/>
+      <c r="D143" t="s">
+        <v>68</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>32</v>
+      </c>
+      <c r="B144" t="s">
         <v>88</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D144" t="s">
         <v>65</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E144" t="s">
         <v>24</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F144" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (tables) Work with text runs (#986)
* [PowerPoint] (tables) Work with text runs

* Add HTML

* Update based on feedback

* Updates based on feedback
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D30CE19-32FD-41C6-AE1E-126407A50794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3FA6A-923C-4ABF-8AAF-E4C511BAF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="185">
   <si>
     <t>Class</t>
   </si>
@@ -566,6 +566,15 @@
   </si>
   <si>
     <t>sendToBack</t>
+  </si>
+  <si>
+    <t>TextRun</t>
+  </si>
+  <si>
+    <t>tableTextRuns</t>
+  </si>
+  <si>
+    <t>textRuns</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,10 +656,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F142" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F142" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F141">
-    <sortCondition ref="B1:B141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F144" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F144" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F142">
+    <sortCondition ref="B1:B142"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -960,11 +970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,17 +1029,16 @@
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>168</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1037,19 +1046,19 @@
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>170</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1057,17 +1066,16 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1075,19 +1083,19 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1095,19 +1103,19 @@
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1115,17 +1123,16 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1693,13 +1700,13 @@
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" t="s">
         <v>168</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2381,17 +2388,16 @@
       <c r="A78" t="s">
         <v>32</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" t="s">
         <v>180</v>
       </c>
-      <c r="C78" s="2"/>
       <c r="D78" t="s">
         <v>65</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" t="s">
         <v>168</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2399,17 +2405,16 @@
       <c r="A79" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2"/>
       <c r="D79" t="s">
         <v>65</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" t="s">
         <v>168</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3164,14 +3169,14 @@
       <c r="B122" t="s">
         <v>138</v>
       </c>
-      <c r="C122" t="s">
-        <v>157</v>
+      <c r="C122" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
-      <c r="F122" t="s">
-        <v>158</v>
+      <c r="F122" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3179,16 +3184,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>125</v>
-      </c>
-      <c r="D123" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C123" t="s">
+        <v>157</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,8 +3203,8 @@
       <c r="B124" t="s">
         <v>125</v>
       </c>
-      <c r="C124" t="s">
-        <v>127</v>
+      <c r="D124" t="s">
+        <v>68</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3213,16 +3218,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>131</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C125" t="s">
+        <v>127</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3232,8 +3237,8 @@
       <c r="B126" t="s">
         <v>131</v>
       </c>
-      <c r="C126" t="s">
-        <v>132</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3250,7 +3255,7 @@
         <v>131</v>
       </c>
       <c r="C127" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3267,7 +3272,7 @@
         <v>131</v>
       </c>
       <c r="C128" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3284,7 +3289,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3298,16 +3303,16 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>126</v>
-      </c>
-      <c r="D130" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C130" t="s">
+        <v>135</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3317,8 +3322,8 @@
       <c r="B131" t="s">
         <v>126</v>
       </c>
-      <c r="C131" t="s">
-        <v>128</v>
+      <c r="D131" t="s">
+        <v>68</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3332,16 +3337,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>98</v>
-      </c>
-      <c r="D132" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C132" t="s">
+        <v>128</v>
       </c>
       <c r="E132" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,7 +3354,7 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D133" t="s">
         <v>87</v>
@@ -3358,7 +3363,7 @@
         <v>14</v>
       </c>
       <c r="F133" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3368,17 +3373,14 @@
       <c r="B134" t="s">
         <v>13</v>
       </c>
-      <c r="C134" t="s">
-        <v>10</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
+      <c r="D134" t="s">
+        <v>87</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3389,7 +3391,7 @@
         <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -3398,7 +3400,7 @@
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3409,7 +3411,7 @@
         <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3418,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3426,16 +3428,19 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>97</v>
-      </c>
-      <c r="D137" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C137" t="s">
+        <v>18</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
       </c>
       <c r="E137" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3443,7 +3448,7 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D138" t="s">
         <v>87</v>
@@ -3452,7 +3457,7 @@
         <v>54</v>
       </c>
       <c r="F138" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3462,8 +3467,8 @@
       <c r="B139" t="s">
         <v>33</v>
       </c>
-      <c r="C139" t="s">
-        <v>57</v>
+      <c r="D139" t="s">
+        <v>87</v>
       </c>
       <c r="E139" t="s">
         <v>54</v>
@@ -3479,17 +3484,14 @@
       <c r="B140" t="s">
         <v>33</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
+      <c r="C140" t="s">
+        <v>57</v>
       </c>
       <c r="E140" t="s">
         <v>54</v>
       </c>
       <c r="F140" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,7 +3511,7 @@
         <v>54</v>
       </c>
       <c r="F141" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3517,15 +3519,53 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>54</v>
+      </c>
+      <c r="F142" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>32</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C143" s="3"/>
+      <c r="D143" t="s">
+        <v>68</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>32</v>
+      </c>
+      <c r="B144" t="s">
         <v>88</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D144" t="s">
         <v>65</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E144" t="s">
         <v>24</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F144" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Map for SlideGetImageOptions
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3FA6A-923C-4ABF-8AAF-E4C511BAF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F7306-F3AD-4EE9-B35D-77B3F5C763FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="186">
   <si>
     <t>Class</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>textRuns</t>
+  </si>
+  <si>
+    <t>SlideGetImageOptions</t>
   </si>
 </sst>
 </file>
@@ -617,11 +620,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,10 +658,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F144" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F144" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F142">
-    <sortCondition ref="B1:B142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F145" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F145" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F143">
+    <sortCondition ref="B1:B143"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -970,11 +972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,17 +2598,18 @@
       <c r="A89" t="s">
         <v>32</v>
       </c>
-      <c r="B89" t="s">
-        <v>75</v>
-      </c>
+      <c r="B89" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" s="2"/>
       <c r="D89" t="s">
-        <v>87</v>
-      </c>
-      <c r="E89" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2616,8 +2619,8 @@
       <c r="B90" t="s">
         <v>75</v>
       </c>
-      <c r="C90" t="s">
-        <v>74</v>
+      <c r="D90" t="s">
+        <v>87</v>
       </c>
       <c r="E90" t="s">
         <v>11</v>
@@ -2631,10 +2634,10 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
-      </c>
-      <c r="D91" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
       </c>
       <c r="E91" t="s">
         <v>11</v>
@@ -2650,11 +2653,8 @@
       <c r="B92" t="s">
         <v>72</v>
       </c>
-      <c r="C92" t="s">
-        <v>70</v>
-      </c>
-      <c r="D92">
-        <v>2</v>
+      <c r="D92" t="s">
+        <v>87</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -2668,10 +2668,13 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
-      </c>
-      <c r="D93" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
@@ -2687,8 +2690,8 @@
       <c r="B94" t="s">
         <v>73</v>
       </c>
-      <c r="C94" t="s">
-        <v>74</v>
+      <c r="D94" t="s">
+        <v>87</v>
       </c>
       <c r="E94" t="s">
         <v>11</v>
@@ -2702,10 +2705,10 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
-      </c>
-      <c r="D95" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C95" t="s">
+        <v>74</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2721,11 +2724,8 @@
       <c r="B96" t="s">
         <v>69</v>
       </c>
-      <c r="C96" t="s">
-        <v>70</v>
-      </c>
-      <c r="D96">
-        <v>2</v>
+      <c r="D96" t="s">
+        <v>87</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -2739,16 +2739,19 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>92</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C97" t="s">
+        <v>70</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2759,16 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D98" t="s">
         <v>87</v>
       </c>
       <c r="E98" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F98" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,11 +2778,8 @@
       <c r="B99" t="s">
         <v>162</v>
       </c>
-      <c r="C99" t="s">
-        <v>164</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
+      <c r="D99" t="s">
+        <v>87</v>
       </c>
       <c r="E99" t="s">
         <v>116</v>
@@ -2793,16 +2793,19 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>118</v>
-      </c>
-      <c r="D100" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C100" t="s">
+        <v>164</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
       </c>
       <c r="E100" t="s">
         <v>116</v>
       </c>
       <c r="F100" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2812,14 +2815,14 @@
       <c r="B101" t="s">
         <v>118</v>
       </c>
-      <c r="C101" t="s">
-        <v>124</v>
+      <c r="D101" t="s">
+        <v>68</v>
       </c>
       <c r="E101" t="s">
         <v>116</v>
       </c>
       <c r="F101" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,13 +2833,13 @@
         <v>118</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
       <c r="F102" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,13 +2850,13 @@
         <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E103" t="s">
         <v>116</v>
       </c>
       <c r="F103" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2864,13 +2867,13 @@
         <v>118</v>
       </c>
       <c r="C104" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E104" t="s">
         <v>116</v>
       </c>
       <c r="F104" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2881,13 +2884,13 @@
         <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2898,13 +2901,13 @@
         <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2915,13 +2918,13 @@
         <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2932,13 +2935,13 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,16 +2949,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
-      </c>
-      <c r="D109" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C109" t="s">
+        <v>51</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2965,8 +2968,8 @@
       <c r="B110" t="s">
         <v>165</v>
       </c>
-      <c r="C110" t="s">
-        <v>166</v>
+      <c r="D110" t="s">
+        <v>87</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
@@ -2980,16 +2983,16 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
-      </c>
-      <c r="D111" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C111" t="s">
+        <v>166</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2999,8 +3002,8 @@
       <c r="B112" t="s">
         <v>149</v>
       </c>
-      <c r="C112" t="s">
-        <v>151</v>
+      <c r="D112" t="s">
+        <v>68</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
@@ -3017,7 +3020,7 @@
         <v>149</v>
       </c>
       <c r="C113" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3034,7 +3037,7 @@
         <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
@@ -3051,7 +3054,7 @@
         <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3065,16 +3068,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>138</v>
-      </c>
-      <c r="D116" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C116" t="s">
+        <v>50</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,14 +3087,14 @@
       <c r="B117" t="s">
         <v>138</v>
       </c>
-      <c r="C117" t="s">
-        <v>148</v>
+      <c r="D117" t="s">
+        <v>68</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3102,13 +3105,13 @@
         <v>138</v>
       </c>
       <c r="C118" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3119,7 +3122,7 @@
         <v>138</v>
       </c>
       <c r="C119" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
@@ -3136,13 +3139,13 @@
         <v>138</v>
       </c>
       <c r="C120" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,13 +3156,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3169,14 +3172,14 @@
       <c r="B122" t="s">
         <v>138</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>184</v>
+      <c r="C122" t="s">
+        <v>154</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>183</v>
+      <c r="F122" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3187,13 +3190,13 @@
         <v>138</v>
       </c>
       <c r="C123" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3201,16 +3204,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>125</v>
-      </c>
-      <c r="D124" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C124" t="s">
+        <v>157</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3220,8 +3223,8 @@
       <c r="B125" t="s">
         <v>125</v>
       </c>
-      <c r="C125" t="s">
-        <v>127</v>
+      <c r="D125" t="s">
+        <v>68</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
@@ -3235,16 +3238,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>131</v>
-      </c>
-      <c r="D126" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C126" t="s">
+        <v>127</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,8 +3257,8 @@
       <c r="B127" t="s">
         <v>131</v>
       </c>
-      <c r="C127" t="s">
-        <v>132</v>
+      <c r="D127" t="s">
+        <v>68</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3272,7 +3275,7 @@
         <v>131</v>
       </c>
       <c r="C128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3289,7 +3292,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3306,7 +3309,7 @@
         <v>131</v>
       </c>
       <c r="C130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3320,16 +3323,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
-      </c>
-      <c r="D131" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C131" t="s">
+        <v>135</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3339,8 +3342,8 @@
       <c r="B132" t="s">
         <v>126</v>
       </c>
-      <c r="C132" t="s">
-        <v>128</v>
+      <c r="D132" t="s">
+        <v>68</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3354,16 +3357,16 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>98</v>
-      </c>
-      <c r="D133" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C133" t="s">
+        <v>128</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,7 +3374,7 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D134" t="s">
         <v>87</v>
@@ -3380,7 +3383,7 @@
         <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3390,17 +3393,14 @@
       <c r="B135" t="s">
         <v>13</v>
       </c>
-      <c r="C135" t="s">
-        <v>10</v>
-      </c>
-      <c r="D135">
-        <v>1</v>
+      <c r="D135" t="s">
+        <v>87</v>
       </c>
       <c r="E135" t="s">
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,7 +3411,7 @@
         <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3420,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3431,7 +3431,7 @@
         <v>13</v>
       </c>
       <c r="C137" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -3440,7 +3440,7 @@
         <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3448,16 +3448,19 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>97</v>
-      </c>
-      <c r="D138" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C138" t="s">
+        <v>18</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
       </c>
       <c r="E138" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F138" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3465,7 +3468,7 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D139" t="s">
         <v>87</v>
@@ -3474,7 +3477,7 @@
         <v>54</v>
       </c>
       <c r="F139" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3484,8 +3487,8 @@
       <c r="B140" t="s">
         <v>33</v>
       </c>
-      <c r="C140" t="s">
-        <v>57</v>
+      <c r="D140" t="s">
+        <v>87</v>
       </c>
       <c r="E140" t="s">
         <v>54</v>
@@ -3501,17 +3504,14 @@
       <c r="B141" t="s">
         <v>33</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D141">
-        <v>1</v>
+      <c r="C141" t="s">
+        <v>57</v>
       </c>
       <c r="E141" t="s">
         <v>54</v>
       </c>
       <c r="F141" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3531,25 +3531,27 @@
         <v>54</v>
       </c>
       <c r="F142" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>32</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C143" s="3"/>
-      <c r="D143" t="s">
-        <v>68</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>183</v>
+      <c r="B143" t="s">
+        <v>33</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
+        <v>54</v>
+      </c>
+      <c r="F143" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3557,15 +3559,33 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
+        <v>182</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="D144" t="s">
+        <v>68</v>
+      </c>
+      <c r="E144" t="s">
+        <v>116</v>
+      </c>
+      <c r="F144" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>32</v>
+      </c>
+      <c r="B145" t="s">
         <v>88</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D145" t="s">
         <v>65</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E145" t="s">
         <v>24</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F145" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] Map for SlideGetImageOptions (#995)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3FA6A-923C-4ABF-8AAF-E4C511BAF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F7306-F3AD-4EE9-B35D-77B3F5C763FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="186">
   <si>
     <t>Class</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>textRuns</t>
+  </si>
+  <si>
+    <t>SlideGetImageOptions</t>
   </si>
 </sst>
 </file>
@@ -617,11 +620,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,10 +658,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F144" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F144" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F142">
-    <sortCondition ref="B1:B142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F145" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F145" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F143">
+    <sortCondition ref="B1:B143"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -970,11 +972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,17 +2598,18 @@
       <c r="A89" t="s">
         <v>32</v>
       </c>
-      <c r="B89" t="s">
-        <v>75</v>
-      </c>
+      <c r="B89" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" s="2"/>
       <c r="D89" t="s">
-        <v>87</v>
-      </c>
-      <c r="E89" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2616,8 +2619,8 @@
       <c r="B90" t="s">
         <v>75</v>
       </c>
-      <c r="C90" t="s">
-        <v>74</v>
+      <c r="D90" t="s">
+        <v>87</v>
       </c>
       <c r="E90" t="s">
         <v>11</v>
@@ -2631,10 +2634,10 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
-      </c>
-      <c r="D91" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
       </c>
       <c r="E91" t="s">
         <v>11</v>
@@ -2650,11 +2653,8 @@
       <c r="B92" t="s">
         <v>72</v>
       </c>
-      <c r="C92" t="s">
-        <v>70</v>
-      </c>
-      <c r="D92">
-        <v>2</v>
+      <c r="D92" t="s">
+        <v>87</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -2668,10 +2668,13 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
-      </c>
-      <c r="D93" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
@@ -2687,8 +2690,8 @@
       <c r="B94" t="s">
         <v>73</v>
       </c>
-      <c r="C94" t="s">
-        <v>74</v>
+      <c r="D94" t="s">
+        <v>87</v>
       </c>
       <c r="E94" t="s">
         <v>11</v>
@@ -2702,10 +2705,10 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
-      </c>
-      <c r="D95" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C95" t="s">
+        <v>74</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2721,11 +2724,8 @@
       <c r="B96" t="s">
         <v>69</v>
       </c>
-      <c r="C96" t="s">
-        <v>70</v>
-      </c>
-      <c r="D96">
-        <v>2</v>
+      <c r="D96" t="s">
+        <v>87</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -2739,16 +2739,19 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>92</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C97" t="s">
+        <v>70</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2759,16 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D98" t="s">
         <v>87</v>
       </c>
       <c r="E98" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F98" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,11 +2778,8 @@
       <c r="B99" t="s">
         <v>162</v>
       </c>
-      <c r="C99" t="s">
-        <v>164</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
+      <c r="D99" t="s">
+        <v>87</v>
       </c>
       <c r="E99" t="s">
         <v>116</v>
@@ -2793,16 +2793,19 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>118</v>
-      </c>
-      <c r="D100" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C100" t="s">
+        <v>164</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
       </c>
       <c r="E100" t="s">
         <v>116</v>
       </c>
       <c r="F100" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2812,14 +2815,14 @@
       <c r="B101" t="s">
         <v>118</v>
       </c>
-      <c r="C101" t="s">
-        <v>124</v>
+      <c r="D101" t="s">
+        <v>68</v>
       </c>
       <c r="E101" t="s">
         <v>116</v>
       </c>
       <c r="F101" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,13 +2833,13 @@
         <v>118</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
       <c r="F102" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,13 +2850,13 @@
         <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E103" t="s">
         <v>116</v>
       </c>
       <c r="F103" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2864,13 +2867,13 @@
         <v>118</v>
       </c>
       <c r="C104" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E104" t="s">
         <v>116</v>
       </c>
       <c r="F104" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2881,13 +2884,13 @@
         <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2898,13 +2901,13 @@
         <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2915,13 +2918,13 @@
         <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2932,13 +2935,13 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,16 +2949,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
-      </c>
-      <c r="D109" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C109" t="s">
+        <v>51</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2965,8 +2968,8 @@
       <c r="B110" t="s">
         <v>165</v>
       </c>
-      <c r="C110" t="s">
-        <v>166</v>
+      <c r="D110" t="s">
+        <v>87</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
@@ -2980,16 +2983,16 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
-      </c>
-      <c r="D111" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C111" t="s">
+        <v>166</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2999,8 +3002,8 @@
       <c r="B112" t="s">
         <v>149</v>
       </c>
-      <c r="C112" t="s">
-        <v>151</v>
+      <c r="D112" t="s">
+        <v>68</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
@@ -3017,7 +3020,7 @@
         <v>149</v>
       </c>
       <c r="C113" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3034,7 +3037,7 @@
         <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
@@ -3051,7 +3054,7 @@
         <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3065,16 +3068,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>138</v>
-      </c>
-      <c r="D116" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C116" t="s">
+        <v>50</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,14 +3087,14 @@
       <c r="B117" t="s">
         <v>138</v>
       </c>
-      <c r="C117" t="s">
-        <v>148</v>
+      <c r="D117" t="s">
+        <v>68</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3102,13 +3105,13 @@
         <v>138</v>
       </c>
       <c r="C118" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3119,7 +3122,7 @@
         <v>138</v>
       </c>
       <c r="C119" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
@@ -3136,13 +3139,13 @@
         <v>138</v>
       </c>
       <c r="C120" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,13 +3156,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3169,14 +3172,14 @@
       <c r="B122" t="s">
         <v>138</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>184</v>
+      <c r="C122" t="s">
+        <v>154</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>183</v>
+      <c r="F122" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3187,13 +3190,13 @@
         <v>138</v>
       </c>
       <c r="C123" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3201,16 +3204,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>125</v>
-      </c>
-      <c r="D124" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C124" t="s">
+        <v>157</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3220,8 +3223,8 @@
       <c r="B125" t="s">
         <v>125</v>
       </c>
-      <c r="C125" t="s">
-        <v>127</v>
+      <c r="D125" t="s">
+        <v>68</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
@@ -3235,16 +3238,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>131</v>
-      </c>
-      <c r="D126" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C126" t="s">
+        <v>127</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,8 +3257,8 @@
       <c r="B127" t="s">
         <v>131</v>
       </c>
-      <c r="C127" t="s">
-        <v>132</v>
+      <c r="D127" t="s">
+        <v>68</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3272,7 +3275,7 @@
         <v>131</v>
       </c>
       <c r="C128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3289,7 +3292,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3306,7 +3309,7 @@
         <v>131</v>
       </c>
       <c r="C130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3320,16 +3323,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
-      </c>
-      <c r="D131" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C131" t="s">
+        <v>135</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3339,8 +3342,8 @@
       <c r="B132" t="s">
         <v>126</v>
       </c>
-      <c r="C132" t="s">
-        <v>128</v>
+      <c r="D132" t="s">
+        <v>68</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3354,16 +3357,16 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>98</v>
-      </c>
-      <c r="D133" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C133" t="s">
+        <v>128</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,7 +3374,7 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D134" t="s">
         <v>87</v>
@@ -3380,7 +3383,7 @@
         <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3390,17 +3393,14 @@
       <c r="B135" t="s">
         <v>13</v>
       </c>
-      <c r="C135" t="s">
-        <v>10</v>
-      </c>
-      <c r="D135">
-        <v>1</v>
+      <c r="D135" t="s">
+        <v>87</v>
       </c>
       <c r="E135" t="s">
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,7 +3411,7 @@
         <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -3420,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3431,7 +3431,7 @@
         <v>13</v>
       </c>
       <c r="C137" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -3440,7 +3440,7 @@
         <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3448,16 +3448,19 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>97</v>
-      </c>
-      <c r="D138" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C138" t="s">
+        <v>18</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
       </c>
       <c r="E138" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F138" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3465,7 +3468,7 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D139" t="s">
         <v>87</v>
@@ -3474,7 +3477,7 @@
         <v>54</v>
       </c>
       <c r="F139" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3484,8 +3487,8 @@
       <c r="B140" t="s">
         <v>33</v>
       </c>
-      <c r="C140" t="s">
-        <v>57</v>
+      <c r="D140" t="s">
+        <v>87</v>
       </c>
       <c r="E140" t="s">
         <v>54</v>
@@ -3501,17 +3504,14 @@
       <c r="B141" t="s">
         <v>33</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D141">
-        <v>1</v>
+      <c r="C141" t="s">
+        <v>57</v>
       </c>
       <c r="E141" t="s">
         <v>54</v>
       </c>
       <c r="F141" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3531,25 +3531,27 @@
         <v>54</v>
       </c>
       <c r="F142" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>32</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C143" s="3"/>
-      <c r="D143" t="s">
-        <v>68</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>183</v>
+      <c r="B143" t="s">
+        <v>33</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
+        <v>54</v>
+      </c>
+      <c r="F143" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3557,15 +3559,33 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
+        <v>182</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="D144" t="s">
+        <v>68</v>
+      </c>
+      <c r="E144" t="s">
+        <v>116</v>
+      </c>
+      <c r="F144" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>32</v>
+      </c>
+      <c r="B145" t="s">
         <v>88</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D145" t="s">
         <v>65</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E145" t="s">
         <v>24</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F145" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (ShapeLineStyle) Update snippet to include reference
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F7306-F3AD-4EE9-B35D-77B3F5C763FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A71E085-B9FE-42A2-B6E2-FD243FA27705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="187">
   <si>
     <t>Class</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>SlideGetImageOptions</t>
+  </si>
+  <si>
+    <t>ShapeLineStyle</t>
   </si>
 </sst>
 </file>
@@ -658,10 +661,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F145" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F145" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F143">
-    <sortCondition ref="B1:B143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F146" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F144">
+    <sortCondition ref="B1:B144"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -972,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,17 +2601,16 @@
       <c r="A89" t="s">
         <v>32</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" t="s">
         <v>185</v>
       </c>
-      <c r="C89" s="2"/>
       <c r="D89" t="s">
         <v>68</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" t="s">
         <v>105</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2687,17 +2689,18 @@
       <c r="A94" t="s">
         <v>32</v>
       </c>
-      <c r="B94" t="s">
-        <v>73</v>
-      </c>
+      <c r="B94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="2"/>
       <c r="D94" t="s">
-        <v>87</v>
-      </c>
-      <c r="E94" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,8 +2710,8 @@
       <c r="B95" t="s">
         <v>73</v>
       </c>
-      <c r="C95" t="s">
-        <v>74</v>
+      <c r="D95" t="s">
+        <v>87</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2722,10 +2725,10 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
-      </c>
-      <c r="D96" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C96" t="s">
+        <v>74</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -2741,11 +2744,8 @@
       <c r="B97" t="s">
         <v>69</v>
       </c>
-      <c r="C97" t="s">
-        <v>70</v>
-      </c>
-      <c r="D97">
-        <v>2</v>
+      <c r="D97" t="s">
+        <v>87</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2759,16 +2759,19 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
-      </c>
-      <c r="D98" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,16 +2779,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D99" t="s">
         <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F99" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2795,11 +2798,8 @@
       <c r="B100" t="s">
         <v>162</v>
       </c>
-      <c r="C100" t="s">
-        <v>164</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
+      <c r="D100" t="s">
+        <v>87</v>
       </c>
       <c r="E100" t="s">
         <v>116</v>
@@ -2813,16 +2813,19 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
-      </c>
-      <c r="D101" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
       </c>
       <c r="E101" t="s">
         <v>116</v>
       </c>
       <c r="F101" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,14 +2835,14 @@
       <c r="B102" t="s">
         <v>118</v>
       </c>
-      <c r="C102" t="s">
-        <v>124</v>
+      <c r="D102" t="s">
+        <v>68</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
       <c r="F102" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,13 +2853,13 @@
         <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E103" t="s">
         <v>116</v>
       </c>
       <c r="F103" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2867,13 +2870,13 @@
         <v>118</v>
       </c>
       <c r="C104" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E104" t="s">
         <v>116</v>
       </c>
       <c r="F104" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2884,13 +2887,13 @@
         <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2901,13 +2904,13 @@
         <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,13 +2921,13 @@
         <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2935,13 +2938,13 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2952,13 +2955,13 @@
         <v>118</v>
       </c>
       <c r="C109" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2966,16 +2969,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
-      </c>
-      <c r="D110" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C110" t="s">
+        <v>51</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2985,8 +2988,8 @@
       <c r="B111" t="s">
         <v>165</v>
       </c>
-      <c r="C111" t="s">
-        <v>166</v>
+      <c r="D111" t="s">
+        <v>87</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
@@ -3000,16 +3003,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>149</v>
-      </c>
-      <c r="D112" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C112" t="s">
+        <v>166</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3019,8 +3022,8 @@
       <c r="B113" t="s">
         <v>149</v>
       </c>
-      <c r="C113" t="s">
-        <v>151</v>
+      <c r="D113" t="s">
+        <v>68</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3037,7 +3040,7 @@
         <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
@@ -3054,7 +3057,7 @@
         <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3071,7 +3074,7 @@
         <v>149</v>
       </c>
       <c r="C116" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
@@ -3085,16 +3088,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
-      </c>
-      <c r="D117" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C117" t="s">
+        <v>50</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3104,14 +3107,14 @@
       <c r="B118" t="s">
         <v>138</v>
       </c>
-      <c r="C118" t="s">
-        <v>148</v>
+      <c r="D118" t="s">
+        <v>68</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3122,13 +3125,13 @@
         <v>138</v>
       </c>
       <c r="C119" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3139,7 +3142,7 @@
         <v>138</v>
       </c>
       <c r="C120" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
@@ -3156,13 +3159,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,13 +3176,13 @@
         <v>138</v>
       </c>
       <c r="C122" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3190,13 +3193,13 @@
         <v>138</v>
       </c>
       <c r="C123" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,13 +3210,13 @@
         <v>138</v>
       </c>
       <c r="C124" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3221,16 +3224,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C125" t="s">
+        <v>157</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,8 +3243,8 @@
       <c r="B126" t="s">
         <v>125</v>
       </c>
-      <c r="C126" t="s">
-        <v>127</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3255,16 +3258,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
-      </c>
-      <c r="D127" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C127" t="s">
+        <v>127</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,8 +3277,8 @@
       <c r="B128" t="s">
         <v>131</v>
       </c>
-      <c r="C128" t="s">
-        <v>132</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3292,7 +3295,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3309,7 +3312,7 @@
         <v>131</v>
       </c>
       <c r="C130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3326,7 +3329,7 @@
         <v>131</v>
       </c>
       <c r="C131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3340,16 +3343,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>126</v>
-      </c>
-      <c r="D132" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C132" t="s">
+        <v>135</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3359,8 +3362,8 @@
       <c r="B133" t="s">
         <v>126</v>
       </c>
-      <c r="C133" t="s">
-        <v>128</v>
+      <c r="D133" t="s">
+        <v>68</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
@@ -3374,16 +3377,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>98</v>
-      </c>
-      <c r="D134" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C134" t="s">
+        <v>128</v>
       </c>
       <c r="E134" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3391,7 +3394,7 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D135" t="s">
         <v>87</v>
@@ -3400,7 +3403,7 @@
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3410,17 +3413,14 @@
       <c r="B136" t="s">
         <v>13</v>
       </c>
-      <c r="C136" t="s">
-        <v>10</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
+      <c r="D136" t="s">
+        <v>87</v>
       </c>
       <c r="E136" t="s">
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3431,7 +3431,7 @@
         <v>13</v>
       </c>
       <c r="C137" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -3440,7 +3440,7 @@
         <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="C138" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>14</v>
       </c>
       <c r="F138" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3468,16 +3468,19 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>97</v>
-      </c>
-      <c r="D139" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C139" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F139" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3485,7 +3488,7 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D140" t="s">
         <v>87</v>
@@ -3494,7 +3497,7 @@
         <v>54</v>
       </c>
       <c r="F140" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3504,8 +3507,8 @@
       <c r="B141" t="s">
         <v>33</v>
       </c>
-      <c r="C141" t="s">
-        <v>57</v>
+      <c r="D141" t="s">
+        <v>87</v>
       </c>
       <c r="E141" t="s">
         <v>54</v>
@@ -3521,17 +3524,14 @@
       <c r="B142" t="s">
         <v>33</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
+      <c r="C142" t="s">
+        <v>57</v>
       </c>
       <c r="E142" t="s">
         <v>54</v>
       </c>
       <c r="F142" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3551,7 +3551,7 @@
         <v>54</v>
       </c>
       <c r="F143" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,17 +3559,19 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>182</v>
-      </c>
-      <c r="C144" s="1"/>
-      <c r="D144" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F144" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3577,15 +3579,33 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
+        <v>182</v>
+      </c>
+      <c r="C145" s="1"/>
+      <c r="D145" t="s">
+        <v>68</v>
+      </c>
+      <c r="E145" t="s">
+        <v>116</v>
+      </c>
+      <c r="F145" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146" t="s">
         <v>88</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D146" t="s">
         <v>65</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E146" t="s">
         <v>24</v>
       </c>
-      <c r="F145" t="s">
+      <c r="F146" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (ShapeLineStyle) Update snippet to include reference (#1030)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F7306-F3AD-4EE9-B35D-77B3F5C763FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A71E085-B9FE-42A2-B6E2-FD243FA27705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="187">
   <si>
     <t>Class</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>SlideGetImageOptions</t>
+  </si>
+  <si>
+    <t>ShapeLineStyle</t>
   </si>
 </sst>
 </file>
@@ -658,10 +661,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F145" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F145" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F143">
-    <sortCondition ref="B1:B143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F146" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F144">
+    <sortCondition ref="B1:B144"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -972,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,17 +2601,16 @@
       <c r="A89" t="s">
         <v>32</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" t="s">
         <v>185</v>
       </c>
-      <c r="C89" s="2"/>
       <c r="D89" t="s">
         <v>68</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" t="s">
         <v>105</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2687,17 +2689,18 @@
       <c r="A94" t="s">
         <v>32</v>
       </c>
-      <c r="B94" t="s">
-        <v>73</v>
-      </c>
+      <c r="B94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="2"/>
       <c r="D94" t="s">
-        <v>87</v>
-      </c>
-      <c r="E94" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,8 +2710,8 @@
       <c r="B95" t="s">
         <v>73</v>
       </c>
-      <c r="C95" t="s">
-        <v>74</v>
+      <c r="D95" t="s">
+        <v>87</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -2722,10 +2725,10 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
-      </c>
-      <c r="D96" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C96" t="s">
+        <v>74</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -2741,11 +2744,8 @@
       <c r="B97" t="s">
         <v>69</v>
       </c>
-      <c r="C97" t="s">
-        <v>70</v>
-      </c>
-      <c r="D97">
-        <v>2</v>
+      <c r="D97" t="s">
+        <v>87</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2759,16 +2759,19 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
-      </c>
-      <c r="D98" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C98" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,16 +2779,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D99" t="s">
         <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F99" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2795,11 +2798,8 @@
       <c r="B100" t="s">
         <v>162</v>
       </c>
-      <c r="C100" t="s">
-        <v>164</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
+      <c r="D100" t="s">
+        <v>87</v>
       </c>
       <c r="E100" t="s">
         <v>116</v>
@@ -2813,16 +2813,19 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
-      </c>
-      <c r="D101" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
       </c>
       <c r="E101" t="s">
         <v>116</v>
       </c>
       <c r="F101" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,14 +2835,14 @@
       <c r="B102" t="s">
         <v>118</v>
       </c>
-      <c r="C102" t="s">
-        <v>124</v>
+      <c r="D102" t="s">
+        <v>68</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
       <c r="F102" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,13 +2853,13 @@
         <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E103" t="s">
         <v>116</v>
       </c>
       <c r="F103" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2867,13 +2870,13 @@
         <v>118</v>
       </c>
       <c r="C104" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E104" t="s">
         <v>116</v>
       </c>
       <c r="F104" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2884,13 +2887,13 @@
         <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2901,13 +2904,13 @@
         <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,13 +2921,13 @@
         <v>118</v>
       </c>
       <c r="C107" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2935,13 +2938,13 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2952,13 +2955,13 @@
         <v>118</v>
       </c>
       <c r="C109" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2966,16 +2969,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
-      </c>
-      <c r="D110" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C110" t="s">
+        <v>51</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2985,8 +2988,8 @@
       <c r="B111" t="s">
         <v>165</v>
       </c>
-      <c r="C111" t="s">
-        <v>166</v>
+      <c r="D111" t="s">
+        <v>87</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
@@ -3000,16 +3003,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>149</v>
-      </c>
-      <c r="D112" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C112" t="s">
+        <v>166</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3019,8 +3022,8 @@
       <c r="B113" t="s">
         <v>149</v>
       </c>
-      <c r="C113" t="s">
-        <v>151</v>
+      <c r="D113" t="s">
+        <v>68</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3037,7 +3040,7 @@
         <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
@@ -3054,7 +3057,7 @@
         <v>149</v>
       </c>
       <c r="C115" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3071,7 +3074,7 @@
         <v>149</v>
       </c>
       <c r="C116" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
@@ -3085,16 +3088,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
-      </c>
-      <c r="D117" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C117" t="s">
+        <v>50</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3104,14 +3107,14 @@
       <c r="B118" t="s">
         <v>138</v>
       </c>
-      <c r="C118" t="s">
-        <v>148</v>
+      <c r="D118" t="s">
+        <v>68</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3122,13 +3125,13 @@
         <v>138</v>
       </c>
       <c r="C119" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3139,7 +3142,7 @@
         <v>138</v>
       </c>
       <c r="C120" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
@@ -3156,13 +3159,13 @@
         <v>138</v>
       </c>
       <c r="C121" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,13 +3176,13 @@
         <v>138</v>
       </c>
       <c r="C122" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3190,13 +3193,13 @@
         <v>138</v>
       </c>
       <c r="C123" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,13 +3210,13 @@
         <v>138</v>
       </c>
       <c r="C124" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3221,16 +3224,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C125" t="s">
+        <v>157</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,8 +3243,8 @@
       <c r="B126" t="s">
         <v>125</v>
       </c>
-      <c r="C126" t="s">
-        <v>127</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3255,16 +3258,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
-      </c>
-      <c r="D127" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C127" t="s">
+        <v>127</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,8 +3277,8 @@
       <c r="B128" t="s">
         <v>131</v>
       </c>
-      <c r="C128" t="s">
-        <v>132</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3292,7 +3295,7 @@
         <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3309,7 +3312,7 @@
         <v>131</v>
       </c>
       <c r="C130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3326,7 +3329,7 @@
         <v>131</v>
       </c>
       <c r="C131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3340,16 +3343,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>126</v>
-      </c>
-      <c r="D132" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C132" t="s">
+        <v>135</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3359,8 +3362,8 @@
       <c r="B133" t="s">
         <v>126</v>
       </c>
-      <c r="C133" t="s">
-        <v>128</v>
+      <c r="D133" t="s">
+        <v>68</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
@@ -3374,16 +3377,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>98</v>
-      </c>
-      <c r="D134" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C134" t="s">
+        <v>128</v>
       </c>
       <c r="E134" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3391,7 +3394,7 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D135" t="s">
         <v>87</v>
@@ -3400,7 +3403,7 @@
         <v>14</v>
       </c>
       <c r="F135" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3410,17 +3413,14 @@
       <c r="B136" t="s">
         <v>13</v>
       </c>
-      <c r="C136" t="s">
-        <v>10</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
+      <c r="D136" t="s">
+        <v>87</v>
       </c>
       <c r="E136" t="s">
         <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3431,7 +3431,7 @@
         <v>13</v>
       </c>
       <c r="C137" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -3440,7 +3440,7 @@
         <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="C138" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>14</v>
       </c>
       <c r="F138" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3468,16 +3468,19 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>97</v>
-      </c>
-      <c r="D139" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C139" t="s">
+        <v>18</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F139" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3485,7 +3488,7 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D140" t="s">
         <v>87</v>
@@ -3494,7 +3497,7 @@
         <v>54</v>
       </c>
       <c r="F140" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3504,8 +3507,8 @@
       <c r="B141" t="s">
         <v>33</v>
       </c>
-      <c r="C141" t="s">
-        <v>57</v>
+      <c r="D141" t="s">
+        <v>87</v>
       </c>
       <c r="E141" t="s">
         <v>54</v>
@@ -3521,17 +3524,14 @@
       <c r="B142" t="s">
         <v>33</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
+      <c r="C142" t="s">
+        <v>57</v>
       </c>
       <c r="E142" t="s">
         <v>54</v>
       </c>
       <c r="F142" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3551,7 +3551,7 @@
         <v>54</v>
       </c>
       <c r="F143" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,17 +3559,19 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>182</v>
-      </c>
-      <c r="C144" s="1"/>
-      <c r="D144" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F144" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3577,15 +3579,33 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
+        <v>182</v>
+      </c>
+      <c r="C145" s="1"/>
+      <c r="D145" t="s">
+        <v>68</v>
+      </c>
+      <c r="E145" t="s">
+        <v>116</v>
+      </c>
+      <c r="F145" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146" t="s">
         <v>88</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D146" t="s">
         <v>65</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E146" t="s">
         <v>24</v>
       </c>
-      <c r="F145" t="s">
+      <c r="F146" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (shapes) Updates to include 1.4 Shape enums
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A71E085-B9FE-42A2-B6E2-FD243FA27705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD923D5-11E5-4AAB-8C75-FC53CA01AF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="192">
   <si>
     <t>Class</t>
   </si>
@@ -581,6 +581,21 @@
   </si>
   <si>
     <t>ShapeLineStyle</t>
+  </si>
+  <si>
+    <t>ShapeAutoSize</t>
+  </si>
+  <si>
+    <t>ShapeFontUnderlineStyle</t>
+  </si>
+  <si>
+    <t>ShapeFillType</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>autoSizeSetting</t>
   </si>
 </sst>
 </file>
@@ -661,10 +676,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F146" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F144">
-    <sortCondition ref="B1:B144"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F152" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F152" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">
+    <sortCondition ref="B1:B150"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -975,11 +990,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1949,17 +1964,18 @@
       <c r="A54" t="s">
         <v>32</v>
       </c>
-      <c r="B54" t="s">
-        <v>21</v>
-      </c>
+      <c r="B54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" t="s">
-        <v>81</v>
+        <v>24</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1969,17 +1985,14 @@
       <c r="B55" t="s">
         <v>21</v>
       </c>
-      <c r="C55" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
+      <c r="D55" t="s">
+        <v>87</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,16 +2003,16 @@
         <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,16 +2023,16 @@
         <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2030,16 +2043,16 @@
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2050,16 +2063,16 @@
         <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F59" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2070,16 +2083,16 @@
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,16 +2103,16 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2110,16 +2123,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,10 +2140,13 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
       </c>
       <c r="E63" t="s">
         <v>85</v>
@@ -2146,17 +2162,14 @@
       <c r="B64" t="s">
         <v>59</v>
       </c>
-      <c r="C64" t="s">
-        <v>179</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+      <c r="D64" t="s">
+        <v>87</v>
       </c>
       <c r="E64" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,16 +2180,16 @@
         <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F65" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,13 +2200,16 @@
         <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
         <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,13 +2220,13 @@
         <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E67" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F67" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2218,16 +2234,16 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C68" t="s">
+        <v>82</v>
       </c>
       <c r="E68" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2235,33 +2251,34 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>32</v>
       </c>
-      <c r="B70" t="s">
-        <v>113</v>
-      </c>
+      <c r="B70" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" s="2"/>
       <c r="D70" t="s">
-        <v>87</v>
-      </c>
-      <c r="E70" t="s">
-        <v>109</v>
-      </c>
-      <c r="F70" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2269,19 +2286,16 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" t="s">
-        <v>114</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="D71" t="s">
+        <v>87</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="F71" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2289,16 +2303,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
-      </c>
-      <c r="D72" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C72" t="s">
+        <v>62</v>
       </c>
       <c r="E72" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F72" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2306,33 +2320,34 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" t="s">
-        <v>87</v>
-      </c>
-      <c r="E73" t="s">
-        <v>85</v>
-      </c>
-      <c r="F73" t="s">
-        <v>79</v>
+        <v>61</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>32</v>
       </c>
-      <c r="B74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" t="s">
-        <v>84</v>
-      </c>
-      <c r="E74" t="s">
-        <v>85</v>
-      </c>
-      <c r="F74" t="s">
-        <v>79</v>
+      <c r="B74" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" t="s">
+        <v>65</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2340,16 +2355,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="D75" t="s">
         <v>87</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,19 +2372,19 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F76" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2377,7 +2392,7 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D77" t="s">
         <v>65</v>
@@ -2394,16 +2409,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E78" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F78" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2411,16 +2426,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>180</v>
-      </c>
-      <c r="D79" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="C79" t="s">
+        <v>84</v>
       </c>
       <c r="E79" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2428,7 +2443,7 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="D80" t="s">
         <v>87</v>
@@ -2437,7 +2452,7 @@
         <v>53</v>
       </c>
       <c r="F80" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2445,19 +2460,19 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F81" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2465,19 +2480,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" t="s">
-        <v>104</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D82" t="s">
+        <v>65</v>
       </c>
       <c r="E82" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,19 +2497,16 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D83" t="s">
+        <v>65</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="F83" t="s">
-        <v>107</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2505,19 +2514,16 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D84" t="s">
+        <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F84" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2527,17 +2533,14 @@
       <c r="B85" t="s">
         <v>19</v>
       </c>
-      <c r="C85" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
+      <c r="D85" t="s">
+        <v>87</v>
       </c>
       <c r="E85" t="s">
         <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2545,16 +2548,19 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
-      </c>
-      <c r="D86" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,19 +2568,19 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F87" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,19 +2588,19 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="F88" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2602,16 +2608,19 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
-      </c>
-      <c r="D89" t="s">
-        <v>68</v>
+        <v>19</v>
+      </c>
+      <c r="C89" t="s">
+        <v>38</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F89" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2619,16 +2628,19 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
-      </c>
-      <c r="D90" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>38</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F90" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2636,16 +2648,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
-      </c>
-      <c r="C91" t="s">
-        <v>74</v>
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>87</v>
       </c>
       <c r="E91" t="s">
         <v>11</v>
       </c>
       <c r="F91" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2653,16 +2665,19 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
-      </c>
-      <c r="D92" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
       </c>
       <c r="F92" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,37 +2685,36 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F93" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>32</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C94" s="2"/>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
       <c r="D94" t="s">
-        <v>65</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="E94" t="s">
+        <v>105</v>
+      </c>
+      <c r="F94" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2708,7 +2722,7 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D95" t="s">
         <v>87</v>
@@ -2725,7 +2739,7 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
         <v>74</v>
@@ -2742,7 +2756,7 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D97" t="s">
         <v>87</v>
@@ -2759,7 +2773,7 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C98" t="s">
         <v>70</v>
@@ -2779,16 +2793,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E99" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F99" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,16 +2810,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="D100" t="s">
         <v>87</v>
       </c>
       <c r="E100" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F100" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,19 +2827,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="C101" t="s">
-        <v>164</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="E101" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2833,16 +2844,16 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="D102" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E102" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F102" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,16 +2861,19 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="C103" t="s">
-        <v>124</v>
+        <v>70</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F103" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2867,16 +2881,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
-      </c>
-      <c r="C104" t="s">
-        <v>52</v>
+        <v>92</v>
+      </c>
+      <c r="D104" t="s">
+        <v>87</v>
       </c>
       <c r="E104" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F104" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2884,16 +2898,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
-      </c>
-      <c r="C105" t="s">
-        <v>129</v>
+        <v>162</v>
+      </c>
+      <c r="D105" t="s">
+        <v>87</v>
       </c>
       <c r="E105" t="s">
         <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2901,16 +2915,19 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C106" t="s">
-        <v>123</v>
+        <v>164</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
       </c>
       <c r="E106" t="s">
         <v>116</v>
       </c>
       <c r="F106" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2920,14 +2937,14 @@
       <c r="B107" t="s">
         <v>118</v>
       </c>
-      <c r="C107" t="s">
-        <v>136</v>
+      <c r="D107" t="s">
+        <v>68</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2938,13 +2955,13 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2955,13 +2972,13 @@
         <v>118</v>
       </c>
       <c r="C109" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2972,13 +2989,13 @@
         <v>118</v>
       </c>
       <c r="C110" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2986,16 +3003,16 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
-      </c>
-      <c r="D111" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C111" t="s">
+        <v>123</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3003,16 +3020,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3020,10 +3037,10 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>149</v>
-      </c>
-      <c r="D113" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="C113" t="s">
+        <v>146</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3037,16 +3054,16 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3054,16 +3071,16 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3071,16 +3088,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>149</v>
-      </c>
-      <c r="C116" t="s">
-        <v>150</v>
+        <v>165</v>
+      </c>
+      <c r="D116" t="s">
+        <v>87</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3088,16 +3105,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C117" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,7 +3122,7 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="D118" t="s">
         <v>68</v>
@@ -3114,7 +3131,7 @@
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3122,10 +3139,10 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C119" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
@@ -3139,16 +3156,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C120" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3156,16 +3173,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C121" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,16 +3190,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3192,14 +3209,14 @@
       <c r="B123" t="s">
         <v>138</v>
       </c>
-      <c r="C123" t="s">
-        <v>154</v>
+      <c r="D123" t="s">
+        <v>68</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3210,13 +3227,13 @@
         <v>138</v>
       </c>
       <c r="C124" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3227,13 +3244,13 @@
         <v>138</v>
       </c>
       <c r="C125" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3241,16 +3258,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
-      </c>
-      <c r="D126" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C126" t="s">
+        <v>57</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3258,16 +3275,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C127" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3275,16 +3292,16 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
-      </c>
-      <c r="D128" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C128" t="s">
+        <v>154</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,16 +3309,16 @@
         <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C129" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3309,16 +3326,16 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3326,16 +3343,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
-      </c>
-      <c r="C131" t="s">
-        <v>134</v>
+        <v>125</v>
+      </c>
+      <c r="D131" t="s">
+        <v>68</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3343,16 +3360,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3360,7 +3377,7 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D133" t="s">
         <v>68</v>
@@ -3369,7 +3386,7 @@
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3377,16 +3394,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C134" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3394,16 +3411,16 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>98</v>
-      </c>
-      <c r="D135" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C135" t="s">
+        <v>133</v>
       </c>
       <c r="E135" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,16 +3428,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C136" t="s">
+        <v>134</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3428,19 +3445,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="C137" t="s">
-        <v>10</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="E137" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3448,19 +3462,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
-      </c>
-      <c r="C138" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
+        <v>126</v>
+      </c>
+      <c r="D138" t="s">
+        <v>68</v>
       </c>
       <c r="E138" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3468,19 +3479,16 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3488,16 +3496,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D140" t="s">
         <v>87</v>
       </c>
       <c r="E140" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F140" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3505,16 +3513,16 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D141" t="s">
         <v>87</v>
       </c>
       <c r="E141" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F141" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3522,16 +3530,19 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C142" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
       </c>
       <c r="E142" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F142" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3539,19 +3550,19 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>33</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C143" t="s">
+        <v>20</v>
       </c>
       <c r="D143">
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F143" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,19 +3570,19 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>33</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C144" t="s">
+        <v>18</v>
       </c>
       <c r="D144">
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F144" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3579,17 +3590,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>182</v>
-      </c>
-      <c r="C145" s="1"/>
+        <v>97</v>
+      </c>
       <c r="D145" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E145" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F145" t="s">
-        <v>183</v>
+        <v>63</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3597,15 +3607,124 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>88</v>
-      </c>
-      <c r="D146" t="s">
-        <v>65</v>
+        <v>97</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="E146" t="s">
         <v>24</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F146" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>32</v>
+      </c>
+      <c r="B147" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" t="s">
+        <v>87</v>
+      </c>
+      <c r="E147" t="s">
+        <v>54</v>
+      </c>
+      <c r="F147" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>32</v>
+      </c>
+      <c r="B148" t="s">
+        <v>33</v>
+      </c>
+      <c r="C148" t="s">
+        <v>57</v>
+      </c>
+      <c r="E148" t="s">
+        <v>54</v>
+      </c>
+      <c r="F148" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>32</v>
+      </c>
+      <c r="B149" t="s">
+        <v>33</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
+        <v>54</v>
+      </c>
+      <c r="F149" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>32</v>
+      </c>
+      <c r="B150" t="s">
+        <v>33</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150" t="s">
+        <v>54</v>
+      </c>
+      <c r="F150" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>32</v>
+      </c>
+      <c r="B151" t="s">
+        <v>182</v>
+      </c>
+      <c r="C151" s="1"/>
+      <c r="D151" t="s">
+        <v>68</v>
+      </c>
+      <c r="E151" t="s">
+        <v>116</v>
+      </c>
+      <c r="F151" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>32</v>
+      </c>
+      <c r="B152" t="s">
+        <v>88</v>
+      </c>
+      <c r="D152" t="s">
+        <v>65</v>
+      </c>
+      <c r="E152" t="s">
+        <v>24</v>
+      </c>
+      <c r="F152" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update TextRange snippet to include ParagraphFormat and BulletFormat references
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD923D5-11E5-4AAB-8C75-FC53CA01AF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F018D6-5A1B-49AB-9291-C4B5C81F4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -596,6 +596,18 @@
   </si>
   <si>
     <t>autoSizeSetting</t>
+  </si>
+  <si>
+    <t>ParagraphFormat</t>
+  </si>
+  <si>
+    <t>getSelectedTextRangeComplexProperties</t>
+  </si>
+  <si>
+    <t>BulletFormat</t>
+  </si>
+  <si>
+    <t>paragraphFormat</t>
   </si>
 </sst>
 </file>
@@ -638,10 +650,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +687,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F152" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F152" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F150">
-    <sortCondition ref="B1:B150"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F155" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F155" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
+    <sortCondition ref="B1:B151"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -990,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1229,16 +1240,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1246,16 +1257,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1265,8 +1276,8 @@
       <c r="B15" t="s">
         <v>139</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
+      <c r="D15" t="s">
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>116</v>
@@ -1280,10 +1291,10 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
       </c>
       <c r="E16" t="s">
         <v>116</v>
@@ -1299,8 +1310,8 @@
       <c r="B17" t="s">
         <v>140</v>
       </c>
-      <c r="C17" t="s">
-        <v>62</v>
+      <c r="D17" t="s">
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>116</v>
@@ -1317,7 +1328,7 @@
         <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>116</v>
@@ -1334,7 +1345,7 @@
         <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
         <v>116</v>
@@ -1351,7 +1362,7 @@
         <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20" t="s">
         <v>116</v>
@@ -1368,7 +1379,7 @@
         <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E21" t="s">
         <v>116</v>
@@ -1385,7 +1396,7 @@
         <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
         <v>116</v>
@@ -1399,16 +1410,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1416,16 +1427,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1433,7 +1444,7 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
         <v>87</v>
@@ -1450,16 +1461,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1467,10 +1478,10 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1484,16 +1495,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,16 +1512,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
         <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1518,19 +1529,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1540,17 +1548,14 @@
       <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
+      <c r="D31" t="s">
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1570,7 +1575,7 @@
         <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,16 +1586,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1601,16 +1606,16 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1621,16 +1626,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1641,16 +1646,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1661,16 +1666,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,16 +1686,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,16 +1706,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,13 +1726,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,16 +1743,19 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1752,19 +1763,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1774,17 +1782,14 @@
       <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
+      <c r="D43" t="s">
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1795,16 +1800,16 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,13 +1820,16 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>161</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,13 +1840,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1849,13 +1860,13 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E47" t="s">
         <v>53</v>
       </c>
       <c r="F47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1866,13 +1877,13 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,7 +1894,7 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
         <v>53</v>
@@ -1900,13 +1911,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1917,7 +1928,7 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" t="s">
         <v>53</v>
@@ -1934,13 +1945,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1948,34 +1959,33 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" t="s">
-        <v>65</v>
+      <c r="B54" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" t="s">
+        <v>178</v>
       </c>
       <c r="E54" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>89</v>
+        <v>168</v>
+      </c>
+      <c r="F54" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,16 +1993,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2000,19 +2010,16 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" t="s">
-        <v>25</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D56" t="s">
+        <v>65</v>
       </c>
       <c r="E56" t="s">
         <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2022,17 +2029,14 @@
       <c r="B57" t="s">
         <v>21</v>
       </c>
-      <c r="C57" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
+      <c r="D57" t="s">
+        <v>87</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2043,7 +2047,7 @@
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2052,7 +2056,7 @@
         <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2063,16 +2067,16 @@
         <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F59" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2083,7 +2087,7 @@
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2092,7 +2096,7 @@
         <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2103,7 +2107,7 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2112,7 +2116,7 @@
         <v>116</v>
       </c>
       <c r="F61" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2123,16 +2127,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2143,16 +2147,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F63" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2160,16 +2164,19 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
-      </c>
-      <c r="D64" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F64" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2177,19 +2184,19 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F65" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2199,17 +2206,14 @@
       <c r="B66" t="s">
         <v>59</v>
       </c>
-      <c r="C66" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
+      <c r="D66" t="s">
+        <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F66" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2220,13 +2224,16 @@
         <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>179</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F67" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,13 +2244,16 @@
         <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>60</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,32 +2263,31 @@
       <c r="B69" t="s">
         <v>59</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>86</v>
+      <c r="C69" t="s">
+        <v>93</v>
       </c>
       <c r="E69" t="s">
         <v>53</v>
       </c>
       <c r="F69" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>32</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" t="s">
-        <v>65</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>44</v>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2286,16 +2295,16 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>61</v>
-      </c>
-      <c r="D71" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C71" t="s">
+        <v>86</v>
       </c>
       <c r="E71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2303,16 +2312,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C72" t="s">
-        <v>62</v>
+        <v>189</v>
+      </c>
+      <c r="D72" t="s">
+        <v>65</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2322,32 +2331,31 @@
       <c r="B73" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>89</v>
+      <c r="D73" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F73" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>32</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" t="s">
-        <v>65</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>89</v>
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" t="s">
+        <v>54</v>
+      </c>
+      <c r="F74" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2355,16 +2363,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>113</v>
-      </c>
-      <c r="D75" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C75" t="s">
+        <v>190</v>
       </c>
       <c r="E75" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F75" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2372,19 +2380,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>113</v>
-      </c>
-      <c r="C76" t="s">
-        <v>114</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
+        <v>188</v>
+      </c>
+      <c r="D76" t="s">
+        <v>65</v>
       </c>
       <c r="E76" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F76" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2392,16 +2397,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D77" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E77" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F77" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2409,16 +2414,19 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
-      </c>
-      <c r="D78" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="C78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F78" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2426,10 +2434,10 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
       </c>
       <c r="E79" t="s">
         <v>85</v>
@@ -2443,16 +2451,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D80" t="s">
         <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2460,19 +2468,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E81" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2480,16 +2485,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D82" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E82" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F82" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2497,16 +2502,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
-      </c>
-      <c r="D83" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C83" t="s">
+        <v>91</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F83" t="s">
-        <v>181</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2514,16 +2522,16 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D84" t="s">
         <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F84" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,16 +2539,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D85" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E85" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F85" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2548,19 +2556,16 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D86" t="s">
+        <v>65</v>
       </c>
       <c r="E86" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F86" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2570,17 +2575,14 @@
       <c r="B87" t="s">
         <v>19</v>
       </c>
-      <c r="C87" t="s">
-        <v>104</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
+      <c r="D87" t="s">
+        <v>87</v>
       </c>
       <c r="E87" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,16 +2593,16 @@
         <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F88" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2611,16 +2613,16 @@
         <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F89" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,16 +2633,16 @@
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F90" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,16 +2650,19 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2665,19 +2670,19 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2687,17 +2692,14 @@
       <c r="B93" t="s">
         <v>9</v>
       </c>
-      <c r="C93" t="s">
-        <v>16</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
+      <c r="D93" t="s">
+        <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F93" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2705,16 +2707,19 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
-      </c>
-      <c r="D94" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F94" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2722,16 +2727,19 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>75</v>
-      </c>
-      <c r="D95" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F95" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2739,16 +2747,16 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D96" t="s">
+        <v>68</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F96" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,7 +2764,7 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D97" t="s">
         <v>87</v>
@@ -2773,13 +2781,10 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
-      </c>
-      <c r="D98">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -2793,16 +2798,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="D99" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2810,10 +2815,13 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
-      </c>
-      <c r="D100" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C100" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -2827,16 +2835,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>73</v>
-      </c>
-      <c r="C101" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="D101" t="s">
+        <v>65</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F101" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2844,7 +2852,7 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D102" t="s">
         <v>87</v>
@@ -2861,13 +2869,10 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2881,16 +2886,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D104" t="s">
         <v>87</v>
       </c>
       <c r="E104" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F104" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2898,16 +2903,19 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>162</v>
-      </c>
-      <c r="D105" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C105" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F105" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2915,19 +2923,16 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>162</v>
-      </c>
-      <c r="C106" t="s">
-        <v>164</v>
-      </c>
-      <c r="D106">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D106" t="s">
+        <v>87</v>
       </c>
       <c r="E106" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F106" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2935,16 +2940,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="D107" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2952,16 +2957,19 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C108" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2971,8 +2979,8 @@
       <c r="B109" t="s">
         <v>118</v>
       </c>
-      <c r="C109" t="s">
-        <v>52</v>
+      <c r="D109" t="s">
+        <v>68</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
@@ -2989,13 +2997,13 @@
         <v>118</v>
       </c>
       <c r="C110" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3006,13 +3014,13 @@
         <v>118</v>
       </c>
       <c r="C111" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3023,13 +3031,13 @@
         <v>118</v>
       </c>
       <c r="C112" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3040,13 +3048,13 @@
         <v>118</v>
       </c>
       <c r="C113" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3057,13 +3065,13 @@
         <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3074,13 +3082,13 @@
         <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3088,16 +3096,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
-      </c>
-      <c r="D116" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C116" t="s">
+        <v>120</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3113,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3122,16 +3130,16 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D118" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3139,16 +3147,16 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C119" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3158,8 +3166,8 @@
       <c r="B120" t="s">
         <v>149</v>
       </c>
-      <c r="C120" t="s">
-        <v>49</v>
+      <c r="D120" t="s">
+        <v>68</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
@@ -3176,7 +3184,7 @@
         <v>149</v>
       </c>
       <c r="C121" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
@@ -3193,7 +3201,7 @@
         <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
@@ -3207,16 +3215,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>138</v>
-      </c>
-      <c r="D123" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C123" t="s">
+        <v>150</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3224,10 +3232,10 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C124" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3243,8 +3251,8 @@
       <c r="B125" t="s">
         <v>138</v>
       </c>
-      <c r="C125" t="s">
-        <v>58</v>
+      <c r="D125" t="s">
+        <v>68</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
@@ -3261,13 +3269,13 @@
         <v>138</v>
       </c>
       <c r="C126" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,13 +3286,13 @@
         <v>138</v>
       </c>
       <c r="C127" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3295,13 +3303,13 @@
         <v>138</v>
       </c>
       <c r="C128" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3312,13 +3320,13 @@
         <v>138</v>
       </c>
       <c r="C129" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3329,13 +3337,13 @@
         <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3343,16 +3351,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>125</v>
-      </c>
-      <c r="D131" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C131" t="s">
+        <v>184</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3360,16 +3368,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3377,7 +3385,7 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D133" t="s">
         <v>68</v>
@@ -3386,7 +3394,7 @@
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3394,16 +3402,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C134" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3413,8 +3421,8 @@
       <c r="B135" t="s">
         <v>131</v>
       </c>
-      <c r="C135" t="s">
-        <v>133</v>
+      <c r="D135" t="s">
+        <v>68</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
@@ -3431,7 +3439,7 @@
         <v>131</v>
       </c>
       <c r="C136" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
@@ -3448,7 +3456,7 @@
         <v>131</v>
       </c>
       <c r="C137" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
@@ -3462,16 +3470,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>126</v>
-      </c>
-      <c r="D138" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C138" t="s">
+        <v>134</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3479,16 +3487,16 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C139" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3496,16 +3504,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D140" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E140" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3513,16 +3521,16 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>13</v>
-      </c>
-      <c r="D141" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C141" t="s">
+        <v>128</v>
       </c>
       <c r="E141" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3530,19 +3538,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>13</v>
-      </c>
-      <c r="C142" t="s">
-        <v>10</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D142" t="s">
+        <v>87</v>
       </c>
       <c r="E142" t="s">
         <v>14</v>
       </c>
       <c r="F142" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3552,17 +3557,14 @@
       <c r="B143" t="s">
         <v>13</v>
       </c>
-      <c r="C143" t="s">
-        <v>20</v>
-      </c>
-      <c r="D143">
-        <v>1</v>
+      <c r="D143" t="s">
+        <v>87</v>
       </c>
       <c r="E143" t="s">
         <v>14</v>
       </c>
       <c r="F143" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3573,7 +3575,7 @@
         <v>13</v>
       </c>
       <c r="C144" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -3582,7 +3584,7 @@
         <v>14</v>
       </c>
       <c r="F144" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3590,16 +3592,19 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>97</v>
-      </c>
-      <c r="D145" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C145" t="s">
+        <v>20</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
       </c>
       <c r="E145" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3607,16 +3612,19 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>97</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>191</v>
+        <v>13</v>
+      </c>
+      <c r="C146" t="s">
+        <v>18</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
       </c>
       <c r="E146" t="s">
-        <v>24</v>
-      </c>
-      <c r="F146" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
+      </c>
+      <c r="F146" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3624,7 +3632,7 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D147" t="s">
         <v>87</v>
@@ -3633,7 +3641,7 @@
         <v>54</v>
       </c>
       <c r="F147" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3641,16 +3649,16 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="C148" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="E148" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F148" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3660,17 +3668,14 @@
       <c r="B149" t="s">
         <v>33</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
+      <c r="D149" t="s">
+        <v>87</v>
       </c>
       <c r="E149" t="s">
         <v>54</v>
       </c>
       <c r="F149" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3690,7 +3695,7 @@
         <v>54</v>
       </c>
       <c r="F150" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3698,17 +3703,19 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>182</v>
-      </c>
-      <c r="C151" s="1"/>
-      <c r="D151" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F151" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3716,15 +3723,67 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
+        <v>33</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E152" t="s">
+        <v>54</v>
+      </c>
+      <c r="F152" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>32</v>
+      </c>
+      <c r="B153" t="s">
+        <v>33</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E153" t="s">
+        <v>54</v>
+      </c>
+      <c r="F153" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>32</v>
+      </c>
+      <c r="B154" t="s">
+        <v>182</v>
+      </c>
+      <c r="C154" s="1"/>
+      <c r="D154" t="s">
+        <v>68</v>
+      </c>
+      <c r="E154" t="s">
+        <v>116</v>
+      </c>
+      <c r="F154" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>32</v>
+      </c>
+      <c r="B155" t="s">
         <v>88</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D155" t="s">
         <v>65</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E155" t="s">
         <v>24</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F155" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (shapes) Updates to include 1.4 Shape enums (#1033)
* [PowerPoint] (shapes) Updates to include 1.4 Shape enums

* Refine text ranges HTML

* Update TextRange snippet to include ParagraphFormat and BulletFormat references
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A71E085-B9FE-42A2-B6E2-FD243FA27705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F018D6-5A1B-49AB-9291-C4B5C81F4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="196">
   <si>
     <t>Class</t>
   </si>
@@ -581,6 +581,33 @@
   </si>
   <si>
     <t>ShapeLineStyle</t>
+  </si>
+  <si>
+    <t>ShapeAutoSize</t>
+  </si>
+  <si>
+    <t>ShapeFontUnderlineStyle</t>
+  </si>
+  <si>
+    <t>ShapeFillType</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>autoSizeSetting</t>
+  </si>
+  <si>
+    <t>ParagraphFormat</t>
+  </si>
+  <si>
+    <t>getSelectedTextRangeComplexProperties</t>
+  </si>
+  <si>
+    <t>BulletFormat</t>
+  </si>
+  <si>
+    <t>paragraphFormat</t>
   </si>
 </sst>
 </file>
@@ -623,10 +650,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +687,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F146" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F146" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F144">
-    <sortCondition ref="B1:B144"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F155" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F155" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
+    <sortCondition ref="B1:B151"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -975,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,16 +1240,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1231,16 +1257,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1250,8 +1276,8 @@
       <c r="B15" t="s">
         <v>139</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
+      <c r="D15" t="s">
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>116</v>
@@ -1265,10 +1291,10 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
       </c>
       <c r="E16" t="s">
         <v>116</v>
@@ -1284,8 +1310,8 @@
       <c r="B17" t="s">
         <v>140</v>
       </c>
-      <c r="C17" t="s">
-        <v>62</v>
+      <c r="D17" t="s">
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>116</v>
@@ -1302,7 +1328,7 @@
         <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>116</v>
@@ -1319,7 +1345,7 @@
         <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
         <v>116</v>
@@ -1336,7 +1362,7 @@
         <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20" t="s">
         <v>116</v>
@@ -1353,7 +1379,7 @@
         <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E21" t="s">
         <v>116</v>
@@ -1370,7 +1396,7 @@
         <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
         <v>116</v>
@@ -1384,16 +1410,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1401,16 +1427,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1418,7 +1444,7 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
         <v>87</v>
@@ -1435,16 +1461,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1452,10 +1478,10 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1469,16 +1495,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1486,16 +1512,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
         <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1503,19 +1529,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1525,17 +1548,14 @@
       <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
+      <c r="D31" t="s">
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1555,7 +1575,7 @@
         <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1566,16 +1586,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1586,16 +1606,16 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1606,16 +1626,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1626,16 +1646,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1646,16 +1666,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1666,16 +1686,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1686,16 +1706,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,13 +1726,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1720,16 +1743,19 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1737,19 +1763,16 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1759,17 +1782,14 @@
       <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
+      <c r="D43" t="s">
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1780,16 +1800,16 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,13 +1820,16 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>161</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,13 +1840,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1834,13 +1860,13 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E47" t="s">
         <v>53</v>
       </c>
       <c r="F47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1851,13 +1877,13 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1868,7 +1894,7 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
         <v>53</v>
@@ -1885,13 +1911,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,7 +1928,7 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" t="s">
         <v>53</v>
@@ -1919,13 +1945,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,16 +1959,16 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1950,16 +1976,16 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C54" t="s">
+        <v>178</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1967,13 +1993,10 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D55" t="s">
+        <v>68</v>
       </c>
       <c r="E55" t="s">
         <v>24</v>
@@ -1987,19 +2010,16 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D56" t="s">
+        <v>65</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2009,17 +2029,14 @@
       <c r="B57" t="s">
         <v>21</v>
       </c>
-      <c r="C57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
+      <c r="D57" t="s">
+        <v>87</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2030,16 +2047,16 @@
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2050,16 +2067,16 @@
         <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F59" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2070,16 +2087,16 @@
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,16 +2107,16 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2110,16 +2127,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,16 +2144,19 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F63" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2144,19 +2164,19 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>168</v>
+        <v>14</v>
       </c>
       <c r="F64" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2164,19 +2184,19 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F65" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2186,14 +2206,14 @@
       <c r="B66" t="s">
         <v>59</v>
       </c>
-      <c r="C66" t="s">
-        <v>93</v>
+      <c r="D66" t="s">
+        <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F66" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,13 +2224,16 @@
         <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>179</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F67" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2218,16 +2241,19 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2235,16 +2261,16 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2252,16 +2278,16 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
-      </c>
-      <c r="D70" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
       </c>
       <c r="E70" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F70" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2269,19 +2295,16 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>114</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2289,16 +2312,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="D72" t="s">
         <v>65</v>
       </c>
       <c r="E72" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2306,16 +2329,16 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
         <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F73" t="s">
-        <v>79</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2323,16 +2346,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E74" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F74" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2340,16 +2363,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
-      </c>
-      <c r="D75" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C75" t="s">
+        <v>190</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,19 +2380,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>90</v>
-      </c>
-      <c r="C76" t="s">
-        <v>91</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
+        <v>188</v>
+      </c>
+      <c r="D76" t="s">
+        <v>65</v>
       </c>
       <c r="E76" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F76" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2377,16 +2397,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="D77" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E77" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F77" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2394,16 +2414,19 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>180</v>
-      </c>
-      <c r="D78" t="s">
-        <v>65</v>
+        <v>113</v>
+      </c>
+      <c r="C78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="F78" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2411,16 +2434,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="D79" t="s">
         <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2428,16 +2451,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="D80" t="s">
         <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2445,19 +2468,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E81" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2465,19 +2485,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" t="s">
-        <v>104</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D82" t="s">
+        <v>87</v>
       </c>
       <c r="E82" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F82" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,19 +2502,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F83" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2505,19 +2522,16 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="D84" t="s">
+        <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F84" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2525,19 +2539,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D85" t="s">
+        <v>65</v>
       </c>
       <c r="E85" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F85" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2545,16 +2556,16 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="D86" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2562,19 +2573,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D87" t="s">
+        <v>87</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,10 +2590,10 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -2594,7 +2602,7 @@
         <v>40</v>
       </c>
       <c r="F88" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2602,10 +2610,13 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
-      </c>
-      <c r="D89" t="s">
-        <v>68</v>
+        <v>19</v>
+      </c>
+      <c r="C89" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
       </c>
       <c r="E89" t="s">
         <v>105</v>
@@ -2619,16 +2630,19 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
-      </c>
-      <c r="D90" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>106</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F90" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2636,16 +2650,19 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>74</v>
+        <v>38</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2653,16 +2670,19 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>72</v>
-      </c>
-      <c r="D92" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C92" t="s">
+        <v>38</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2670,37 +2690,36 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
-      </c>
-      <c r="C93" t="s">
-        <v>70</v>
-      </c>
-      <c r="D93">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>87</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
       </c>
       <c r="F93" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>32</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="D94" t="s">
-        <v>65</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>79</v>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2708,16 +2727,19 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
-      </c>
-      <c r="D95" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F95" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2725,16 +2747,16 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>73</v>
-      </c>
-      <c r="C96" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D96" t="s">
+        <v>68</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F96" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2742,7 +2764,7 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D97" t="s">
         <v>87</v>
@@ -2759,13 +2781,10 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C98" t="s">
-        <v>70</v>
-      </c>
-      <c r="D98">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -2779,16 +2798,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D99" t="s">
         <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,16 +2815,19 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>162</v>
-      </c>
-      <c r="D100" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C100" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F100" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,19 +2835,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>162</v>
-      </c>
-      <c r="C101" t="s">
-        <v>164</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
+        <v>186</v>
+      </c>
+      <c r="D101" t="s">
+        <v>65</v>
       </c>
       <c r="E101" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F101" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2833,16 +2852,16 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="D102" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E102" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F102" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,16 +2869,16 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="C103" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="E103" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F103" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2867,16 +2886,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
-      </c>
-      <c r="C104" t="s">
-        <v>52</v>
+        <v>69</v>
+      </c>
+      <c r="D104" t="s">
+        <v>87</v>
       </c>
       <c r="E104" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F104" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2884,16 +2903,19 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="C105" t="s">
-        <v>129</v>
+        <v>70</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F105" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2901,16 +2923,16 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
-      </c>
-      <c r="C106" t="s">
-        <v>123</v>
+        <v>92</v>
+      </c>
+      <c r="D106" t="s">
+        <v>87</v>
       </c>
       <c r="E106" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F106" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,16 +2940,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
-      </c>
-      <c r="C107" t="s">
-        <v>136</v>
+        <v>162</v>
+      </c>
+      <c r="D107" t="s">
+        <v>87</v>
       </c>
       <c r="E107" t="s">
         <v>116</v>
       </c>
       <c r="F107" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2935,16 +2957,19 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C108" t="s">
-        <v>146</v>
+        <v>164</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
       </c>
       <c r="E108" t="s">
         <v>116</v>
       </c>
       <c r="F108" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2954,14 +2979,14 @@
       <c r="B109" t="s">
         <v>118</v>
       </c>
-      <c r="C109" t="s">
-        <v>120</v>
+      <c r="D109" t="s">
+        <v>68</v>
       </c>
       <c r="E109" t="s">
         <v>116</v>
       </c>
       <c r="F109" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2972,13 +2997,13 @@
         <v>118</v>
       </c>
       <c r="C110" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2986,16 +3011,16 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
-      </c>
-      <c r="D111" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C111" t="s">
+        <v>52</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3003,16 +3028,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3020,16 +3045,16 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>149</v>
-      </c>
-      <c r="D113" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="C113" t="s">
+        <v>123</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3037,16 +3062,16 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3054,10 +3079,10 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3071,16 +3096,16 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3088,16 +3113,16 @@
         <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,16 +3130,16 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="D118" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3122,16 +3147,16 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="C119" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3139,16 +3164,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>138</v>
-      </c>
-      <c r="C120" t="s">
-        <v>58</v>
+        <v>149</v>
+      </c>
+      <c r="D120" t="s">
+        <v>68</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3156,16 +3181,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C121" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,16 +3198,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>156</v>
+        <v>49</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3190,16 +3215,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C123" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,16 +3232,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C124" t="s">
-        <v>184</v>
+        <v>50</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3226,14 +3251,14 @@
       <c r="B125" t="s">
         <v>138</v>
       </c>
-      <c r="C125" t="s">
-        <v>157</v>
+      <c r="D125" t="s">
+        <v>68</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3241,16 +3266,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
-      </c>
-      <c r="D126" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C126" t="s">
+        <v>148</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3258,16 +3283,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C127" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3275,16 +3300,16 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
-      </c>
-      <c r="D128" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C128" t="s">
+        <v>57</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,16 +3317,16 @@
         <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C129" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3309,16 +3334,16 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3326,16 +3351,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3343,16 +3368,16 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3360,7 +3385,7 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D133" t="s">
         <v>68</v>
@@ -3377,10 +3402,10 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C134" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
@@ -3394,16 +3419,16 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D135" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E135" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,16 +3436,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C136" t="s">
+        <v>132</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3428,19 +3453,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="C137" t="s">
-        <v>10</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
+        <v>133</v>
       </c>
       <c r="E137" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3448,19 +3470,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="C138" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
+        <v>134</v>
       </c>
       <c r="E138" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3468,19 +3487,16 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3488,16 +3504,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="D140" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E140" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3505,16 +3521,16 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>33</v>
-      </c>
-      <c r="D141" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C141" t="s">
+        <v>128</v>
       </c>
       <c r="E141" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3522,16 +3538,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>33</v>
-      </c>
-      <c r="C142" t="s">
-        <v>57</v>
+        <v>98</v>
+      </c>
+      <c r="D142" t="s">
+        <v>87</v>
       </c>
       <c r="E142" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F142" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3539,19 +3555,16 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>33</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D143">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D143" t="s">
+        <v>87</v>
       </c>
       <c r="E143" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F143" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,19 +3572,19 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>33</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
       </c>
       <c r="D144">
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F144" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3579,17 +3592,19 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>182</v>
-      </c>
-      <c r="C145" s="1"/>
-      <c r="D145" t="s">
-        <v>68</v>
+        <v>13</v>
+      </c>
+      <c r="C145" t="s">
+        <v>20</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
       </c>
       <c r="E145" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>183</v>
+        <v>23</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3597,15 +3612,178 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146" t="s">
+        <v>18</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>32</v>
+      </c>
+      <c r="B147" t="s">
+        <v>97</v>
+      </c>
+      <c r="D147" t="s">
+        <v>87</v>
+      </c>
+      <c r="E147" t="s">
+        <v>54</v>
+      </c>
+      <c r="F147" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>32</v>
+      </c>
+      <c r="B148" t="s">
+        <v>97</v>
+      </c>
+      <c r="C148" t="s">
+        <v>191</v>
+      </c>
+      <c r="E148" t="s">
+        <v>24</v>
+      </c>
+      <c r="F148" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>32</v>
+      </c>
+      <c r="B149" t="s">
+        <v>33</v>
+      </c>
+      <c r="D149" t="s">
+        <v>87</v>
+      </c>
+      <c r="E149" t="s">
+        <v>54</v>
+      </c>
+      <c r="F149" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>32</v>
+      </c>
+      <c r="B150" t="s">
+        <v>33</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150" t="s">
+        <v>54</v>
+      </c>
+      <c r="F150" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>32</v>
+      </c>
+      <c r="B151" t="s">
+        <v>33</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151" t="s">
+        <v>54</v>
+      </c>
+      <c r="F151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>32</v>
+      </c>
+      <c r="B152" t="s">
+        <v>33</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E152" t="s">
+        <v>54</v>
+      </c>
+      <c r="F152" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>32</v>
+      </c>
+      <c r="B153" t="s">
+        <v>33</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E153" t="s">
+        <v>54</v>
+      </c>
+      <c r="F153" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>32</v>
+      </c>
+      <c r="B154" t="s">
+        <v>182</v>
+      </c>
+      <c r="C154" s="1"/>
+      <c r="D154" t="s">
+        <v>68</v>
+      </c>
+      <c r="E154" t="s">
+        <v>116</v>
+      </c>
+      <c r="F154" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>32</v>
+      </c>
+      <c r="B155" t="s">
         <v>88</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D155" t="s">
         <v>65</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E155" t="s">
         <v>24</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F155" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (Shape) Add placeholder snippet
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F018D6-5A1B-49AB-9291-C4B5C81F4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D902EC-FD39-449E-B854-98898D62E7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="200">
   <si>
     <t>Class</t>
   </si>
@@ -608,6 +608,18 @@
   </si>
   <si>
     <t>paragraphFormat</t>
+  </si>
+  <si>
+    <t>placeholderFormat</t>
+  </si>
+  <si>
+    <t>getPlaceholderShapes</t>
+  </si>
+  <si>
+    <t>PlaceholderFormat</t>
+  </si>
+  <si>
+    <t>PlaceholderType</t>
   </si>
 </sst>
 </file>
@@ -650,9 +662,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +700,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F155" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F155" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
-    <sortCondition ref="B1:B151"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F158" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
+    <sortCondition ref="B1:B154"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1001,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1545,37 +1558,36 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
+      <c r="B31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>87</v>
       </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" t="s">
-        <v>7</v>
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" t="s">
-        <v>48</v>
+      <c r="B32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1585,17 +1597,14 @@
       <c r="B33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+      <c r="D33" t="s">
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,7 +1624,7 @@
         <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1626,16 +1635,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1646,16 +1655,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1666,16 +1675,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1686,16 +1695,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,16 +1715,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1726,16 +1735,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1746,16 +1755,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,13 +1775,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1780,16 +1792,19 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,19 +1812,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1819,17 +1831,14 @@
       <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="C45" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
+      <c r="D45" t="s">
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,16 +1849,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1860,13 +1869,16 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>161</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,13 +1889,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,13 +1909,13 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E49" t="s">
         <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1911,13 +1926,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,7 +1943,7 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E51" t="s">
         <v>53</v>
@@ -1945,13 +1960,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1961,14 +1976,14 @@
       <c r="B53" t="s">
         <v>45</v>
       </c>
-      <c r="C53" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" t="s">
-        <v>53</v>
-      </c>
-      <c r="F53" t="s">
-        <v>48</v>
+      <c r="C53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1979,13 +1994,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="E54" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1993,16 +2008,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,16 +2025,16 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
+        <v>51</v>
       </c>
       <c r="E56" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,16 +2042,16 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>178</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,13 +2059,10 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
       </c>
       <c r="E58" t="s">
         <v>24</v>
@@ -2064,19 +2076,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" t="s">
-        <v>111</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D59" t="s">
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2086,17 +2095,14 @@
       <c r="B60" t="s">
         <v>21</v>
       </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
+      <c r="D60" t="s">
+        <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F60" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2107,16 +2113,16 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,16 +2133,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2147,16 +2153,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,16 +2173,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,16 +2193,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,16 +2210,19 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,19 +2230,19 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>168</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2241,19 +2250,19 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F68" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2263,14 +2272,14 @@
       <c r="B69" t="s">
         <v>59</v>
       </c>
-      <c r="C69" t="s">
-        <v>93</v>
+      <c r="D69" t="s">
+        <v>87</v>
       </c>
       <c r="E69" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F69" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2281,13 +2290,16 @@
         <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>179</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F70" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2298,7 +2310,10 @@
         <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>60</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>53</v>
@@ -2312,16 +2327,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>189</v>
-      </c>
-      <c r="D72" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
       </c>
       <c r="E72" t="s">
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2329,16 +2344,16 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
-      </c>
-      <c r="D73" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C73" t="s">
+        <v>82</v>
       </c>
       <c r="E73" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>193</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2346,16 +2361,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,16 +2378,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="D75" t="s">
+        <v>65</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2380,16 +2395,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E76" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F76" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,16 +2412,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
-      </c>
-      <c r="D77" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C77" t="s">
+        <v>62</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,19 +2429,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F78" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2434,16 +2446,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
       <c r="D79" t="s">
         <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F79" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2451,16 +2463,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="D80" t="s">
         <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F80" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2468,16 +2480,19 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>114</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F81" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,16 +2500,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D82" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E82" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2502,19 +2517,16 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C83" t="s">
-        <v>91</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
       </c>
       <c r="E83" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F83" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,10 +2534,10 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>84</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2539,16 +2551,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E85" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2556,16 +2568,19 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C86" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F86" t="s">
-        <v>177</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2573,16 +2588,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D87" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E87" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F87" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2590,19 +2605,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D88" t="s">
+        <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F88" t="s">
-        <v>43</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2610,19 +2622,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" t="s">
-        <v>104</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D89" t="s">
+        <v>65</v>
       </c>
       <c r="E89" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="F89" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2632,17 +2641,14 @@
       <c r="B90" t="s">
         <v>19</v>
       </c>
-      <c r="C90" t="s">
-        <v>106</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
+      <c r="D90" t="s">
+        <v>87</v>
       </c>
       <c r="E90" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F90" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2653,16 +2659,16 @@
         <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F91" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2673,16 +2679,16 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F92" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2690,16 +2696,19 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,19 +2716,19 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2727,19 +2736,19 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,16 +2756,16 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
       <c r="D96" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E96" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F96" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2764,16 +2773,19 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>75</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2781,16 +2793,19 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F98" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2798,16 +2813,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F99" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2815,13 +2830,10 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
-      </c>
-      <c r="C100" t="s">
-        <v>70</v>
-      </c>
-      <c r="D100">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="D100" t="s">
+        <v>87</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -2835,16 +2847,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>186</v>
-      </c>
-      <c r="D101" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="C101" t="s">
+        <v>74</v>
       </c>
       <c r="E101" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2852,7 +2864,7 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D102" t="s">
         <v>87</v>
@@ -2869,10 +2881,13 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2886,16 +2901,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>69</v>
+        <v>186</v>
       </c>
       <c r="D104" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F104" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2903,13 +2918,10 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>69</v>
-      </c>
-      <c r="C105" t="s">
-        <v>70</v>
-      </c>
-      <c r="D105">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="D105" t="s">
+        <v>87</v>
       </c>
       <c r="E105" t="s">
         <v>11</v>
@@ -2923,16 +2935,16 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
-      </c>
-      <c r="D106" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
+        <v>74</v>
       </c>
       <c r="E106" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F106" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2940,16 +2952,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="D107" t="s">
         <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F107" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,19 +2969,19 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F108" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2977,16 +2989,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="D109" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E109" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F109" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2994,16 +3006,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
-      </c>
-      <c r="C110" t="s">
-        <v>124</v>
+        <v>162</v>
+      </c>
+      <c r="D110" t="s">
+        <v>87</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3011,16 +3023,19 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C111" t="s">
-        <v>52</v>
+        <v>164</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3030,14 +3045,14 @@
       <c r="B112" t="s">
         <v>118</v>
       </c>
-      <c r="C112" t="s">
-        <v>129</v>
+      <c r="D112" t="s">
+        <v>68</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3048,7 +3063,7 @@
         <v>118</v>
       </c>
       <c r="C113" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3065,13 +3080,13 @@
         <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3082,13 +3097,13 @@
         <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3099,13 +3114,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3116,13 +3131,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3130,16 +3145,16 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
-      </c>
-      <c r="D118" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C118" t="s">
+        <v>146</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3147,16 +3162,16 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3164,16 +3179,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>149</v>
-      </c>
-      <c r="D120" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="C120" t="s">
+        <v>51</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3181,16 +3196,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
-      </c>
-      <c r="C121" t="s">
-        <v>151</v>
+        <v>165</v>
+      </c>
+      <c r="D121" t="s">
+        <v>87</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,16 +3213,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C122" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3217,8 +3232,8 @@
       <c r="B123" t="s">
         <v>149</v>
       </c>
-      <c r="C123" t="s">
-        <v>150</v>
+      <c r="D123" t="s">
+        <v>68</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
@@ -3235,7 +3250,7 @@
         <v>149</v>
       </c>
       <c r="C124" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3249,16 +3264,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>138</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C125" t="s">
+        <v>49</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3266,10 +3281,10 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3283,16 +3298,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3302,8 +3317,8 @@
       <c r="B128" t="s">
         <v>138</v>
       </c>
-      <c r="C128" t="s">
-        <v>57</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3320,13 +3335,13 @@
         <v>138</v>
       </c>
       <c r="C129" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3337,13 +3352,13 @@
         <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3354,13 +3369,13 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,7 +3386,7 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3385,16 +3400,16 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>125</v>
-      </c>
-      <c r="D133" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C133" t="s">
+        <v>154</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3402,16 +3417,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3419,16 +3434,16 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>131</v>
-      </c>
-      <c r="D135" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C135" t="s">
+        <v>157</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3436,16 +3451,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>131</v>
-      </c>
-      <c r="C136" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="D136" t="s">
+        <v>68</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3453,16 +3468,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C137" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3472,8 +3487,8 @@
       <c r="B138" t="s">
         <v>131</v>
       </c>
-      <c r="C138" t="s">
-        <v>134</v>
+      <c r="D138" t="s">
+        <v>68</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
@@ -3490,7 +3505,7 @@
         <v>131</v>
       </c>
       <c r="C139" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
@@ -3504,16 +3519,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>126</v>
-      </c>
-      <c r="D140" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C140" t="s">
+        <v>133</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3521,16 +3536,16 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C141" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3538,16 +3553,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>98</v>
-      </c>
-      <c r="D142" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C142" t="s">
+        <v>135</v>
       </c>
       <c r="E142" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F142" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3555,16 +3570,16 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="D143" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F143" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3572,19 +3587,16 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F144" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3592,19 +3604,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>13</v>
-      </c>
-      <c r="C145" t="s">
-        <v>20</v>
-      </c>
-      <c r="D145">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D145" t="s">
+        <v>87</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,11 +3623,8 @@
       <c r="B146" t="s">
         <v>13</v>
       </c>
-      <c r="C146" t="s">
-        <v>18</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
+      <c r="D146" t="s">
+        <v>87</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
@@ -3632,16 +3638,19 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>97</v>
-      </c>
-      <c r="D147" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
       </c>
       <c r="E147" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3649,16 +3658,19 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>191</v>
+        <v>20</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
       </c>
       <c r="E148" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3666,16 +3678,19 @@
         <v>32</v>
       </c>
       <c r="B149" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C149" t="s">
+        <v>18</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
       </c>
       <c r="E149" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3683,13 +3698,10 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>33</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="D150" t="s">
+        <v>87</v>
       </c>
       <c r="E150" t="s">
         <v>54</v>
@@ -3703,19 +3715,16 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>33</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C151" t="s">
+        <v>191</v>
       </c>
       <c r="E151" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F151" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3725,8 +3734,8 @@
       <c r="B152" t="s">
         <v>33</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>57</v>
+      <c r="D152" t="s">
+        <v>87</v>
       </c>
       <c r="E152" t="s">
         <v>54</v>
@@ -3743,13 +3752,16 @@
         <v>33</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
       </c>
       <c r="E153" t="s">
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>193</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3757,17 +3769,19 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>182</v>
-      </c>
-      <c r="C154" s="1"/>
-      <c r="D154" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
       </c>
       <c r="E154" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F154" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3775,15 +3789,67 @@
         <v>32</v>
       </c>
       <c r="B155" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E155" t="s">
+        <v>54</v>
+      </c>
+      <c r="F155" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>32</v>
+      </c>
+      <c r="B156" t="s">
+        <v>33</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E156" t="s">
+        <v>54</v>
+      </c>
+      <c r="F156" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>32</v>
+      </c>
+      <c r="B157" t="s">
+        <v>182</v>
+      </c>
+      <c r="C157" s="1"/>
+      <c r="D157" t="s">
+        <v>68</v>
+      </c>
+      <c r="E157" t="s">
+        <v>116</v>
+      </c>
+      <c r="F157" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>32</v>
+      </c>
+      <c r="B158" t="s">
         <v>88</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D158" t="s">
         <v>65</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E158" t="s">
         <v>24</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F158" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (Shape) Add placeholder snippet (#1035)
* [PowerPoint] (Shape) Add placeholder snippet

* Fix typo
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F018D6-5A1B-49AB-9291-C4B5C81F4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D902EC-FD39-449E-B854-98898D62E7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="200">
   <si>
     <t>Class</t>
   </si>
@@ -608,6 +608,18 @@
   </si>
   <si>
     <t>paragraphFormat</t>
+  </si>
+  <si>
+    <t>placeholderFormat</t>
+  </si>
+  <si>
+    <t>getPlaceholderShapes</t>
+  </si>
+  <si>
+    <t>PlaceholderFormat</t>
+  </si>
+  <si>
+    <t>PlaceholderType</t>
   </si>
 </sst>
 </file>
@@ -650,9 +662,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +700,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F155" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F155" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F151">
-    <sortCondition ref="B1:B151"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F158" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
+    <sortCondition ref="B1:B154"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1001,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1545,37 +1558,36 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
+      <c r="B31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>87</v>
       </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" t="s">
-        <v>7</v>
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" t="s">
-        <v>48</v>
+      <c r="B32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1585,17 +1597,14 @@
       <c r="B33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
+      <c r="D33" t="s">
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,7 +1624,7 @@
         <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1626,16 +1635,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1646,16 +1655,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1666,16 +1675,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1686,16 +1695,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,16 +1715,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1726,16 +1735,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1746,16 +1755,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,13 +1775,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1780,16 +1792,19 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,19 +1812,16 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1819,17 +1831,14 @@
       <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="C45" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
+      <c r="D45" t="s">
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,16 +1849,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1860,13 +1869,16 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>161</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,13 +1889,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,13 +1909,13 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E49" t="s">
         <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1911,13 +1926,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,7 +1943,7 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E51" t="s">
         <v>53</v>
@@ -1945,13 +1960,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1961,14 +1976,14 @@
       <c r="B53" t="s">
         <v>45</v>
       </c>
-      <c r="C53" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" t="s">
-        <v>53</v>
-      </c>
-      <c r="F53" t="s">
-        <v>48</v>
+      <c r="C53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1979,13 +1994,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="E54" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1993,16 +2008,16 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,16 +2025,16 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
+        <v>51</v>
       </c>
       <c r="E56" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,16 +2042,16 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>178</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,13 +2059,10 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
       </c>
       <c r="E58" t="s">
         <v>24</v>
@@ -2064,19 +2076,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" t="s">
-        <v>111</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D59" t="s">
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2086,17 +2095,14 @@
       <c r="B60" t="s">
         <v>21</v>
       </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
+      <c r="D60" t="s">
+        <v>87</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F60" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2107,16 +2113,16 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2127,16 +2133,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2147,16 +2153,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,16 +2173,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,16 +2193,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,16 +2210,19 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,19 +2230,19 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>168</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2241,19 +2250,19 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F68" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2263,14 +2272,14 @@
       <c r="B69" t="s">
         <v>59</v>
       </c>
-      <c r="C69" t="s">
-        <v>93</v>
+      <c r="D69" t="s">
+        <v>87</v>
       </c>
       <c r="E69" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F69" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2281,13 +2290,16 @@
         <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>82</v>
+        <v>179</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F70" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2298,7 +2310,10 @@
         <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>60</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>53</v>
@@ -2312,16 +2327,16 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>189</v>
-      </c>
-      <c r="D72" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
       </c>
       <c r="E72" t="s">
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2329,16 +2344,16 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
-      </c>
-      <c r="D73" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C73" t="s">
+        <v>82</v>
       </c>
       <c r="E73" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>193</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2346,16 +2361,16 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2363,16 +2378,16 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="D75" t="s">
+        <v>65</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2380,16 +2395,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E76" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F76" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,16 +2412,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
-      </c>
-      <c r="D77" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C77" t="s">
+        <v>62</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,19 +2429,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F78" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2434,16 +2446,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
       <c r="D79" t="s">
         <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F79" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2451,16 +2463,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="D80" t="s">
         <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F80" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2468,16 +2480,19 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>114</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F81" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2485,16 +2500,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D82" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E82" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2502,19 +2517,16 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C83" t="s">
-        <v>91</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
       </c>
       <c r="E83" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F83" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,10 +2534,10 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>84</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2539,16 +2551,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E85" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F85" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2556,16 +2568,19 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C86" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F86" t="s">
-        <v>177</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2573,16 +2588,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D87" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E87" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F87" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2590,19 +2605,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D88" t="s">
+        <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F88" t="s">
-        <v>43</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2610,19 +2622,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" t="s">
-        <v>104</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D89" t="s">
+        <v>65</v>
       </c>
       <c r="E89" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="F89" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2632,17 +2641,14 @@
       <c r="B90" t="s">
         <v>19</v>
       </c>
-      <c r="C90" t="s">
-        <v>106</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
+      <c r="D90" t="s">
+        <v>87</v>
       </c>
       <c r="E90" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F90" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2653,16 +2659,16 @@
         <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F91" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2673,16 +2679,16 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F92" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2690,16 +2696,19 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2707,19 +2716,19 @@
         <v>32</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2727,19 +2736,19 @@
         <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,16 +2756,16 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
       <c r="D96" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E96" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F96" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2764,16 +2773,19 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>75</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -2781,16 +2793,19 @@
         <v>32</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F98" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2798,16 +2813,16 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F99" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2815,13 +2830,10 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
-      </c>
-      <c r="C100" t="s">
-        <v>70</v>
-      </c>
-      <c r="D100">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="D100" t="s">
+        <v>87</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -2835,16 +2847,16 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>186</v>
-      </c>
-      <c r="D101" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="C101" t="s">
+        <v>74</v>
       </c>
       <c r="E101" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2852,7 +2864,7 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D102" t="s">
         <v>87</v>
@@ -2869,10 +2881,13 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2886,16 +2901,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>69</v>
+        <v>186</v>
       </c>
       <c r="D104" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F104" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2903,13 +2918,10 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>69</v>
-      </c>
-      <c r="C105" t="s">
-        <v>70</v>
-      </c>
-      <c r="D105">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="D105" t="s">
+        <v>87</v>
       </c>
       <c r="E105" t="s">
         <v>11</v>
@@ -2923,16 +2935,16 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
-      </c>
-      <c r="D106" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
+        <v>74</v>
       </c>
       <c r="E106" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F106" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2940,16 +2952,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="D107" t="s">
         <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F107" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,19 +2969,19 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F108" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2977,16 +2989,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="D109" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E109" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F109" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2994,16 +3006,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
-      </c>
-      <c r="C110" t="s">
-        <v>124</v>
+        <v>162</v>
+      </c>
+      <c r="D110" t="s">
+        <v>87</v>
       </c>
       <c r="E110" t="s">
         <v>116</v>
       </c>
       <c r="F110" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3011,16 +3023,19 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C111" t="s">
-        <v>52</v>
+        <v>164</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
       </c>
       <c r="F111" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3030,14 +3045,14 @@
       <c r="B112" t="s">
         <v>118</v>
       </c>
-      <c r="C112" t="s">
-        <v>129</v>
+      <c r="D112" t="s">
+        <v>68</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3048,7 +3063,7 @@
         <v>118</v>
       </c>
       <c r="C113" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
@@ -3065,13 +3080,13 @@
         <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3082,13 +3097,13 @@
         <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3099,13 +3114,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3116,13 +3131,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3130,16 +3145,16 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
-      </c>
-      <c r="D118" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C118" t="s">
+        <v>146</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3147,16 +3162,16 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3164,16 +3179,16 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>149</v>
-      </c>
-      <c r="D120" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="C120" t="s">
+        <v>51</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3181,16 +3196,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
-      </c>
-      <c r="C121" t="s">
-        <v>151</v>
+        <v>165</v>
+      </c>
+      <c r="D121" t="s">
+        <v>87</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3198,16 +3213,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C122" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3217,8 +3232,8 @@
       <c r="B123" t="s">
         <v>149</v>
       </c>
-      <c r="C123" t="s">
-        <v>150</v>
+      <c r="D123" t="s">
+        <v>68</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
@@ -3235,7 +3250,7 @@
         <v>149</v>
       </c>
       <c r="C124" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3249,16 +3264,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>138</v>
-      </c>
-      <c r="D125" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C125" t="s">
+        <v>49</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3266,10 +3281,10 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3283,16 +3298,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3302,8 +3317,8 @@
       <c r="B128" t="s">
         <v>138</v>
       </c>
-      <c r="C128" t="s">
-        <v>57</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3320,13 +3335,13 @@
         <v>138</v>
       </c>
       <c r="C129" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3337,13 +3352,13 @@
         <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3354,13 +3369,13 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,7 +3386,7 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3385,16 +3400,16 @@
         <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>125</v>
-      </c>
-      <c r="D133" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C133" t="s">
+        <v>154</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3402,16 +3417,16 @@
         <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3419,16 +3434,16 @@
         <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>131</v>
-      </c>
-      <c r="D135" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C135" t="s">
+        <v>157</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3436,16 +3451,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>131</v>
-      </c>
-      <c r="C136" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="D136" t="s">
+        <v>68</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3453,16 +3468,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C137" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3472,8 +3487,8 @@
       <c r="B138" t="s">
         <v>131</v>
       </c>
-      <c r="C138" t="s">
-        <v>134</v>
+      <c r="D138" t="s">
+        <v>68</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
@@ -3490,7 +3505,7 @@
         <v>131</v>
       </c>
       <c r="C139" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
@@ -3504,16 +3519,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>126</v>
-      </c>
-      <c r="D140" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C140" t="s">
+        <v>133</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3521,16 +3536,16 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C141" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3538,16 +3553,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>98</v>
-      </c>
-      <c r="D142" t="s">
-        <v>87</v>
+        <v>131</v>
+      </c>
+      <c r="C142" t="s">
+        <v>135</v>
       </c>
       <c r="E142" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F142" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3555,16 +3570,16 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="D143" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F143" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3572,19 +3587,16 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F144" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3592,19 +3604,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>13</v>
-      </c>
-      <c r="C145" t="s">
-        <v>20</v>
-      </c>
-      <c r="D145">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D145" t="s">
+        <v>87</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,11 +3623,8 @@
       <c r="B146" t="s">
         <v>13</v>
       </c>
-      <c r="C146" t="s">
-        <v>18</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
+      <c r="D146" t="s">
+        <v>87</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
@@ -3632,16 +3638,19 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>97</v>
-      </c>
-      <c r="D147" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
       </c>
       <c r="E147" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3649,16 +3658,19 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>191</v>
+        <v>20</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
       </c>
       <c r="E148" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3666,16 +3678,19 @@
         <v>32</v>
       </c>
       <c r="B149" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C149" t="s">
+        <v>18</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
       </c>
       <c r="E149" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3683,13 +3698,10 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>33</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="D150" t="s">
+        <v>87</v>
       </c>
       <c r="E150" t="s">
         <v>54</v>
@@ -3703,19 +3715,16 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>33</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C151" t="s">
+        <v>191</v>
       </c>
       <c r="E151" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F151" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3725,8 +3734,8 @@
       <c r="B152" t="s">
         <v>33</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>57</v>
+      <c r="D152" t="s">
+        <v>87</v>
       </c>
       <c r="E152" t="s">
         <v>54</v>
@@ -3743,13 +3752,16 @@
         <v>33</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
       </c>
       <c r="E153" t="s">
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>193</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3757,17 +3769,19 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>182</v>
-      </c>
-      <c r="C154" s="1"/>
-      <c r="D154" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
       </c>
       <c r="E154" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F154" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3775,15 +3789,67 @@
         <v>32</v>
       </c>
       <c r="B155" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E155" t="s">
+        <v>54</v>
+      </c>
+      <c r="F155" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>32</v>
+      </c>
+      <c r="B156" t="s">
+        <v>33</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E156" t="s">
+        <v>54</v>
+      </c>
+      <c r="F156" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>32</v>
+      </c>
+      <c r="B157" t="s">
+        <v>182</v>
+      </c>
+      <c r="C157" s="1"/>
+      <c r="D157" t="s">
+        <v>68</v>
+      </c>
+      <c r="E157" t="s">
+        <v>116</v>
+      </c>
+      <c r="F157" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>32</v>
+      </c>
+      <c r="B158" t="s">
         <v>88</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D158" t="s">
         <v>65</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E158" t="s">
         <v>24</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F158" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (beta) Add snippet for Presentation.getActiveSlide
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D902EC-FD39-449E-B854-98898D62E7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD69F-DE60-4A39-A2D8-9D33F8E2C07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="203">
   <si>
     <t>Class</t>
   </si>
@@ -620,6 +620,15 @@
   </si>
   <si>
     <t>PlaceholderType</t>
+  </si>
+  <si>
+    <t>getActiveSlideOrNullObject</t>
+  </si>
+  <si>
+    <t>powerpoint-basics-presentation-get-active-slide</t>
+  </si>
+  <si>
+    <t>getActiveSlide</t>
   </si>
 </sst>
 </file>
@@ -700,10 +709,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F158" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
-    <sortCondition ref="B1:B154"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F159" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F159" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F155">
+    <sortCondition ref="B1:B155"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1014,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,17 +1567,16 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1576,17 +1584,16 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="2"/>
       <c r="D32" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1614,17 +1621,17 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
-        <v>35</v>
+      <c r="C34" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" t="s">
-        <v>48</v>
+      <c r="E34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1644,7 +1651,7 @@
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1664,7 +1671,7 @@
         <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1675,16 +1682,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1704,7 +1711,7 @@
         <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1715,16 +1722,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1744,7 +1751,7 @@
         <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,16 +1762,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1775,16 +1782,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1804,7 +1811,7 @@
         <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,13 +1822,16 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1829,16 +1839,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>175</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,17 +1858,14 @@
       <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
+      <c r="D46" t="s">
+        <v>87</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,16 +1876,16 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,16 +1896,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1909,13 +1916,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,13 +1936,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,13 +1953,13 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F51" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1960,7 +1970,7 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E52" t="s">
         <v>53</v>
@@ -1976,14 +1986,14 @@
       <c r="B53" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>197</v>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,13 +2004,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>48</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,13 +2021,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2028,13 +2038,13 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2045,13 +2055,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E57" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2059,16 +2069,16 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>178</v>
       </c>
       <c r="E58" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2076,16 +2086,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E59" t="s">
         <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2093,16 +2103,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="D60" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2112,17 +2122,14 @@
       <c r="B61" t="s">
         <v>21</v>
       </c>
-      <c r="C61" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
+      <c r="D61" t="s">
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,16 +2140,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2153,16 +2160,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,16 +2180,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F64" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,16 +2200,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2213,16 +2220,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F66" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2233,16 +2240,16 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,16 +2260,16 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,10 +2277,13 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
-      </c>
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
       </c>
       <c r="E69" t="s">
         <v>85</v>
@@ -2289,17 +2299,14 @@
       <c r="B70" t="s">
         <v>59</v>
       </c>
-      <c r="C70" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+      <c r="D70" t="s">
+        <v>87</v>
       </c>
       <c r="E70" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F70" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,16 +2317,16 @@
         <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F71" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2330,13 +2337,16 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2347,13 +2357,13 @@
         <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E73" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2364,13 +2374,13 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F74" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2378,10 +2388,10 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>189</v>
-      </c>
-      <c r="D75" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C75" t="s">
+        <v>86</v>
       </c>
       <c r="E75" t="s">
         <v>53</v>
@@ -2395,16 +2405,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="D76" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,14 +2424,14 @@
       <c r="B77" t="s">
         <v>61</v>
       </c>
-      <c r="C77" t="s">
-        <v>62</v>
+      <c r="D77" t="s">
+        <v>87</v>
       </c>
       <c r="E77" t="s">
         <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2432,13 +2442,13 @@
         <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="E78" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2446,10 +2456,10 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>190</v>
       </c>
       <c r="E79" t="s">
         <v>24</v>
@@ -2463,16 +2473,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E80" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F80" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2482,11 +2492,8 @@
       <c r="B81" t="s">
         <v>113</v>
       </c>
-      <c r="C81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
+      <c r="D81" t="s">
+        <v>87</v>
       </c>
       <c r="E81" t="s">
         <v>109</v>
@@ -2500,16 +2507,19 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" t="s">
-        <v>65</v>
+        <v>113</v>
+      </c>
+      <c r="C82" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F82" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,10 +2527,10 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D83" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E83" t="s">
         <v>85</v>
@@ -2536,8 +2546,8 @@
       <c r="B84" t="s">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
-        <v>84</v>
+      <c r="D84" t="s">
+        <v>87</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2551,16 +2561,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>90</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C85" t="s">
+        <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F85" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2570,17 +2580,14 @@
       <c r="B86" t="s">
         <v>90</v>
       </c>
-      <c r="C86" t="s">
-        <v>91</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
+      <c r="D86" t="s">
+        <v>87</v>
       </c>
       <c r="E86" t="s">
         <v>53</v>
       </c>
       <c r="F86" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2588,16 +2595,19 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
-      </c>
-      <c r="D87" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C87" t="s">
+        <v>91</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2605,16 +2615,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F88" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,7 +2641,7 @@
         <v>168</v>
       </c>
       <c r="F89" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2639,16 +2649,16 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D90" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E90" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F90" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2658,17 +2668,14 @@
       <c r="B91" t="s">
         <v>19</v>
       </c>
-      <c r="C91" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
+      <c r="D91" t="s">
+        <v>87</v>
       </c>
       <c r="E91" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,16 +2686,16 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F92" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2699,7 +2706,7 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -2719,16 +2726,16 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F94" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2748,7 +2755,7 @@
         <v>53</v>
       </c>
       <c r="F95" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2763,19 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,11 +2785,8 @@
       <c r="B97" t="s">
         <v>9</v>
       </c>
-      <c r="C97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
+      <c r="D97" t="s">
+        <v>87</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2796,16 +2803,16 @@
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D98">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,16 +2820,19 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>185</v>
-      </c>
-      <c r="D99" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F99" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,16 +2840,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="D100" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F100" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2849,8 +2859,8 @@
       <c r="B101" t="s">
         <v>75</v>
       </c>
-      <c r="C101" t="s">
-        <v>74</v>
+      <c r="D101" t="s">
+        <v>87</v>
       </c>
       <c r="E101" t="s">
         <v>11</v>
@@ -2864,10 +2874,10 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>72</v>
-      </c>
-      <c r="D102" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="C102" t="s">
+        <v>74</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -2883,11 +2893,8 @@
       <c r="B103" t="s">
         <v>72</v>
       </c>
-      <c r="C103" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103">
-        <v>2</v>
+      <c r="D103" t="s">
+        <v>87</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2901,16 +2908,19 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>186</v>
-      </c>
-      <c r="D104" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="C104" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F104" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,16 +2928,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="D105" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F105" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2937,8 +2947,8 @@
       <c r="B106" t="s">
         <v>73</v>
       </c>
-      <c r="C106" t="s">
-        <v>74</v>
+      <c r="D106" t="s">
+        <v>87</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2952,10 +2962,10 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>69</v>
-      </c>
-      <c r="D107" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>74</v>
       </c>
       <c r="E107" t="s">
         <v>11</v>
@@ -2971,11 +2981,8 @@
       <c r="B108" t="s">
         <v>69</v>
       </c>
-      <c r="C108" t="s">
-        <v>70</v>
-      </c>
-      <c r="D108">
-        <v>2</v>
+      <c r="D108" t="s">
+        <v>87</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -2989,16 +2996,19 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
-      </c>
-      <c r="D109" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C109" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F109" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3006,16 +3016,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
       </c>
       <c r="E110" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F110" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3025,11 +3035,8 @@
       <c r="B111" t="s">
         <v>162</v>
       </c>
-      <c r="C111" t="s">
-        <v>164</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
+      <c r="D111" t="s">
+        <v>87</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
@@ -3043,16 +3050,19 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
-      </c>
-      <c r="D112" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C112" t="s">
+        <v>164</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3062,14 +3072,14 @@
       <c r="B113" t="s">
         <v>118</v>
       </c>
-      <c r="C113" t="s">
-        <v>124</v>
+      <c r="D113" t="s">
+        <v>68</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3080,13 +3090,13 @@
         <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3097,13 +3107,13 @@
         <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3114,13 +3124,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3131,13 +3141,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3148,13 +3158,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,13 +3175,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3182,13 +3192,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3196,16 +3206,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>165</v>
-      </c>
-      <c r="D121" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C121" t="s">
+        <v>51</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3215,8 +3225,8 @@
       <c r="B122" t="s">
         <v>165</v>
       </c>
-      <c r="C122" t="s">
-        <v>166</v>
+      <c r="D122" t="s">
+        <v>87</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
@@ -3230,16 +3240,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
-      </c>
-      <c r="D123" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C123" t="s">
+        <v>166</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3249,8 +3259,8 @@
       <c r="B124" t="s">
         <v>149</v>
       </c>
-      <c r="C124" t="s">
-        <v>151</v>
+      <c r="D124" t="s">
+        <v>68</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3267,7 +3277,7 @@
         <v>149</v>
       </c>
       <c r="C125" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
@@ -3284,7 +3294,7 @@
         <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3301,7 +3311,7 @@
         <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3315,16 +3325,16 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
-      </c>
-      <c r="D128" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C128" t="s">
+        <v>50</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3334,14 +3344,14 @@
       <c r="B129" t="s">
         <v>138</v>
       </c>
-      <c r="C129" t="s">
-        <v>148</v>
+      <c r="D129" t="s">
+        <v>68</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3352,13 +3362,13 @@
         <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3369,7 +3379,7 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3386,13 +3396,13 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,13 +3413,13 @@
         <v>138</v>
       </c>
       <c r="C133" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3420,13 +3430,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3437,13 +3447,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,16 +3461,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>125</v>
-      </c>
-      <c r="D136" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C136" t="s">
+        <v>157</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3470,8 +3480,8 @@
       <c r="B137" t="s">
         <v>125</v>
       </c>
-      <c r="C137" t="s">
-        <v>127</v>
+      <c r="D137" t="s">
+        <v>68</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
@@ -3485,16 +3495,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>131</v>
-      </c>
-      <c r="D138" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C138" t="s">
+        <v>127</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3504,8 +3514,8 @@
       <c r="B139" t="s">
         <v>131</v>
       </c>
-      <c r="C139" t="s">
-        <v>132</v>
+      <c r="D139" t="s">
+        <v>68</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
@@ -3522,7 +3532,7 @@
         <v>131</v>
       </c>
       <c r="C140" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
@@ -3539,7 +3549,7 @@
         <v>131</v>
       </c>
       <c r="C141" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
@@ -3556,7 +3566,7 @@
         <v>131</v>
       </c>
       <c r="C142" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
@@ -3570,16 +3580,16 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>126</v>
-      </c>
-      <c r="D143" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C143" t="s">
+        <v>135</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
       </c>
       <c r="F143" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3589,8 +3599,8 @@
       <c r="B144" t="s">
         <v>126</v>
       </c>
-      <c r="C144" t="s">
-        <v>128</v>
+      <c r="D144" t="s">
+        <v>68</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
@@ -3604,16 +3614,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>98</v>
-      </c>
-      <c r="D145" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C145" t="s">
+        <v>128</v>
       </c>
       <c r="E145" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F145" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3621,7 +3631,7 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D146" t="s">
         <v>87</v>
@@ -3630,7 +3640,7 @@
         <v>14</v>
       </c>
       <c r="F146" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3640,17 +3650,14 @@
       <c r="B147" t="s">
         <v>13</v>
       </c>
-      <c r="C147" t="s">
-        <v>10</v>
-      </c>
-      <c r="D147">
-        <v>1</v>
+      <c r="D147" t="s">
+        <v>87</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3661,7 +3668,7 @@
         <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -3670,7 +3677,7 @@
         <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3681,7 +3688,7 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -3690,7 +3697,7 @@
         <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3698,16 +3705,19 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>97</v>
-      </c>
-      <c r="D150" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C150" t="s">
+        <v>18</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
       </c>
       <c r="E150" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,14 +3727,14 @@
       <c r="B151" t="s">
         <v>97</v>
       </c>
-      <c r="C151" t="s">
-        <v>191</v>
+      <c r="D151" t="s">
+        <v>87</v>
       </c>
       <c r="E151" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F151" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3732,16 +3742,16 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>33</v>
-      </c>
-      <c r="D152" t="s">
-        <v>87</v>
+        <v>97</v>
+      </c>
+      <c r="C152" t="s">
+        <v>191</v>
       </c>
       <c r="E152" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F152" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3751,17 +3761,14 @@
       <c r="B153" t="s">
         <v>33</v>
       </c>
-      <c r="C153" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D153">
-        <v>1</v>
+      <c r="D153" t="s">
+        <v>87</v>
       </c>
       <c r="E153" t="s">
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3781,7 +3788,7 @@
         <v>54</v>
       </c>
       <c r="F154" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3792,13 +3799,16 @@
         <v>33</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
       </c>
       <c r="E155" t="s">
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3809,13 +3819,13 @@
         <v>33</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="E156" t="s">
         <v>54</v>
       </c>
       <c r="F156" t="s">
-        <v>193</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,17 +3833,16 @@
         <v>32</v>
       </c>
       <c r="B157" t="s">
-        <v>182</v>
-      </c>
-      <c r="C157" s="1"/>
-      <c r="D157" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="E157" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3841,15 +3850,33 @@
         <v>32</v>
       </c>
       <c r="B158" t="s">
+        <v>182</v>
+      </c>
+      <c r="C158" s="1"/>
+      <c r="D158" t="s">
+        <v>68</v>
+      </c>
+      <c r="E158" t="s">
+        <v>116</v>
+      </c>
+      <c r="F158" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>32</v>
+      </c>
+      <c r="B159" t="s">
         <v>88</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D159" t="s">
         <v>65</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E159" t="s">
         <v>24</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F159" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (beta) Add snippet for Presentation.getActiveSlide (#1040)
* [PowerPoint] (beta) Add snippet for Presentation.getActiveSlide

* Tweaks
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D902EC-FD39-449E-B854-98898D62E7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD69F-DE60-4A39-A2D8-9D33F8E2C07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="203">
   <si>
     <t>Class</t>
   </si>
@@ -620,6 +620,15 @@
   </si>
   <si>
     <t>PlaceholderType</t>
+  </si>
+  <si>
+    <t>getActiveSlideOrNullObject</t>
+  </si>
+  <si>
+    <t>powerpoint-basics-presentation-get-active-slide</t>
+  </si>
+  <si>
+    <t>getActiveSlide</t>
   </si>
 </sst>
 </file>
@@ -700,10 +709,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F158" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F158" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F154">
-    <sortCondition ref="B1:B154"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F159" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F159" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F155">
+    <sortCondition ref="B1:B155"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1014,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,17 +1567,16 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1576,17 +1584,16 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="2"/>
       <c r="D32" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1614,17 +1621,17 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
-        <v>35</v>
+      <c r="C34" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" t="s">
-        <v>48</v>
+      <c r="E34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1644,7 +1651,7 @@
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1664,7 +1671,7 @@
         <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1675,16 +1682,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1704,7 +1711,7 @@
         <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1715,16 +1722,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1744,7 +1751,7 @@
         <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,16 +1762,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1775,16 +1782,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1804,7 +1811,7 @@
         <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1815,13 +1822,16 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1829,16 +1839,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>175</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,17 +1858,14 @@
       <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
+      <c r="D46" t="s">
+        <v>87</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,16 +1876,16 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,16 +1896,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1909,13 +1916,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,13 +1936,13 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F50" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,13 +1953,13 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F51" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1960,7 +1970,7 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E52" t="s">
         <v>53</v>
@@ -1976,14 +1986,14 @@
       <c r="B53" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>197</v>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,13 +2004,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>48</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2011,13 +2021,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2028,13 +2038,13 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2045,13 +2055,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E57" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2059,16 +2069,16 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>178</v>
       </c>
       <c r="E58" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2076,16 +2086,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E59" t="s">
         <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2093,16 +2103,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="D60" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2112,17 +2122,14 @@
       <c r="B61" t="s">
         <v>21</v>
       </c>
-      <c r="C61" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
+      <c r="D61" t="s">
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,16 +2140,16 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2153,16 +2160,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,16 +2180,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F64" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,16 +2200,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2213,16 +2220,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F66" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2233,16 +2240,16 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,16 +2260,16 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,10 +2277,13 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
-      </c>
-      <c r="D69" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
       </c>
       <c r="E69" t="s">
         <v>85</v>
@@ -2289,17 +2299,14 @@
       <c r="B70" t="s">
         <v>59</v>
       </c>
-      <c r="C70" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
+      <c r="D70" t="s">
+        <v>87</v>
       </c>
       <c r="E70" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F70" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,16 +2317,16 @@
         <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F71" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2330,13 +2337,16 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2347,13 +2357,13 @@
         <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E73" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2364,13 +2374,13 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F74" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2378,10 +2388,10 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>189</v>
-      </c>
-      <c r="D75" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C75" t="s">
+        <v>86</v>
       </c>
       <c r="E75" t="s">
         <v>53</v>
@@ -2395,16 +2405,16 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="D76" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,14 +2424,14 @@
       <c r="B77" t="s">
         <v>61</v>
       </c>
-      <c r="C77" t="s">
-        <v>62</v>
+      <c r="D77" t="s">
+        <v>87</v>
       </c>
       <c r="E77" t="s">
         <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2432,13 +2442,13 @@
         <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="E78" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2446,10 +2456,10 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>190</v>
       </c>
       <c r="E79" t="s">
         <v>24</v>
@@ -2463,16 +2473,16 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E80" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F80" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2482,11 +2492,8 @@
       <c r="B81" t="s">
         <v>113</v>
       </c>
-      <c r="C81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
+      <c r="D81" t="s">
+        <v>87</v>
       </c>
       <c r="E81" t="s">
         <v>109</v>
@@ -2500,16 +2507,19 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" t="s">
-        <v>65</v>
+        <v>113</v>
+      </c>
+      <c r="C82" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F82" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2517,10 +2527,10 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D83" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E83" t="s">
         <v>85</v>
@@ -2536,8 +2546,8 @@
       <c r="B84" t="s">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
-        <v>84</v>
+      <c r="D84" t="s">
+        <v>87</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2551,16 +2561,16 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>90</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C85" t="s">
+        <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F85" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2570,17 +2580,14 @@
       <c r="B86" t="s">
         <v>90</v>
       </c>
-      <c r="C86" t="s">
-        <v>91</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
+      <c r="D86" t="s">
+        <v>87</v>
       </c>
       <c r="E86" t="s">
         <v>53</v>
       </c>
       <c r="F86" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2588,16 +2595,19 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
-      </c>
-      <c r="D87" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C87" t="s">
+        <v>91</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2605,16 +2615,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F88" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,7 +2641,7 @@
         <v>168</v>
       </c>
       <c r="F89" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2639,16 +2649,16 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D90" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E90" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F90" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2658,17 +2668,14 @@
       <c r="B91" t="s">
         <v>19</v>
       </c>
-      <c r="C91" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
+      <c r="D91" t="s">
+        <v>87</v>
       </c>
       <c r="E91" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,16 +2686,16 @@
         <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F92" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2699,7 +2706,7 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -2719,16 +2726,16 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F94" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2748,7 +2755,7 @@
         <v>53</v>
       </c>
       <c r="F95" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2763,19 @@
         <v>32</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,11 +2785,8 @@
       <c r="B97" t="s">
         <v>9</v>
       </c>
-      <c r="C97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
+      <c r="D97" t="s">
+        <v>87</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -2796,16 +2803,16 @@
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D98">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,16 +2820,19 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>185</v>
-      </c>
-      <c r="D99" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F99" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,16 +2840,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="D100" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F100" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2849,8 +2859,8 @@
       <c r="B101" t="s">
         <v>75</v>
       </c>
-      <c r="C101" t="s">
-        <v>74</v>
+      <c r="D101" t="s">
+        <v>87</v>
       </c>
       <c r="E101" t="s">
         <v>11</v>
@@ -2864,10 +2874,10 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>72</v>
-      </c>
-      <c r="D102" t="s">
-        <v>87</v>
+        <v>75</v>
+      </c>
+      <c r="C102" t="s">
+        <v>74</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -2883,11 +2893,8 @@
       <c r="B103" t="s">
         <v>72</v>
       </c>
-      <c r="C103" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103">
-        <v>2</v>
+      <c r="D103" t="s">
+        <v>87</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2901,16 +2908,19 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>186</v>
-      </c>
-      <c r="D104" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="C104" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F104" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,16 +2928,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="D105" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F105" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2937,8 +2947,8 @@
       <c r="B106" t="s">
         <v>73</v>
       </c>
-      <c r="C106" t="s">
-        <v>74</v>
+      <c r="D106" t="s">
+        <v>87</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2952,10 +2962,10 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>69</v>
-      </c>
-      <c r="D107" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>74</v>
       </c>
       <c r="E107" t="s">
         <v>11</v>
@@ -2971,11 +2981,8 @@
       <c r="B108" t="s">
         <v>69</v>
       </c>
-      <c r="C108" t="s">
-        <v>70</v>
-      </c>
-      <c r="D108">
-        <v>2</v>
+      <c r="D108" t="s">
+        <v>87</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -2989,16 +2996,19 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
-      </c>
-      <c r="D109" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C109" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F109" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3006,16 +3016,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
       </c>
       <c r="E110" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F110" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3025,11 +3035,8 @@
       <c r="B111" t="s">
         <v>162</v>
       </c>
-      <c r="C111" t="s">
-        <v>164</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
+      <c r="D111" t="s">
+        <v>87</v>
       </c>
       <c r="E111" t="s">
         <v>116</v>
@@ -3043,16 +3050,19 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
-      </c>
-      <c r="D112" t="s">
-        <v>68</v>
+        <v>162</v>
+      </c>
+      <c r="C112" t="s">
+        <v>164</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
       </c>
       <c r="E112" t="s">
         <v>116</v>
       </c>
       <c r="F112" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3062,14 +3072,14 @@
       <c r="B113" t="s">
         <v>118</v>
       </c>
-      <c r="C113" t="s">
-        <v>124</v>
+      <c r="D113" t="s">
+        <v>68</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3080,13 +3090,13 @@
         <v>118</v>
       </c>
       <c r="C114" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3097,13 +3107,13 @@
         <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3114,13 +3124,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3131,13 +3141,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3148,13 +3158,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,13 +3175,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3182,13 +3192,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3196,16 +3206,16 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>165</v>
-      </c>
-      <c r="D121" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C121" t="s">
+        <v>51</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3215,8 +3225,8 @@
       <c r="B122" t="s">
         <v>165</v>
       </c>
-      <c r="C122" t="s">
-        <v>166</v>
+      <c r="D122" t="s">
+        <v>87</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
@@ -3230,16 +3240,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
-      </c>
-      <c r="D123" t="s">
-        <v>68</v>
+        <v>165</v>
+      </c>
+      <c r="C123" t="s">
+        <v>166</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3249,8 +3259,8 @@
       <c r="B124" t="s">
         <v>149</v>
       </c>
-      <c r="C124" t="s">
-        <v>151</v>
+      <c r="D124" t="s">
+        <v>68</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
@@ -3267,7 +3277,7 @@
         <v>149</v>
       </c>
       <c r="C125" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
@@ -3284,7 +3294,7 @@
         <v>149</v>
       </c>
       <c r="C126" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3301,7 +3311,7 @@
         <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3315,16 +3325,16 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
-      </c>
-      <c r="D128" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C128" t="s">
+        <v>50</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
       </c>
       <c r="F128" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3334,14 +3344,14 @@
       <c r="B129" t="s">
         <v>138</v>
       </c>
-      <c r="C129" t="s">
-        <v>148</v>
+      <c r="D129" t="s">
+        <v>68</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3352,13 +3362,13 @@
         <v>138</v>
       </c>
       <c r="C130" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
       </c>
       <c r="F130" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3369,7 +3379,7 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3386,13 +3396,13 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,13 +3413,13 @@
         <v>138</v>
       </c>
       <c r="C133" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3420,13 +3430,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3437,13 +3447,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,16 +3461,16 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>125</v>
-      </c>
-      <c r="D136" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C136" t="s">
+        <v>157</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3470,8 +3480,8 @@
       <c r="B137" t="s">
         <v>125</v>
       </c>
-      <c r="C137" t="s">
-        <v>127</v>
+      <c r="D137" t="s">
+        <v>68</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
@@ -3485,16 +3495,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>131</v>
-      </c>
-      <c r="D138" t="s">
-        <v>68</v>
+        <v>125</v>
+      </c>
+      <c r="C138" t="s">
+        <v>127</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3504,8 +3514,8 @@
       <c r="B139" t="s">
         <v>131</v>
       </c>
-      <c r="C139" t="s">
-        <v>132</v>
+      <c r="D139" t="s">
+        <v>68</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
@@ -3522,7 +3532,7 @@
         <v>131</v>
       </c>
       <c r="C140" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
@@ -3539,7 +3549,7 @@
         <v>131</v>
       </c>
       <c r="C141" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
@@ -3556,7 +3566,7 @@
         <v>131</v>
       </c>
       <c r="C142" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
@@ -3570,16 +3580,16 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>126</v>
-      </c>
-      <c r="D143" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C143" t="s">
+        <v>135</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
       </c>
       <c r="F143" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -3589,8 +3599,8 @@
       <c r="B144" t="s">
         <v>126</v>
       </c>
-      <c r="C144" t="s">
-        <v>128</v>
+      <c r="D144" t="s">
+        <v>68</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
@@ -3604,16 +3614,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>98</v>
-      </c>
-      <c r="D145" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C145" t="s">
+        <v>128</v>
       </c>
       <c r="E145" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F145" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3621,7 +3631,7 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D146" t="s">
         <v>87</v>
@@ -3630,7 +3640,7 @@
         <v>14</v>
       </c>
       <c r="F146" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3640,17 +3650,14 @@
       <c r="B147" t="s">
         <v>13</v>
       </c>
-      <c r="C147" t="s">
-        <v>10</v>
-      </c>
-      <c r="D147">
-        <v>1</v>
+      <c r="D147" t="s">
+        <v>87</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3661,7 +3668,7 @@
         <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -3670,7 +3677,7 @@
         <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3681,7 +3688,7 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -3690,7 +3697,7 @@
         <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3698,16 +3705,19 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>97</v>
-      </c>
-      <c r="D150" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C150" t="s">
+        <v>18</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
       </c>
       <c r="E150" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,14 +3727,14 @@
       <c r="B151" t="s">
         <v>97</v>
       </c>
-      <c r="C151" t="s">
-        <v>191</v>
+      <c r="D151" t="s">
+        <v>87</v>
       </c>
       <c r="E151" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F151" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3732,16 +3742,16 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>33</v>
-      </c>
-      <c r="D152" t="s">
-        <v>87</v>
+        <v>97</v>
+      </c>
+      <c r="C152" t="s">
+        <v>191</v>
       </c>
       <c r="E152" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F152" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3751,17 +3761,14 @@
       <c r="B153" t="s">
         <v>33</v>
       </c>
-      <c r="C153" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D153">
-        <v>1</v>
+      <c r="D153" t="s">
+        <v>87</v>
       </c>
       <c r="E153" t="s">
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3781,7 +3788,7 @@
         <v>54</v>
       </c>
       <c r="F154" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3792,13 +3799,16 @@
         <v>33</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
       </c>
       <c r="E155" t="s">
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3809,13 +3819,13 @@
         <v>33</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="E156" t="s">
         <v>54</v>
       </c>
       <c r="F156" t="s">
-        <v>193</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,17 +3833,16 @@
         <v>32</v>
       </c>
       <c r="B157" t="s">
-        <v>182</v>
-      </c>
-      <c r="C157" s="1"/>
-      <c r="D157" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="E157" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3841,15 +3850,33 @@
         <v>32</v>
       </c>
       <c r="B158" t="s">
+        <v>182</v>
+      </c>
+      <c r="C158" s="1"/>
+      <c r="D158" t="s">
+        <v>68</v>
+      </c>
+      <c r="E158" t="s">
+        <v>116</v>
+      </c>
+      <c r="F158" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>32</v>
+      </c>
+      <c r="B159" t="s">
         <v>88</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D159" t="s">
         <v>65</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E159" t="s">
         <v>24</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F159" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (manage-hyperlinks) Show how to set hyperlinks
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD69F-DE60-4A39-A2D8-9D33F8E2C07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3DAC6-52F5-4FC1-8F18-301093C2AA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="207">
   <si>
     <t>Class</t>
   </si>
@@ -629,6 +629,18 @@
   </si>
   <si>
     <t>getActiveSlide</t>
+  </si>
+  <si>
+    <t>HyperlinkAddOptions</t>
+  </si>
+  <si>
+    <t>setHyperlinkOnShape</t>
+  </si>
+  <si>
+    <t>setHyperlinkOnTextRange</t>
+  </si>
+  <si>
+    <t>hyperlinks</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F159" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F159" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F155">
-    <sortCondition ref="B1:B155"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F161" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F161" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F157">
+    <sortCondition ref="B1:B157"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1023,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,17 +1494,18 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
-        <v>101</v>
-      </c>
+      <c r="B26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
         <v>103</v>
       </c>
-      <c r="F26" t="s">
-        <v>102</v>
+      <c r="F26" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1500,16 +1513,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,10 +1530,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1534,16 +1547,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1551,16 +1564,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1568,16 +1581,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F31" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1585,10 +1598,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
         <v>85</v>
@@ -1602,16 +1615,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="D33" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1621,17 +1634,14 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>202</v>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1642,16 +1652,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F35" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1671,7 +1681,7 @@
         <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1691,7 +1701,7 @@
         <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1702,16 +1712,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1731,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1742,16 +1752,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,7 +1781,7 @@
         <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1782,16 +1792,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,16 +1812,16 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1831,7 +1841,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1842,13 +1852,16 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,16 +1869,16 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>175</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,17 +1888,14 @@
       <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
+      <c r="D47" t="s">
+        <v>87</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1896,16 +1906,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1916,16 +1926,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1936,13 +1946,16 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F50" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1953,13 +1966,13 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1970,13 +1983,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F52" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1987,7 +2000,7 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E53" t="s">
         <v>53</v>
@@ -2004,13 +2017,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>49</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2021,13 +2034,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>48</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2038,13 +2051,13 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,13 +2068,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2072,13 +2085,13 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F58" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2086,16 +2099,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2103,16 +2116,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2120,16 +2133,16 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="D61" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E61" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2139,17 +2152,14 @@
       <c r="B62" t="s">
         <v>21</v>
       </c>
-      <c r="C62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
+      <c r="D62" t="s">
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2160,16 +2170,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2180,16 +2190,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2200,16 +2210,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2220,16 +2230,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2240,16 +2250,16 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2260,16 +2270,16 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F68" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2280,16 +2290,16 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2297,10 +2307,13 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
       </c>
       <c r="E70" t="s">
         <v>85</v>
@@ -2316,17 +2329,14 @@
       <c r="B71" t="s">
         <v>59</v>
       </c>
-      <c r="C71" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+      <c r="D71" t="s">
+        <v>87</v>
       </c>
       <c r="E71" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,16 +2347,16 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F72" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,13 +2367,16 @@
         <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73" t="s">
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2374,13 +2387,13 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2391,13 +2404,13 @@
         <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2405,10 +2418,10 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>189</v>
-      </c>
-      <c r="D76" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C76" t="s">
+        <v>86</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
@@ -2422,16 +2435,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="D77" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F77" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2441,14 +2454,14 @@
       <c r="B78" t="s">
         <v>61</v>
       </c>
-      <c r="C78" t="s">
-        <v>62</v>
+      <c r="D78" t="s">
+        <v>87</v>
       </c>
       <c r="E78" t="s">
         <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,13 +2472,13 @@
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="E79" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F79" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,10 +2486,10 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
-      </c>
-      <c r="D80" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
+        <v>190</v>
       </c>
       <c r="E80" t="s">
         <v>24</v>
@@ -2490,16 +2503,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F81" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,11 +2522,8 @@
       <c r="B82" t="s">
         <v>113</v>
       </c>
-      <c r="C82" t="s">
-        <v>114</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
+      <c r="D82" t="s">
+        <v>87</v>
       </c>
       <c r="E82" t="s">
         <v>109</v>
@@ -2527,16 +2537,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
-      </c>
-      <c r="D83" t="s">
-        <v>65</v>
+        <v>113</v>
+      </c>
+      <c r="C83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F83" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2544,10 +2557,10 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D84" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2563,8 +2576,8 @@
       <c r="B85" t="s">
         <v>83</v>
       </c>
-      <c r="C85" t="s">
-        <v>84</v>
+      <c r="D85" t="s">
+        <v>87</v>
       </c>
       <c r="E85" t="s">
         <v>85</v>
@@ -2578,16 +2591,16 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
-      </c>
-      <c r="D86" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
       </c>
       <c r="E86" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F86" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,17 +2610,14 @@
       <c r="B87" t="s">
         <v>90</v>
       </c>
-      <c r="C87" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
+      <c r="D87" t="s">
+        <v>87</v>
       </c>
       <c r="E87" t="s">
         <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2615,16 +2625,19 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
-      </c>
-      <c r="D88" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F88" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2632,16 +2645,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D89" t="s">
         <v>65</v>
       </c>
       <c r="E89" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2658,7 +2671,7 @@
         <v>168</v>
       </c>
       <c r="F90" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2666,16 +2679,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D91" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E91" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F91" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2685,17 +2698,14 @@
       <c r="B92" t="s">
         <v>19</v>
       </c>
-      <c r="C92" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92">
-        <v>1</v>
+      <c r="D92" t="s">
+        <v>87</v>
       </c>
       <c r="E92" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2706,16 +2716,16 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F93" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2726,7 +2736,7 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -2746,16 +2756,16 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F95" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,7 +2785,7 @@
         <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2783,36 +2793,36 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>32</v>
       </c>
-      <c r="B98" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" t="s">
-        <v>12</v>
+      <c r="B98" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2822,17 +2832,14 @@
       <c r="B99" t="s">
         <v>9</v>
       </c>
-      <c r="C99" t="s">
-        <v>16</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
+      <c r="D99" t="s">
+        <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2840,16 +2847,19 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
-      </c>
-      <c r="D100" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F100" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2857,16 +2867,19 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
-      </c>
-      <c r="D101" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F101" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2874,16 +2887,16 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
-      </c>
-      <c r="C102" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D102" t="s">
+        <v>68</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F102" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2891,7 +2904,7 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D103" t="s">
         <v>87</v>
@@ -2908,13 +2921,10 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
-      </c>
-      <c r="D104">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E104" t="s">
         <v>11</v>
@@ -2928,16 +2938,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="D105" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E105" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F105" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2945,10 +2955,13 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>73</v>
-      </c>
-      <c r="D106" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C106" t="s">
+        <v>70</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2962,16 +2975,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="D107" t="s">
+        <v>65</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F107" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2979,7 +2992,7 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D108" t="s">
         <v>87</v>
@@ -2996,13 +3009,10 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C109" t="s">
-        <v>70</v>
-      </c>
-      <c r="D109">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
@@ -3016,16 +3026,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
       </c>
       <c r="E110" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F110" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3033,16 +3043,19 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
-      </c>
-      <c r="D111" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
       </c>
       <c r="E111" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3050,19 +3063,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>162</v>
-      </c>
-      <c r="C112" t="s">
-        <v>164</v>
-      </c>
-      <c r="D112">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D112" t="s">
+        <v>87</v>
       </c>
       <c r="E112" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F112" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3070,16 +3080,16 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="D113" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3087,16 +3097,19 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3106,8 +3119,8 @@
       <c r="B115" t="s">
         <v>118</v>
       </c>
-      <c r="C115" t="s">
-        <v>52</v>
+      <c r="D115" t="s">
+        <v>68</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3124,13 +3137,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3141,13 +3154,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3158,13 +3171,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3175,13 +3188,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3192,13 +3205,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3209,13 +3222,13 @@
         <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,16 +3236,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>165</v>
-      </c>
-      <c r="D122" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C122" t="s">
+        <v>120</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,16 +3253,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,16 +3270,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D124" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,16 +3287,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C125" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,8 +3306,8 @@
       <c r="B126" t="s">
         <v>149</v>
       </c>
-      <c r="C126" t="s">
-        <v>49</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3311,7 +3324,7 @@
         <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3328,7 +3341,7 @@
         <v>149</v>
       </c>
       <c r="C128" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3342,16 +3355,16 @@
         <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
-      </c>
-      <c r="D129" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C129" t="s">
+        <v>150</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3359,10 +3372,10 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C130" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3378,8 +3391,8 @@
       <c r="B131" t="s">
         <v>138</v>
       </c>
-      <c r="C131" t="s">
-        <v>58</v>
+      <c r="D131" t="s">
+        <v>68</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3396,13 +3409,13 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3413,13 +3426,13 @@
         <v>138</v>
       </c>
       <c r="C133" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,13 +3443,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3447,13 +3460,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3464,13 +3477,13 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3478,16 +3491,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>125</v>
-      </c>
-      <c r="D137" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C137" t="s">
+        <v>184</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3495,16 +3508,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3512,7 +3525,7 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D139" t="s">
         <v>68</v>
@@ -3521,7 +3534,7 @@
         <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3529,16 +3542,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C140" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3548,8 +3561,8 @@
       <c r="B141" t="s">
         <v>131</v>
       </c>
-      <c r="C141" t="s">
-        <v>133</v>
+      <c r="D141" t="s">
+        <v>68</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
@@ -3566,7 +3579,7 @@
         <v>131</v>
       </c>
       <c r="C142" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
@@ -3583,7 +3596,7 @@
         <v>131</v>
       </c>
       <c r="C143" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
@@ -3597,16 +3610,16 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
-      </c>
-      <c r="D144" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C144" t="s">
+        <v>134</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
       </c>
       <c r="F144" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,16 +3627,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C145" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E145" t="s">
         <v>116</v>
       </c>
       <c r="F145" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3631,16 +3644,16 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D146" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E146" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F146" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3648,16 +3661,16 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>13</v>
-      </c>
-      <c r="D147" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C147" t="s">
+        <v>128</v>
       </c>
       <c r="E147" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F147" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,19 +3678,16 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>13</v>
-      </c>
-      <c r="C148" t="s">
-        <v>10</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D148" t="s">
+        <v>87</v>
       </c>
       <c r="E148" t="s">
         <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3687,17 +3697,14 @@
       <c r="B149" t="s">
         <v>13</v>
       </c>
-      <c r="C149" t="s">
-        <v>20</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
+      <c r="D149" t="s">
+        <v>87</v>
       </c>
       <c r="E149" t="s">
         <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3708,7 +3715,7 @@
         <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D150">
         <v>1</v>
@@ -3717,7 +3724,7 @@
         <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3725,16 +3732,19 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>97</v>
-      </c>
-      <c r="D151" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C151" t="s">
+        <v>20</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3742,16 +3752,19 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C152" t="s">
-        <v>191</v>
+        <v>18</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3759,7 +3772,7 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D153" t="s">
         <v>87</v>
@@ -3768,7 +3781,7 @@
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3776,19 +3789,16 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>33</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C154" t="s">
+        <v>191</v>
       </c>
       <c r="E154" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3798,17 +3808,14 @@
       <c r="B155" t="s">
         <v>33</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D155">
-        <v>1</v>
+      <c r="D155" t="s">
+        <v>87</v>
       </c>
       <c r="E155" t="s">
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3819,13 +3826,16 @@
         <v>33</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
       </c>
       <c r="E156" t="s">
         <v>54</v>
       </c>
       <c r="F156" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3836,13 +3846,16 @@
         <v>33</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
       </c>
       <c r="E157" t="s">
         <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3850,17 +3863,16 @@
         <v>32</v>
       </c>
       <c r="B158" t="s">
-        <v>182</v>
-      </c>
-      <c r="C158" s="1"/>
-      <c r="D158" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E158" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F158" t="s">
-        <v>183</v>
+        <v>56</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -3868,15 +3880,50 @@
         <v>32</v>
       </c>
       <c r="B159" t="s">
+        <v>33</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E159" t="s">
+        <v>54</v>
+      </c>
+      <c r="F159" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>32</v>
+      </c>
+      <c r="B160" t="s">
+        <v>182</v>
+      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" t="s">
+        <v>68</v>
+      </c>
+      <c r="E160" t="s">
+        <v>116</v>
+      </c>
+      <c r="F160" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>32</v>
+      </c>
+      <c r="B161" t="s">
         <v>88</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D161" t="s">
         <v>65</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E161" t="s">
         <v>24</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F161" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (manage-hyperlinks) Show how to set hyperlinks (#1053)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD69F-DE60-4A39-A2D8-9D33F8E2C07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3DAC6-52F5-4FC1-8F18-301093C2AA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="207">
   <si>
     <t>Class</t>
   </si>
@@ -629,6 +629,18 @@
   </si>
   <si>
     <t>getActiveSlide</t>
+  </si>
+  <si>
+    <t>HyperlinkAddOptions</t>
+  </si>
+  <si>
+    <t>setHyperlinkOnShape</t>
+  </si>
+  <si>
+    <t>setHyperlinkOnTextRange</t>
+  </si>
+  <si>
+    <t>hyperlinks</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F159" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F159" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F155">
-    <sortCondition ref="B1:B155"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F161" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F161" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F157">
+    <sortCondition ref="B1:B157"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1023,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,17 +1494,18 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
-        <v>101</v>
-      </c>
+      <c r="B26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
         <v>103</v>
       </c>
-      <c r="F26" t="s">
-        <v>102</v>
+      <c r="F26" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1500,16 +1513,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,10 +1530,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1534,16 +1547,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1551,16 +1564,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1568,16 +1581,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F31" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1585,10 +1598,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
         <v>85</v>
@@ -1602,16 +1615,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="D33" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1621,17 +1634,14 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>202</v>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1642,16 +1652,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F35" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1671,7 +1681,7 @@
         <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1691,7 +1701,7 @@
         <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1702,16 +1712,16 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1731,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1742,16 +1752,16 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,7 +1781,7 @@
         <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1782,16 +1792,16 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,16 +1812,16 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1831,7 +1841,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1842,13 +1852,16 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,16 +1869,16 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>175</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1875,17 +1888,14 @@
       <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
+      <c r="D47" t="s">
+        <v>87</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1896,16 +1906,16 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1916,16 +1926,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1936,13 +1946,16 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F50" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1953,13 +1966,13 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1970,13 +1983,13 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F52" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1987,7 +2000,7 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E53" t="s">
         <v>53</v>
@@ -2004,13 +2017,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>49</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2021,13 +2034,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>48</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2038,13 +2051,13 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,13 +2068,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2072,13 +2085,13 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F58" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2086,16 +2099,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2103,16 +2116,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2120,16 +2133,16 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
       <c r="D61" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E61" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2139,17 +2152,14 @@
       <c r="B62" t="s">
         <v>21</v>
       </c>
-      <c r="C62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
+      <c r="D62" t="s">
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2160,16 +2170,16 @@
         <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2180,16 +2190,16 @@
         <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2200,16 +2210,16 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2220,16 +2230,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2240,16 +2250,16 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2260,16 +2270,16 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F68" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2280,16 +2290,16 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2297,10 +2307,13 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
       </c>
       <c r="E70" t="s">
         <v>85</v>
@@ -2316,17 +2329,14 @@
       <c r="B71" t="s">
         <v>59</v>
       </c>
-      <c r="C71" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+      <c r="D71" t="s">
+        <v>87</v>
       </c>
       <c r="E71" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,16 +2347,16 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F72" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,13 +2367,16 @@
         <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73" t="s">
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2374,13 +2387,13 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2391,13 +2404,13 @@
         <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2405,10 +2418,10 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>189</v>
-      </c>
-      <c r="D76" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C76" t="s">
+        <v>86</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
@@ -2422,16 +2435,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="D77" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F77" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2441,14 +2454,14 @@
       <c r="B78" t="s">
         <v>61</v>
       </c>
-      <c r="C78" t="s">
-        <v>62</v>
+      <c r="D78" t="s">
+        <v>87</v>
       </c>
       <c r="E78" t="s">
         <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,13 +2472,13 @@
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="E79" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F79" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2473,10 +2486,10 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
-      </c>
-      <c r="D80" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
+        <v>190</v>
       </c>
       <c r="E80" t="s">
         <v>24</v>
@@ -2490,16 +2503,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F81" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,11 +2522,8 @@
       <c r="B82" t="s">
         <v>113</v>
       </c>
-      <c r="C82" t="s">
-        <v>114</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
+      <c r="D82" t="s">
+        <v>87</v>
       </c>
       <c r="E82" t="s">
         <v>109</v>
@@ -2527,16 +2537,19 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
-      </c>
-      <c r="D83" t="s">
-        <v>65</v>
+        <v>113</v>
+      </c>
+      <c r="C83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F83" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2544,10 +2557,10 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D84" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
@@ -2563,8 +2576,8 @@
       <c r="B85" t="s">
         <v>83</v>
       </c>
-      <c r="C85" t="s">
-        <v>84</v>
+      <c r="D85" t="s">
+        <v>87</v>
       </c>
       <c r="E85" t="s">
         <v>85</v>
@@ -2578,16 +2591,16 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
-      </c>
-      <c r="D86" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
       </c>
       <c r="E86" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F86" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,17 +2610,14 @@
       <c r="B87" t="s">
         <v>90</v>
       </c>
-      <c r="C87" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
+      <c r="D87" t="s">
+        <v>87</v>
       </c>
       <c r="E87" t="s">
         <v>53</v>
       </c>
       <c r="F87" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2615,16 +2625,19 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
-      </c>
-      <c r="D88" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F88" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2632,16 +2645,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D89" t="s">
         <v>65</v>
       </c>
       <c r="E89" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2658,7 +2671,7 @@
         <v>168</v>
       </c>
       <c r="F90" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2666,16 +2679,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D91" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E91" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F91" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2685,17 +2698,14 @@
       <c r="B92" t="s">
         <v>19</v>
       </c>
-      <c r="C92" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92">
-        <v>1</v>
+      <c r="D92" t="s">
+        <v>87</v>
       </c>
       <c r="E92" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F92" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2706,16 +2716,16 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F93" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2726,7 +2736,7 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -2746,16 +2756,16 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F95" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2775,7 +2785,7 @@
         <v>53</v>
       </c>
       <c r="F96" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2783,36 +2793,36 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>32</v>
       </c>
-      <c r="B98" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" t="s">
-        <v>12</v>
+      <c r="B98" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2822,17 +2832,14 @@
       <c r="B99" t="s">
         <v>9</v>
       </c>
-      <c r="C99" t="s">
-        <v>16</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
+      <c r="D99" t="s">
+        <v>87</v>
       </c>
       <c r="E99" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2840,16 +2847,19 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
-      </c>
-      <c r="D100" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F100" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2857,16 +2867,19 @@
         <v>32</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
-      </c>
-      <c r="D101" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F101" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2874,16 +2887,16 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
-      </c>
-      <c r="C102" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D102" t="s">
+        <v>68</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F102" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2891,7 +2904,7 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D103" t="s">
         <v>87</v>
@@ -2908,13 +2921,10 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
-      </c>
-      <c r="D104">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E104" t="s">
         <v>11</v>
@@ -2928,16 +2938,16 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="D105" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E105" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F105" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2945,10 +2955,13 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>73</v>
-      </c>
-      <c r="D106" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C106" t="s">
+        <v>70</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2962,16 +2975,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="D107" t="s">
+        <v>65</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F107" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2979,7 +2992,7 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D108" t="s">
         <v>87</v>
@@ -2996,13 +3009,10 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C109" t="s">
-        <v>70</v>
-      </c>
-      <c r="D109">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
@@ -3016,16 +3026,16 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
       </c>
       <c r="E110" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F110" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -3033,16 +3043,19 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
-      </c>
-      <c r="D111" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
       </c>
       <c r="E111" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3050,19 +3063,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>162</v>
-      </c>
-      <c r="C112" t="s">
-        <v>164</v>
-      </c>
-      <c r="D112">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D112" t="s">
+        <v>87</v>
       </c>
       <c r="E112" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F112" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3070,16 +3080,16 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="D113" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E113" t="s">
         <v>116</v>
       </c>
       <c r="F113" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3087,16 +3097,19 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
       </c>
       <c r="E114" t="s">
         <v>116</v>
       </c>
       <c r="F114" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3106,8 +3119,8 @@
       <c r="B115" t="s">
         <v>118</v>
       </c>
-      <c r="C115" t="s">
-        <v>52</v>
+      <c r="D115" t="s">
+        <v>68</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
@@ -3124,13 +3137,13 @@
         <v>118</v>
       </c>
       <c r="C116" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3141,13 +3154,13 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
       </c>
       <c r="F117" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3158,13 +3171,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3175,13 +3188,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3192,13 +3205,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3209,13 +3222,13 @@
         <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,16 +3236,16 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>165</v>
-      </c>
-      <c r="D122" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C122" t="s">
+        <v>120</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,16 +3253,16 @@
         <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,16 +3270,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D124" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,16 +3287,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C125" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,8 +3306,8 @@
       <c r="B126" t="s">
         <v>149</v>
       </c>
-      <c r="C126" t="s">
-        <v>49</v>
+      <c r="D126" t="s">
+        <v>68</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
@@ -3311,7 +3324,7 @@
         <v>149</v>
       </c>
       <c r="C127" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
@@ -3328,7 +3341,7 @@
         <v>149</v>
       </c>
       <c r="C128" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3342,16 +3355,16 @@
         <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
-      </c>
-      <c r="D129" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C129" t="s">
+        <v>150</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
       </c>
       <c r="F129" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3359,10 +3372,10 @@
         <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C130" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3378,8 +3391,8 @@
       <c r="B131" t="s">
         <v>138</v>
       </c>
-      <c r="C131" t="s">
-        <v>58</v>
+      <c r="D131" t="s">
+        <v>68</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
@@ -3396,13 +3409,13 @@
         <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
       </c>
       <c r="F132" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3413,13 +3426,13 @@
         <v>138</v>
       </c>
       <c r="C133" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
       </c>
       <c r="F133" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,13 +3443,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3447,13 +3460,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3464,13 +3477,13 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3478,16 +3491,16 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>125</v>
-      </c>
-      <c r="D137" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C137" t="s">
+        <v>184</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3495,16 +3508,16 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3512,7 +3525,7 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D139" t="s">
         <v>68</v>
@@ -3521,7 +3534,7 @@
         <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3529,16 +3542,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C140" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3548,8 +3561,8 @@
       <c r="B141" t="s">
         <v>131</v>
       </c>
-      <c r="C141" t="s">
-        <v>133</v>
+      <c r="D141" t="s">
+        <v>68</v>
       </c>
       <c r="E141" t="s">
         <v>116</v>
@@ -3566,7 +3579,7 @@
         <v>131</v>
       </c>
       <c r="C142" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
@@ -3583,7 +3596,7 @@
         <v>131</v>
       </c>
       <c r="C143" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
@@ -3597,16 +3610,16 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
-      </c>
-      <c r="D144" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C144" t="s">
+        <v>134</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
       </c>
       <c r="F144" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,16 +3627,16 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C145" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E145" t="s">
         <v>116</v>
       </c>
       <c r="F145" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -3631,16 +3644,16 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D146" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E146" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F146" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3648,16 +3661,16 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>13</v>
-      </c>
-      <c r="D147" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C147" t="s">
+        <v>128</v>
       </c>
       <c r="E147" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F147" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,19 +3678,16 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>13</v>
-      </c>
-      <c r="C148" t="s">
-        <v>10</v>
-      </c>
-      <c r="D148">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D148" t="s">
+        <v>87</v>
       </c>
       <c r="E148" t="s">
         <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3687,17 +3697,14 @@
       <c r="B149" t="s">
         <v>13</v>
       </c>
-      <c r="C149" t="s">
-        <v>20</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
+      <c r="D149" t="s">
+        <v>87</v>
       </c>
       <c r="E149" t="s">
         <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3708,7 +3715,7 @@
         <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D150">
         <v>1</v>
@@ -3717,7 +3724,7 @@
         <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3725,16 +3732,19 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>97</v>
-      </c>
-      <c r="D151" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C151" t="s">
+        <v>20</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3742,16 +3752,19 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C152" t="s">
-        <v>191</v>
+        <v>18</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3759,7 +3772,7 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D153" t="s">
         <v>87</v>
@@ -3768,7 +3781,7 @@
         <v>54</v>
       </c>
       <c r="F153" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3776,19 +3789,16 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>33</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C154" t="s">
+        <v>191</v>
       </c>
       <c r="E154" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F154" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3798,17 +3808,14 @@
       <c r="B155" t="s">
         <v>33</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D155">
-        <v>1</v>
+      <c r="D155" t="s">
+        <v>87</v>
       </c>
       <c r="E155" t="s">
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3819,13 +3826,16 @@
         <v>33</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
       </c>
       <c r="E156" t="s">
         <v>54</v>
       </c>
       <c r="F156" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3836,13 +3846,16 @@
         <v>33</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
       </c>
       <c r="E157" t="s">
         <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3850,17 +3863,16 @@
         <v>32</v>
       </c>
       <c r="B158" t="s">
-        <v>182</v>
-      </c>
-      <c r="C158" s="1"/>
-      <c r="D158" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E158" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F158" t="s">
-        <v>183</v>
+        <v>56</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -3868,15 +3880,50 @@
         <v>32</v>
       </c>
       <c r="B159" t="s">
+        <v>33</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E159" t="s">
+        <v>54</v>
+      </c>
+      <c r="F159" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>32</v>
+      </c>
+      <c r="B160" t="s">
+        <v>182</v>
+      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" t="s">
+        <v>68</v>
+      </c>
+      <c r="E160" t="s">
+        <v>116</v>
+      </c>
+      <c r="F160" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>32</v>
+      </c>
+      <c r="B161" t="s">
         <v>88</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D161" t="s">
         <v>65</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E161" t="s">
         <v>24</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F161" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (hyperlinks) Include how to update and delete hyperlinks
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3DAC6-52F5-4FC1-8F18-301093C2AA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995B1E0C-ED6E-4740-AEB3-BEC61464CEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="210">
   <si>
     <t>Class</t>
   </si>
@@ -641,6 +641,15 @@
   </si>
   <si>
     <t>hyperlinks</t>
+  </si>
+  <si>
+    <t>deleteHyperlinkFromTextRange</t>
+  </si>
+  <si>
+    <t>setHyperlink</t>
+  </si>
+  <si>
+    <t>updateHyperlinkOnShape</t>
   </si>
 </sst>
 </file>
@@ -721,10 +730,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F161" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F161" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F157">
-    <sortCondition ref="B1:B157"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F163" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F163" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F159">
+    <sortCondition ref="B1:B159"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1035,11 +1044,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,18 +1503,20 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" t="s">
-        <v>68</v>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,16 +1524,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
         <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1530,16 +1541,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1547,10 +1558,10 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1564,16 +1575,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,16 +1592,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1598,16 +1609,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,10 +1626,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -1632,16 +1643,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,17 +1662,14 @@
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>200</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+      <c r="D35" t="s">
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>201</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,16 +1680,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F36" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,7 +1709,7 @@
         <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,7 +1729,7 @@
         <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,16 +1740,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,7 +1769,7 @@
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1772,16 +1780,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1801,7 +1809,7 @@
         <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,16 +1820,16 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,16 +1840,16 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,7 +1869,7 @@
         <v>40</v>
       </c>
       <c r="F45" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1872,13 +1880,16 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1886,16 +1897,16 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1905,17 +1916,14 @@
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
+      <c r="D48" t="s">
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,16 +1934,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1946,16 +1954,16 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1965,14 +1973,17 @@
       <c r="B51" t="s">
         <v>45</v>
       </c>
-      <c r="C51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E51" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" t="s">
-        <v>44</v>
+      <c r="C51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,13 +1994,16 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2000,13 +2014,13 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E53" t="s">
         <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,13 +2031,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2034,13 +2048,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>196</v>
+        <v>52</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2051,7 +2065,7 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E56" t="s">
         <v>53</v>
@@ -2068,13 +2082,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="E57" t="s">
         <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2085,7 +2099,7 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>53</v>
@@ -2102,13 +2116,13 @@
         <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F59" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2116,16 +2130,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C60" t="s">
+        <v>51</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,16 +2147,16 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
-      </c>
-      <c r="D61" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>178</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F61" t="s">
-        <v>89</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2150,16 +2164,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,19 +2181,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
       </c>
       <c r="E63" t="s">
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,17 +2200,14 @@
       <c r="B64" t="s">
         <v>21</v>
       </c>
-      <c r="C64" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+      <c r="D64" t="s">
+        <v>87</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,7 +2218,7 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2219,7 +2227,7 @@
         <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2230,16 +2238,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F66" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2250,7 +2258,7 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2259,7 +2267,7 @@
         <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,7 +2278,7 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2279,7 +2287,7 @@
         <v>116</v>
       </c>
       <c r="F68" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2290,16 +2298,16 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,16 +2318,16 @@
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F70" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2327,16 +2335,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
-      </c>
-      <c r="D71" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2344,19 +2355,19 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F72" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2366,17 +2377,14 @@
       <c r="B73" t="s">
         <v>59</v>
       </c>
-      <c r="C73" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
+      <c r="D73" t="s">
+        <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2387,13 +2395,16 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>179</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F74" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2404,13 +2415,16 @@
         <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>60</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2421,13 +2435,13 @@
         <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2435,16 +2449,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
-      </c>
-      <c r="D77" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C77" t="s">
+        <v>82</v>
       </c>
       <c r="E77" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2452,16 +2466,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>61</v>
-      </c>
-      <c r="D78" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
+        <v>86</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F78" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2469,16 +2483,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
+        <v>189</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F79" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,14 +2502,14 @@
       <c r="B80" t="s">
         <v>61</v>
       </c>
-      <c r="C80" t="s">
-        <v>190</v>
+      <c r="D80" t="s">
+        <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F80" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2503,16 +2517,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
-      </c>
-      <c r="D81" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
+        <v>62</v>
       </c>
       <c r="E81" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F81" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2520,16 +2534,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
-      </c>
-      <c r="D82" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C82" t="s">
+        <v>190</v>
       </c>
       <c r="E82" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F82" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2537,19 +2551,16 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
-      </c>
-      <c r="C83" t="s">
-        <v>114</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>188</v>
+      </c>
+      <c r="D83" t="s">
+        <v>65</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F83" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2557,16 +2568,16 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D84" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E84" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F84" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2574,16 +2585,19 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="C85" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F85" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,10 +2605,10 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
-      </c>
-      <c r="C86" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D86" t="s">
+        <v>65</v>
       </c>
       <c r="E86" t="s">
         <v>85</v>
@@ -2608,16 +2622,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D87" t="s">
         <v>87</v>
       </c>
       <c r="E87" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2625,19 +2639,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E88" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F88" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2645,16 +2656,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D89" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E89" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F89" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,16 +2673,19 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
-      </c>
-      <c r="D90" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F90" t="s">
-        <v>181</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,16 +2693,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D91" t="s">
         <v>65</v>
       </c>
       <c r="E91" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F91" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2696,16 +2710,16 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D92" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F92" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2713,19 +2727,16 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D93" t="s">
+        <v>65</v>
       </c>
       <c r="E93" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F93" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2735,17 +2746,14 @@
       <c r="B94" t="s">
         <v>19</v>
       </c>
-      <c r="C94" t="s">
-        <v>104</v>
-      </c>
-      <c r="D94">
-        <v>1</v>
+      <c r="D94" t="s">
+        <v>87</v>
       </c>
       <c r="E94" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F94" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2764,16 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F95" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,16 +2784,16 @@
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D96">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F96" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,33 +2804,36 @@
         <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F97" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>32</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" t="s">
         <v>19</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>204</v>
+      <c r="C98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,16 +2841,19 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="D99" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>38</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,19 +2861,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2869,17 +2880,14 @@
       <c r="B101" t="s">
         <v>9</v>
       </c>
-      <c r="C101" t="s">
-        <v>16</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
+      <c r="D101" t="s">
+        <v>87</v>
       </c>
       <c r="E101" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2887,16 +2895,19 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>185</v>
-      </c>
-      <c r="D102" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F102" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2904,16 +2915,19 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
-      </c>
-      <c r="D103" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F103" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2921,16 +2935,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
-      </c>
-      <c r="C104" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D104" t="s">
+        <v>68</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F104" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2938,7 +2952,7 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D105" t="s">
         <v>87</v>
@@ -2955,13 +2969,10 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C106" t="s">
-        <v>70</v>
-      </c>
-      <c r="D106">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2975,16 +2986,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="D107" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F107" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2992,10 +3003,13 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C108" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -3009,16 +3023,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>73</v>
-      </c>
-      <c r="C109" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="D109" t="s">
+        <v>65</v>
       </c>
       <c r="E109" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F109" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3026,7 +3040,7 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
@@ -3043,13 +3057,10 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C111" t="s">
-        <v>70</v>
-      </c>
-      <c r="D111">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E111" t="s">
         <v>11</v>
@@ -3063,16 +3074,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D112" t="s">
         <v>87</v>
       </c>
       <c r="E112" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F112" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3080,16 +3091,19 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
-      </c>
-      <c r="D113" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C113" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F113" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3097,19 +3111,16 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
-      </c>
-      <c r="C114" t="s">
-        <v>164</v>
-      </c>
-      <c r="D114">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D114" t="s">
+        <v>87</v>
       </c>
       <c r="E114" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F114" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,16 +3128,16 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="D115" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3134,16 +3145,19 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,8 +3167,8 @@
       <c r="B117" t="s">
         <v>118</v>
       </c>
-      <c r="C117" t="s">
-        <v>52</v>
+      <c r="D117" t="s">
+        <v>68</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
@@ -3171,13 +3185,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3188,13 +3202,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3205,13 +3219,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3222,13 +3236,13 @@
         <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3239,13 +3253,13 @@
         <v>118</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3256,13 +3270,13 @@
         <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3270,16 +3284,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
-      </c>
-      <c r="D124" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C124" t="s">
+        <v>120</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3287,16 +3301,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C125" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3304,16 +3318,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D126" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3321,16 +3335,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C127" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3340,8 +3354,8 @@
       <c r="B128" t="s">
         <v>149</v>
       </c>
-      <c r="C128" t="s">
-        <v>49</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3358,7 +3372,7 @@
         <v>149</v>
       </c>
       <c r="C129" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3375,7 +3389,7 @@
         <v>149</v>
       </c>
       <c r="C130" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3389,16 +3403,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>138</v>
-      </c>
-      <c r="D131" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C131" t="s">
+        <v>150</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3406,10 +3420,10 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C132" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3425,8 +3439,8 @@
       <c r="B133" t="s">
         <v>138</v>
       </c>
-      <c r="C133" t="s">
-        <v>58</v>
+      <c r="D133" t="s">
+        <v>68</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
@@ -3443,13 +3457,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3460,13 +3474,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3477,13 +3491,13 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3494,13 +3508,13 @@
         <v>138</v>
       </c>
       <c r="C137" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3511,13 +3525,13 @@
         <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3525,16 +3539,16 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>125</v>
-      </c>
-      <c r="D139" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C139" t="s">
+        <v>184</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3542,16 +3556,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C140" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,7 +3573,7 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D141" t="s">
         <v>68</v>
@@ -3568,7 +3582,7 @@
         <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3576,16 +3590,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C142" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
       </c>
       <c r="F142" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3595,8 +3609,8 @@
       <c r="B143" t="s">
         <v>131</v>
       </c>
-      <c r="C143" t="s">
-        <v>133</v>
+      <c r="D143" t="s">
+        <v>68</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
@@ -3613,7 +3627,7 @@
         <v>131</v>
       </c>
       <c r="C144" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
@@ -3630,7 +3644,7 @@
         <v>131</v>
       </c>
       <c r="C145" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E145" t="s">
         <v>116</v>
@@ -3644,16 +3658,16 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>126</v>
-      </c>
-      <c r="D146" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C146" t="s">
+        <v>134</v>
       </c>
       <c r="E146" t="s">
         <v>116</v>
       </c>
       <c r="F146" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3661,16 +3675,16 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C147" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E147" t="s">
         <v>116</v>
       </c>
       <c r="F147" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3678,16 +3692,16 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D148" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E148" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F148" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,16 +3709,16 @@
         <v>32</v>
       </c>
       <c r="B149" t="s">
-        <v>13</v>
-      </c>
-      <c r="D149" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C149" t="s">
+        <v>128</v>
       </c>
       <c r="E149" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F149" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3712,19 +3726,16 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>13</v>
-      </c>
-      <c r="C150" t="s">
-        <v>10</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D150" t="s">
+        <v>87</v>
       </c>
       <c r="E150" t="s">
         <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3734,17 +3745,14 @@
       <c r="B151" t="s">
         <v>13</v>
       </c>
-      <c r="C151" t="s">
-        <v>20</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
+      <c r="D151" t="s">
+        <v>87</v>
       </c>
       <c r="E151" t="s">
         <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3755,7 +3763,7 @@
         <v>13</v>
       </c>
       <c r="C152" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -3764,7 +3772,7 @@
         <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3772,16 +3780,19 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>97</v>
-      </c>
-      <c r="D153" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C153" t="s">
+        <v>20</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
       </c>
       <c r="E153" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F153" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3789,16 +3800,19 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C154" t="s">
-        <v>191</v>
+        <v>18</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
       </c>
       <c r="E154" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F154" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3806,7 +3820,7 @@
         <v>32</v>
       </c>
       <c r="B155" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D155" t="s">
         <v>87</v>
@@ -3815,7 +3829,7 @@
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,19 +3837,16 @@
         <v>32</v>
       </c>
       <c r="B156" t="s">
-        <v>33</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D156">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C156" t="s">
+        <v>191</v>
       </c>
       <c r="E156" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F156" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3845,17 +3856,14 @@
       <c r="B157" t="s">
         <v>33</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D157">
-        <v>1</v>
+      <c r="D157" t="s">
+        <v>87</v>
       </c>
       <c r="E157" t="s">
         <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3866,13 +3874,16 @@
         <v>33</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
       </c>
       <c r="E158" t="s">
         <v>54</v>
       </c>
       <c r="F158" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -3883,13 +3894,16 @@
         <v>33</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
       </c>
       <c r="E159" t="s">
         <v>54</v>
       </c>
       <c r="F159" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -3897,17 +3911,16 @@
         <v>32</v>
       </c>
       <c r="B160" t="s">
-        <v>182</v>
-      </c>
-      <c r="C160" s="1"/>
-      <c r="D160" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E160" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F160" t="s">
-        <v>183</v>
+        <v>56</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -3915,15 +3928,50 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E161" t="s">
+        <v>54</v>
+      </c>
+      <c r="F161" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>32</v>
+      </c>
+      <c r="B162" t="s">
+        <v>182</v>
+      </c>
+      <c r="C162" s="1"/>
+      <c r="D162" t="s">
+        <v>68</v>
+      </c>
+      <c r="E162" t="s">
+        <v>116</v>
+      </c>
+      <c r="F162" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>32</v>
+      </c>
+      <c r="B163" t="s">
         <v>88</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D163" t="s">
         <v>65</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E163" t="s">
         <v>24</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F163" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[PowerPoint] (hyperlinks) Include how to update and delete hyperlinks (#1054)
</commit_message>
<xml_diff>
--- a/snippet-extractor-metadata/powerpoint.xlsx
+++ b/snippet-extractor-metadata/powerpoint.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3DAC6-52F5-4FC1-8F18-301093C2AA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995B1E0C-ED6E-4740-AEB3-BEC61464CEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB5595D7-4492-4192-A1C1-2583BA1957AA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="210">
   <si>
     <t>Class</t>
   </si>
@@ -641,6 +641,15 @@
   </si>
   <si>
     <t>hyperlinks</t>
+  </si>
+  <si>
+    <t>deleteHyperlinkFromTextRange</t>
+  </si>
+  <si>
+    <t>setHyperlink</t>
+  </si>
+  <si>
+    <t>updateHyperlinkOnShape</t>
   </si>
 </sst>
 </file>
@@ -721,10 +730,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F161" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F161" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F157">
-    <sortCondition ref="B1:B157"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78C585A5-D505-49C6-9CA1-8E6558948317}" name="Snippets" displayName="Snippets" ref="A1:F163" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F163" xr:uid="{EAC65D03-FDD2-4352-A5F3-1CDEDE6251B2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F159">
+    <sortCondition ref="B1:B159"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{408888B8-C1DD-4B51-B1EB-5663F091D142}" name="Package"/>
@@ -1035,11 +1044,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809930CD-A227-47DC-AAA4-BB816AEDEB59}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,18 +1503,20 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" t="s">
-        <v>68</v>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,16 +1524,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
         <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1530,16 +1541,16 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1547,10 +1558,10 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1564,16 +1575,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,16 +1592,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1598,16 +1609,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,10 +1626,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -1632,16 +1643,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,17 +1662,14 @@
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>200</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+      <c r="D35" t="s">
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>201</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,16 +1680,16 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F36" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,7 +1709,7 @@
         <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,7 +1729,7 @@
         <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,16 +1740,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,7 +1769,7 @@
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1772,16 +1780,16 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1801,7 +1809,7 @@
         <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,16 +1820,16 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1832,16 +1840,16 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,7 +1869,7 @@
         <v>40</v>
       </c>
       <c r="F45" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1872,13 +1880,16 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>175</v>
+        <v>37</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1886,16 +1897,16 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1905,17 +1916,14 @@
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
+      <c r="D48" t="s">
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1926,16 +1934,16 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1946,16 +1954,16 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1965,14 +1973,17 @@
       <c r="B51" t="s">
         <v>45</v>
       </c>
-      <c r="C51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E51" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" t="s">
-        <v>44</v>
+      <c r="C51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,13 +1994,16 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2000,13 +2014,13 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E53" t="s">
         <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,13 +2031,13 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2034,13 +2048,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>196</v>
+        <v>52</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2051,7 +2065,7 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E56" t="s">
         <v>53</v>
@@ -2068,13 +2082,13 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="E57" t="s">
         <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2085,7 +2099,7 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>53</v>
@@ -2102,13 +2116,13 @@
         <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F59" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2116,16 +2130,16 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="C60" t="s">
+        <v>51</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,16 +2147,16 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
-      </c>
-      <c r="D61" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>178</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F61" t="s">
-        <v>89</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2150,16 +2164,16 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,19 +2181,16 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
       </c>
       <c r="E63" t="s">
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,17 +2200,14 @@
       <c r="B64" t="s">
         <v>21</v>
       </c>
-      <c r="C64" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
+      <c r="D64" t="s">
+        <v>87</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2210,7 +2218,7 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2219,7 +2227,7 @@
         <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2230,16 +2238,16 @@
         <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F66" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2250,7 +2258,7 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2259,7 +2267,7 @@
         <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,7 +2278,7 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2279,7 +2287,7 @@
         <v>116</v>
       </c>
       <c r="F68" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2290,16 +2298,16 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2310,16 +2318,16 @@
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="F70" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2327,16 +2335,19 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
-      </c>
-      <c r="D71" t="s">
-        <v>87</v>
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2344,19 +2355,19 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F72" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2366,17 +2377,14 @@
       <c r="B73" t="s">
         <v>59</v>
       </c>
-      <c r="C73" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
+      <c r="D73" t="s">
+        <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2387,13 +2395,16 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>179</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F74" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2404,13 +2415,16 @@
         <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>60</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2421,13 +2435,13 @@
         <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E76" t="s">
         <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2435,16 +2449,16 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
-      </c>
-      <c r="D77" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C77" t="s">
+        <v>82</v>
       </c>
       <c r="E77" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2452,16 +2466,16 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>61</v>
-      </c>
-      <c r="D78" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
+        <v>86</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F78" t="s">
-        <v>193</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2469,16 +2483,16 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" t="s">
-        <v>62</v>
+        <v>189</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F79" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,14 +2502,14 @@
       <c r="B80" t="s">
         <v>61</v>
       </c>
-      <c r="C80" t="s">
-        <v>190</v>
+      <c r="D80" t="s">
+        <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F80" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2503,16 +2517,16 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
-      </c>
-      <c r="D81" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
+        <v>62</v>
       </c>
       <c r="E81" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F81" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2520,16 +2534,16 @@
         <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
-      </c>
-      <c r="D82" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="C82" t="s">
+        <v>190</v>
       </c>
       <c r="E82" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F82" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2537,19 +2551,16 @@
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
-      </c>
-      <c r="C83" t="s">
-        <v>114</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>188</v>
+      </c>
+      <c r="D83" t="s">
+        <v>65</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="F83" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2557,16 +2568,16 @@
         <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D84" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E84" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F84" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2574,16 +2585,19 @@
         <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
-      </c>
-      <c r="D85" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="C85" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F85" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2591,10 +2605,10 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
-      </c>
-      <c r="C86" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D86" t="s">
+        <v>65</v>
       </c>
       <c r="E86" t="s">
         <v>85</v>
@@ -2608,16 +2622,16 @@
         <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D87" t="s">
         <v>87</v>
       </c>
       <c r="E87" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2625,19 +2639,16 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E88" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F88" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2645,16 +2656,16 @@
         <v>32</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D89" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E89" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F89" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,16 +2673,19 @@
         <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
-      </c>
-      <c r="D90" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="F90" t="s">
-        <v>181</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,16 +2693,16 @@
         <v>32</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="D91" t="s">
         <v>65</v>
       </c>
       <c r="E91" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F91" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2696,16 +2710,16 @@
         <v>32</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="D92" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="F92" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -2713,19 +2727,16 @@
         <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="D93" t="s">
+        <v>65</v>
       </c>
       <c r="E93" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="F93" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2735,17 +2746,14 @@
       <c r="B94" t="s">
         <v>19</v>
       </c>
-      <c r="C94" t="s">
-        <v>104</v>
-      </c>
-      <c r="D94">
-        <v>1</v>
+      <c r="D94" t="s">
+        <v>87</v>
       </c>
       <c r="E94" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="F94" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,16 +2764,16 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="D95">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F95" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,16 +2784,16 @@
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D96">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F96" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,33 +2804,36 @@
         <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="F97" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>32</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" t="s">
         <v>19</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>204</v>
+      <c r="C98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,16 +2841,19 @@
         <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="D99" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>38</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,19 +2861,16 @@
         <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
+        <v>206</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2869,17 +2880,14 @@
       <c r="B101" t="s">
         <v>9</v>
       </c>
-      <c r="C101" t="s">
-        <v>16</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
+      <c r="D101" t="s">
+        <v>87</v>
       </c>
       <c r="E101" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2887,16 +2895,19 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>185</v>
-      </c>
-      <c r="D102" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F102" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2904,16 +2915,19 @@
         <v>32</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
-      </c>
-      <c r="D103" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F103" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2921,16 +2935,16 @@
         <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
-      </c>
-      <c r="C104" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D104" t="s">
+        <v>68</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="F104" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2938,7 +2952,7 @@
         <v>32</v>
       </c>
       <c r="B105" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D105" t="s">
         <v>87</v>
@@ -2955,13 +2969,10 @@
         <v>32</v>
       </c>
       <c r="B106" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C106" t="s">
-        <v>70</v>
-      </c>
-      <c r="D106">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -2975,16 +2986,16 @@
         <v>32</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="D107" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="F107" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2992,10 +3003,13 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" t="s">
-        <v>87</v>
+        <v>72</v>
+      </c>
+      <c r="C108" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -3009,16 +3023,16 @@
         <v>32</v>
       </c>
       <c r="B109" t="s">
-        <v>73</v>
-      </c>
-      <c r="C109" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="D109" t="s">
+        <v>65</v>
       </c>
       <c r="E109" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="F109" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -3026,7 +3040,7 @@
         <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D110" t="s">
         <v>87</v>
@@ -3043,13 +3057,10 @@
         <v>32</v>
       </c>
       <c r="B111" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C111" t="s">
-        <v>70</v>
-      </c>
-      <c r="D111">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E111" t="s">
         <v>11</v>
@@ -3063,16 +3074,16 @@
         <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D112" t="s">
         <v>87</v>
       </c>
       <c r="E112" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="F112" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3080,16 +3091,19 @@
         <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
-      </c>
-      <c r="D113" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="C113" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="F113" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3097,19 +3111,16 @@
         <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
-      </c>
-      <c r="C114" t="s">
-        <v>164</v>
-      </c>
-      <c r="D114">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D114" t="s">
+        <v>87</v>
       </c>
       <c r="E114" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="F114" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,16 +3128,16 @@
         <v>32</v>
       </c>
       <c r="B115" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="D115" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E115" t="s">
         <v>116</v>
       </c>
       <c r="F115" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3134,16 +3145,19 @@
         <v>32</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>124</v>
+        <v>164</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
       </c>
       <c r="E116" t="s">
         <v>116</v>
       </c>
       <c r="F116" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,8 +3167,8 @@
       <c r="B117" t="s">
         <v>118</v>
       </c>
-      <c r="C117" t="s">
-        <v>52</v>
+      <c r="D117" t="s">
+        <v>68</v>
       </c>
       <c r="E117" t="s">
         <v>116</v>
@@ -3171,13 +3185,13 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E118" t="s">
         <v>116</v>
       </c>
       <c r="F118" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3188,13 +3202,13 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="E119" t="s">
         <v>116</v>
       </c>
       <c r="F119" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3205,13 +3219,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3222,13 +3236,13 @@
         <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E121" t="s">
         <v>116</v>
       </c>
       <c r="F121" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3239,13 +3253,13 @@
         <v>118</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E122" t="s">
         <v>116</v>
       </c>
       <c r="F122" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3256,13 +3270,13 @@
         <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E123" t="s">
         <v>116</v>
       </c>
       <c r="F123" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3270,16 +3284,16 @@
         <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
-      </c>
-      <c r="D124" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="C124" t="s">
+        <v>120</v>
       </c>
       <c r="E124" t="s">
         <v>116</v>
       </c>
       <c r="F124" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3287,16 +3301,16 @@
         <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C125" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E125" t="s">
         <v>116</v>
       </c>
       <c r="F125" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3304,16 +3318,16 @@
         <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D126" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E126" t="s">
         <v>116</v>
       </c>
       <c r="F126" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3321,16 +3335,16 @@
         <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C127" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E127" t="s">
         <v>116</v>
       </c>
       <c r="F127" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3340,8 +3354,8 @@
       <c r="B128" t="s">
         <v>149</v>
       </c>
-      <c r="C128" t="s">
-        <v>49</v>
+      <c r="D128" t="s">
+        <v>68</v>
       </c>
       <c r="E128" t="s">
         <v>116</v>
@@ -3358,7 +3372,7 @@
         <v>149</v>
       </c>
       <c r="C129" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E129" t="s">
         <v>116</v>
@@ -3375,7 +3389,7 @@
         <v>149</v>
       </c>
       <c r="C130" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E130" t="s">
         <v>116</v>
@@ -3389,16 +3403,16 @@
         <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>138</v>
-      </c>
-      <c r="D131" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="C131" t="s">
+        <v>150</v>
       </c>
       <c r="E131" t="s">
         <v>116</v>
       </c>
       <c r="F131" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3406,10 +3420,10 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C132" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E132" t="s">
         <v>116</v>
@@ -3425,8 +3439,8 @@
       <c r="B133" t="s">
         <v>138</v>
       </c>
-      <c r="C133" t="s">
-        <v>58</v>
+      <c r="D133" t="s">
+        <v>68</v>
       </c>
       <c r="E133" t="s">
         <v>116</v>
@@ -3443,13 +3457,13 @@
         <v>138</v>
       </c>
       <c r="C134" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="E134" t="s">
         <v>116</v>
       </c>
       <c r="F134" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3460,13 +3474,13 @@
         <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="E135" t="s">
         <v>116</v>
       </c>
       <c r="F135" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3477,13 +3491,13 @@
         <v>138</v>
       </c>
       <c r="C136" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E136" t="s">
         <v>116</v>
       </c>
       <c r="F136" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3494,13 +3508,13 @@
         <v>138</v>
       </c>
       <c r="C137" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E137" t="s">
         <v>116</v>
       </c>
       <c r="F137" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3511,13 +3525,13 @@
         <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E138" t="s">
         <v>116</v>
       </c>
       <c r="F138" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3525,16 +3539,16 @@
         <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>125</v>
-      </c>
-      <c r="D139" t="s">
-        <v>68</v>
+        <v>138</v>
+      </c>
+      <c r="C139" t="s">
+        <v>184</v>
       </c>
       <c r="E139" t="s">
         <v>116</v>
       </c>
       <c r="F139" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3542,16 +3556,16 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C140" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="E140" t="s">
         <v>116</v>
       </c>
       <c r="F140" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,7 +3573,7 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D141" t="s">
         <v>68</v>
@@ -3568,7 +3582,7 @@
         <v>116</v>
       </c>
       <c r="F141" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3576,16 +3590,16 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C142" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E142" t="s">
         <v>116</v>
       </c>
       <c r="F142" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -3595,8 +3609,8 @@
       <c r="B143" t="s">
         <v>131</v>
       </c>
-      <c r="C143" t="s">
-        <v>133</v>
+      <c r="D143" t="s">
+        <v>68</v>
       </c>
       <c r="E143" t="s">
         <v>116</v>
@@ -3613,7 +3627,7 @@
         <v>131</v>
       </c>
       <c r="C144" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E144" t="s">
         <v>116</v>
@@ -3630,7 +3644,7 @@
         <v>131</v>
       </c>
       <c r="C145" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E145" t="s">
         <v>116</v>
@@ -3644,16 +3658,16 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>126</v>
-      </c>
-      <c r="D146" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C146" t="s">
+        <v>134</v>
       </c>
       <c r="E146" t="s">
         <v>116</v>
       </c>
       <c r="F146" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -3661,16 +3675,16 @@
         <v>32</v>
       </c>
       <c r="B147" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C147" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E147" t="s">
         <v>116</v>
       </c>
       <c r="F147" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3678,16 +3692,16 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D148" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E148" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F148" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,16 +3709,16 @@
         <v>32</v>
       </c>
       <c r="B149" t="s">
-        <v>13</v>
-      </c>
-      <c r="D149" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="C149" t="s">
+        <v>128</v>
       </c>
       <c r="E149" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="F149" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3712,19 +3726,16 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>13</v>
-      </c>
-      <c r="C150" t="s">
-        <v>10</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D150" t="s">
+        <v>87</v>
       </c>
       <c r="E150" t="s">
         <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3734,17 +3745,14 @@
       <c r="B151" t="s">
         <v>13</v>
       </c>
-      <c r="C151" t="s">
-        <v>20</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
+      <c r="D151" t="s">
+        <v>87</v>
       </c>
       <c r="E151" t="s">
         <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3755,7 +3763,7 @@
         <v>13</v>
       </c>
       <c r="C152" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -3764,7 +3772,7 @@
         <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -3772,16 +3780,19 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>97</v>
-      </c>
-      <c r="D153" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="C153" t="s">
+        <v>20</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
       </c>
       <c r="E153" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F153" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3789,16 +3800,19 @@
         <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C154" t="s">
-        <v>191</v>
+        <v>18</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
       </c>
       <c r="E154" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F154" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3806,7 +3820,7 @@
         <v>32</v>
       </c>
       <c r="B155" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D155" t="s">
         <v>87</v>
@@ -3815,7 +3829,7 @@
         <v>54</v>
       </c>
       <c r="F155" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,19 +3837,16 @@
         <v>32</v>
       </c>
       <c r="B156" t="s">
-        <v>33</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D156">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C156" t="s">
+        <v>191</v>
       </c>
       <c r="E156" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F156" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -3845,17 +3856,14 @@
       <c r="B157" t="s">
         <v>33</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D157">
-        <v>1</v>
+      <c r="D157" t="s">
+        <v>87</v>
       </c>
       <c r="E157" t="s">
         <v>54</v>
       </c>
       <c r="F157" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3866,13 +3874,16 @@
         <v>33</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
       </c>
       <c r="E158" t="s">
         <v>54</v>
       </c>
       <c r="F158" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -3883,13 +3894,16 @@
         <v>33</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>195</v>
+        <v>39</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
       </c>
       <c r="E159" t="s">
         <v>54</v>
       </c>
       <c r="F159" t="s">
-        <v>193</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -3897,17 +3911,16 @@
         <v>32</v>
       </c>
       <c r="B160" t="s">
-        <v>182</v>
-      </c>
-      <c r="C160" s="1"/>
-      <c r="D160" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E160" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F160" t="s">
-        <v>183</v>
+        <v>56</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -3915,15 +3928,50 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E161" t="s">
+        <v>54</v>
+      </c>
+      <c r="F161" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>32</v>
+      </c>
+      <c r="B162" t="s">
+        <v>182</v>
+      </c>
+      <c r="C162" s="1"/>
+      <c r="D162" t="s">
+        <v>68</v>
+      </c>
+      <c r="E162" t="s">
+        <v>116</v>
+      </c>
+      <c r="F162" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>32</v>
+      </c>
+      <c r="B163" t="s">
         <v>88</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D163" t="s">
         <v>65</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E163" t="s">
         <v>24</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F163" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>